<commit_message>
Performer process ongoing. First steps
</commit_message>
<xml_diff>
--- a/STS IR Bot Performer/Data/Config.xlsx
+++ b/STS IR Bot Performer/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://taxwarellc-my.sharepoint.com/personal/nahuel_delacruz_sovos_com/Documents/Desktop/Nahuel/Projects/STS Internal Review bot/STS IR Bot Performer/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="13_ncr:1_{7EB2D2BA-2ADF-4595-A83F-0537891C1675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{99F53D70-615D-4370-B22C-47DD19DDC836}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="13_ncr:1_{7EB2D2BA-2ADF-4595-A83F-0537891C1675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A8F96A17-E996-4D29-8F75-E46B4E46DD39}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="70">
   <si>
     <t>Name</t>
   </si>
@@ -237,6 +237,15 @@
   </si>
   <si>
     <t>OtherDeductionsList_SheetScreenScraping</t>
+  </si>
+  <si>
+    <t>ScreenScraping</t>
+  </si>
+  <si>
+    <t>PathPDriveFolder</t>
+  </si>
+  <si>
+    <t>\\somproddfs1.prod.sovos.org\depts\TaxSolver Files</t>
   </si>
 </sst>
 </file>
@@ -289,7 +298,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -299,6 +308,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -619,12 +629,12 @@
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" customWidth="1"/>
+    <col min="1" max="1" width="43.54296875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.5703125" customWidth="1"/>
+    <col min="3" max="3" width="81.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -672,7 +682,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="45">
+    <row r="3" spans="1:26" ht="43.5">
       <c r="A3" s="2" t="s">
         <v>29</v>
       </c>
@@ -691,7 +701,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="30">
+    <row r="5" spans="1:26" ht="29">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1736,16 +1746,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z742"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
-    <col min="2" max="2" width="89.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="75.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.5703125" customWidth="1"/>
+    <col min="2" max="2" width="89.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="75.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1782,7 +1792,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="30">
+    <row r="2" spans="1:26" ht="29">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1793,7 +1803,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="45">
+    <row r="3" spans="1:26" ht="43.5">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -1915,7 +1925,14 @@
         <v>63</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="18" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A18" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
@@ -1965,6 +1982,9 @@
     <row r="31" spans="1:3" ht="14.25" customHeight="1">
       <c r="A31" t="s">
         <v>66</v>
+      </c>
+      <c r="B31" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2693,12 +2713,12 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" customWidth="1"/>
-    <col min="3" max="3" width="60.42578125" customWidth="1"/>
-    <col min="4" max="26" width="65.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.81640625" customWidth="1"/>
+    <col min="2" max="2" width="30.1796875" customWidth="1"/>
+    <col min="3" max="3" width="60.453125" customWidth="1"/>
+    <col min="4" max="26" width="65.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
Performer Process Ongoing. Review Sheet logic was added
</commit_message>
<xml_diff>
--- a/STS IR Bot Performer/Data/Config.xlsx
+++ b/STS IR Bot Performer/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://taxwarellc-my.sharepoint.com/personal/nahuel_delacruz_sovos_com/Documents/Desktop/Nahuel/Projects/STS Internal Review bot/STS IR Bot Performer/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="13_ncr:1_{7EB2D2BA-2ADF-4595-A83F-0537891C1675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A8F96A17-E996-4D29-8F75-E46B4E46DD39}"/>
+  <xr:revisionPtr revIDLastSave="51" documentId="13_ncr:1_{7EB2D2BA-2ADF-4595-A83F-0537891C1675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{14132EAB-E2CF-49A0-88D5-997352BE6FD3}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="83">
   <si>
     <t>Name</t>
   </si>
@@ -246,6 +246,45 @@
   </si>
   <si>
     <t>\\somproddfs1.prod.sovos.org\depts\TaxSolver Files</t>
+  </si>
+  <si>
+    <t>ReturnNameExceptionalCase</t>
+  </si>
+  <si>
+    <t>SER</t>
+  </si>
+  <si>
+    <t>Any return which name ends with this word, must be skipped or ignored.</t>
+  </si>
+  <si>
+    <t>PathTemplateReviewSheet</t>
+  </si>
+  <si>
+    <t>Data\Template_ReviewSheet.xlsx</t>
+  </si>
+  <si>
+    <t>ReviewSheet_WorksheetName</t>
+  </si>
+  <si>
+    <t>Template</t>
+  </si>
+  <si>
+    <t>ReviewSheet_StartCellReturnsFailedTable</t>
+  </si>
+  <si>
+    <t>G6</t>
+  </si>
+  <si>
+    <t>ReviewSheet_RequiredColumns</t>
+  </si>
+  <si>
+    <t>ReviewSheet_DateFormat</t>
+  </si>
+  <si>
+    <t>MMMM yyyy</t>
+  </si>
+  <si>
+    <t>Form Name,Legal Entity,Reason(s) Denied,Fixed?</t>
   </si>
 </sst>
 </file>
@@ -298,7 +337,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -308,7 +347,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -629,12 +667,12 @@
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.54296875" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.453125" customWidth="1"/>
-    <col min="4" max="26" width="8.54296875" customWidth="1"/>
+    <col min="3" max="3" width="81.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -682,7 +720,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.5">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" s="2" t="s">
         <v>29</v>
       </c>
@@ -701,7 +739,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="29">
+    <row r="5" spans="1:26" ht="30">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1744,18 +1782,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z742"/>
+  <dimension ref="A1:Z744"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
-    <col min="2" max="2" width="89.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="75.453125" customWidth="1"/>
-    <col min="4" max="26" width="8.54296875" customWidth="1"/>
+    <col min="2" max="2" width="89.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="75.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1792,7 +1830,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="29">
+    <row r="2" spans="1:26" ht="30">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1803,7 +1841,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.5">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -1929,81 +1967,126 @@
       <c r="A18" t="s">
         <v>68</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A19" t="s">
+        <v>73</v>
+      </c>
+      <c r="B19" t="s">
+        <v>74</v>
+      </c>
+    </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A21" t="s">
+        <v>70</v>
+      </c>
+      <c r="B21" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" t="s">
+        <v>72</v>
+      </c>
+    </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A23" t="s">
+        <v>75</v>
+      </c>
+      <c r="B23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A24" t="s">
+        <v>77</v>
+      </c>
+      <c r="B24" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A25" t="s">
+        <v>79</v>
+      </c>
+      <c r="B25" t="s">
+        <v>82</v>
+      </c>
+    </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
       <c r="A26" t="s">
-        <v>54</v>
+        <v>80</v>
       </c>
       <c r="B26" t="s">
-        <v>55</v>
+        <v>81</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A27" t="s">
-        <v>56</v>
-      </c>
-      <c r="B27" t="s">
-        <v>57</v>
-      </c>
-      <c r="C27" t="s">
-        <v>58</v>
-      </c>
-    </row>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="28" spans="1:3" ht="14.25" customHeight="1">
       <c r="A28" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B28" t="s">
-        <v>60</v>
-      </c>
-      <c r="C28" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A29" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" t="s">
+        <v>57</v>
+      </c>
+      <c r="C29" t="s">
+        <v>58</v>
+      </c>
+    </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1">
       <c r="A30" t="s">
+        <v>59</v>
+      </c>
+      <c r="B30" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A32" t="s">
         <v>64</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B32" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A31" t="s">
+    <row r="33" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A33" t="s">
         <v>66</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B33" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="33" ht="14.25" customHeight="1"/>
-    <row r="34" ht="14.25" customHeight="1"/>
-    <row r="35" ht="14.25" customHeight="1"/>
-    <row r="36" ht="14.25" customHeight="1"/>
-    <row r="37" ht="14.25" customHeight="1"/>
-    <row r="38" ht="14.25" customHeight="1"/>
-    <row r="39" ht="14.25" customHeight="1"/>
-    <row r="40" ht="14.25" customHeight="1"/>
-    <row r="41" ht="14.25" customHeight="1"/>
-    <row r="42" ht="14.25" customHeight="1"/>
-    <row r="43" ht="14.25" customHeight="1"/>
-    <row r="44" ht="14.25" customHeight="1"/>
-    <row r="45" ht="14.25" customHeight="1"/>
-    <row r="46" ht="14.25" customHeight="1"/>
-    <row r="47" ht="14.25" customHeight="1"/>
-    <row r="48" ht="14.25" customHeight="1"/>
+    <row r="34" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="35" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="36" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="37" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="38" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="39" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="40" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="41" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="42" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="43" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="44" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="45" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="46" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="47" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="48" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="49" ht="14.25" customHeight="1"/>
     <row r="50" ht="14.25" customHeight="1"/>
     <row r="51" ht="14.25" customHeight="1"/>
@@ -2698,6 +2781,8 @@
     <row r="740" ht="14.25" customHeight="1"/>
     <row r="741" ht="14.25" customHeight="1"/>
     <row r="742" ht="14.25" customHeight="1"/>
+    <row r="743" ht="14.25" customHeight="1"/>
+    <row r="744" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2713,12 +2798,12 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.81640625" customWidth="1"/>
-    <col min="2" max="2" width="30.1796875" customWidth="1"/>
-    <col min="3" max="3" width="60.453125" customWidth="1"/>
-    <col min="4" max="26" width="65.453125" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="60.42578125" customWidth="1"/>
+    <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
Performer Process Ongoing. Review Sheet logic was added and corrections in the main workflow.
</commit_message>
<xml_diff>
--- a/STS IR Bot Performer/Data/Config.xlsx
+++ b/STS IR Bot Performer/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://taxwarellc-my.sharepoint.com/personal/nahuel_delacruz_sovos_com/Documents/Desktop/Nahuel/Projects/STS Internal Review bot/STS IR Bot Performer/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="51" documentId="13_ncr:1_{7EB2D2BA-2ADF-4595-A83F-0537891C1675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{14132EAB-E2CF-49A0-88D5-997352BE6FD3}"/>
+  <xr:revisionPtr revIDLastSave="72" documentId="13_ncr:1_{7EB2D2BA-2ADF-4595-A83F-0537891C1675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{226AE3DD-7A39-4CB0-94FC-0440D9C23CF6}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="94">
   <si>
     <t>Name</t>
   </si>
@@ -257,12 +257,6 @@
     <t>Any return which name ends with this word, must be skipped or ignored.</t>
   </si>
   <si>
-    <t>PathTemplateReviewSheet</t>
-  </si>
-  <si>
-    <t>Data\Template_ReviewSheet.xlsx</t>
-  </si>
-  <si>
     <t>ReviewSheet_WorksheetName</t>
   </si>
   <si>
@@ -285,6 +279,45 @@
   </si>
   <si>
     <t>Form Name,Legal Entity,Reason(s) Denied,Fixed?</t>
+  </si>
+  <si>
+    <t>PathMarginsList</t>
+  </si>
+  <si>
+    <t>Data\Margins List.xlsx</t>
+  </si>
+  <si>
+    <t>PathCustomerNameList</t>
+  </si>
+  <si>
+    <t>Data\Customer Account List.xlsx</t>
+  </si>
+  <si>
+    <t>CustomerNameList_WorksheetName</t>
+  </si>
+  <si>
+    <t>Sheet1</t>
+  </si>
+  <si>
+    <t>The sheet name of the customer name list file.</t>
+  </si>
+  <si>
+    <t>PathTemplatesFile</t>
+  </si>
+  <si>
+    <t>Data\Templatesxlsx</t>
+  </si>
+  <si>
+    <t>TemplateFile_WorksheetReviewSheetTemplate</t>
+  </si>
+  <si>
+    <t>Review Sheet</t>
+  </si>
+  <si>
+    <t>OtherDeductionsList_SheetClickOnText</t>
+  </si>
+  <si>
+    <t>ClickOnText</t>
   </si>
 </sst>
 </file>
@@ -1782,10 +1815,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z744"/>
+  <dimension ref="A1:Z749"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1973,120 +2006,158 @@
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="B19" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A20" t="s">
+        <v>81</v>
+      </c>
+      <c r="B20" t="s">
+        <v>82</v>
+      </c>
+    </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="B21" t="s">
-        <v>71</v>
-      </c>
-      <c r="C21" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="B23" t="s">
-        <v>76</v>
+        <v>86</v>
+      </c>
+      <c r="C23" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
       <c r="B24" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A25" t="s">
-        <v>79</v>
-      </c>
-      <c r="B25" t="s">
-        <v>82</v>
-      </c>
-    </row>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
       <c r="A26" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="B26" t="s">
-        <v>81</v>
+        <v>71</v>
+      </c>
+      <c r="C26" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="28" spans="1:3" ht="14.25" customHeight="1">
       <c r="A28" t="s">
-        <v>54</v>
+        <v>73</v>
       </c>
       <c r="B28" t="s">
-        <v>55</v>
+        <v>74</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1">
       <c r="A29" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="B29" t="s">
-        <v>57</v>
-      </c>
-      <c r="C29" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1">
       <c r="A30" t="s">
+        <v>77</v>
+      </c>
+      <c r="B30" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A31" t="s">
+        <v>78</v>
+      </c>
+      <c r="B31" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="33" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A33" t="s">
+        <v>54</v>
+      </c>
+      <c r="B33" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A34" t="s">
+        <v>56</v>
+      </c>
+      <c r="B34" t="s">
+        <v>57</v>
+      </c>
+      <c r="C34" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A35" t="s">
         <v>59</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B35" t="s">
         <v>60</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C35" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="32" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A32" t="s">
+    <row r="36" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="37" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A37" t="s">
         <v>64</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B37" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A33" t="s">
+    <row r="38" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A38" t="s">
         <v>66</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B38" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="35" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="36" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="37" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="38" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="39" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="40" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="41" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="42" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="43" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="44" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="45" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="46" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="47" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="48" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="39" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A39" t="s">
+        <v>92</v>
+      </c>
+      <c r="B39" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="41" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="42" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="43" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="44" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="45" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="46" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="47" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="48" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="49" ht="14.25" customHeight="1"/>
     <row r="50" ht="14.25" customHeight="1"/>
     <row r="51" ht="14.25" customHeight="1"/>
@@ -2783,6 +2854,11 @@
     <row r="742" ht="14.25" customHeight="1"/>
     <row r="743" ht="14.25" customHeight="1"/>
     <row r="744" ht="14.25" customHeight="1"/>
+    <row r="745" ht="14.25" customHeight="1"/>
+    <row r="746" ht="14.25" customHeight="1"/>
+    <row r="747" ht="14.25" customHeight="1"/>
+    <row r="748" ht="14.25" customHeight="1"/>
+    <row r="749" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Changes in calue to zero workflow
</commit_message>
<xml_diff>
--- a/STS IR Bot Performer/Data/Config.xlsx
+++ b/STS IR Bot Performer/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://taxwarellc-my.sharepoint.com/personal/nahuel_delacruz_sovos_com/Documents/Desktop/Nahuel/Projects/STS Internal Review bot/STS IR Bot Performer/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\martin.martinez\Documents\githubProject-IRBot\STS_InternalReviewBot\STS IR Bot Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="72" documentId="13_ncr:1_{7EB2D2BA-2ADF-4595-A83F-0537891C1675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{226AE3DD-7A39-4CB0-94FC-0440D9C23CF6}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3F35D37-BFE4-4E97-B691-C8BE20145DB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="-21255" yWindow="2205" windowWidth="21600" windowHeight="11265" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -305,9 +305,6 @@
     <t>PathTemplatesFile</t>
   </si>
   <si>
-    <t>Data\Templatesxlsx</t>
-  </si>
-  <si>
     <t>TemplateFile_WorksheetReviewSheetTemplate</t>
   </si>
   <si>
@@ -318,6 +315,9 @@
   </si>
   <si>
     <t>ClickOnText</t>
+  </si>
+  <si>
+    <t>Data\Templates.xlsx</t>
   </si>
 </sst>
 </file>
@@ -1817,8 +1817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z749"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2009,7 +2009,7 @@
         <v>88</v>
       </c>
       <c r="B19" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
@@ -2042,10 +2042,10 @@
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" t="s">
+        <v>89</v>
+      </c>
+      <c r="B24" t="s">
         <v>90</v>
-      </c>
-      <c r="B24" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2143,10 +2143,10 @@
     </row>
     <row r="39" spans="1:3" ht="14.25" customHeight="1">
       <c r="A39" t="s">
+        <v>91</v>
+      </c>
+      <c r="B39" t="s">
         <v>92</v>
-      </c>
-      <c r="B39" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2870,7 +2870,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z989"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Tests made for review sheet. AddNewRow workflow was changed
</commit_message>
<xml_diff>
--- a/STS IR Bot Performer/Data/Config.xlsx
+++ b/STS IR Bot Performer/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://taxwarellc-my.sharepoint.com/personal/nahuel_delacruz_sovos_com/Documents/Desktop/Nahuel/Projects/STS Internal Review bot/STS IR Bot Performer/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="72" documentId="13_ncr:1_{7EB2D2BA-2ADF-4595-A83F-0537891C1675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{226AE3DD-7A39-4CB0-94FC-0440D9C23CF6}"/>
+  <xr:revisionPtr revIDLastSave="73" documentId="13_ncr:1_{7EB2D2BA-2ADF-4595-A83F-0537891C1675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{61C5E823-4B56-46FC-8D87-76E587461FB0}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -305,9 +305,6 @@
     <t>PathTemplatesFile</t>
   </si>
   <si>
-    <t>Data\Templatesxlsx</t>
-  </si>
-  <si>
     <t>TemplateFile_WorksheetReviewSheetTemplate</t>
   </si>
   <si>
@@ -318,6 +315,9 @@
   </si>
   <si>
     <t>ClickOnText</t>
+  </si>
+  <si>
+    <t>Data\Templates.xlsx</t>
   </si>
 </sst>
 </file>
@@ -1817,8 +1817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z749"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2009,7 +2009,7 @@
         <v>88</v>
       </c>
       <c r="B19" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
@@ -2042,10 +2042,10 @@
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" t="s">
+        <v>89</v>
+      </c>
+      <c r="B24" t="s">
         <v>90</v>
-      </c>
-      <c r="B24" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2143,10 +2143,10 @@
     </row>
     <row r="39" spans="1:3" ht="14.25" customHeight="1">
       <c r="A39" t="s">
+        <v>91</v>
+      </c>
+      <c r="B39" t="s">
         <v>92</v>
-      </c>
-      <c r="B39" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
commit again cause rebase
</commit_message>
<xml_diff>
--- a/STS IR Bot Performer/Data/Config.xlsx
+++ b/STS IR Bot Performer/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\martin.martinez\Documents\githubProject-IRBot\STS_InternalReviewBot\STS IR Bot Performer\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://taxwarellc-my.sharepoint.com/personal/nahuel_delacruz_sovos_com/Documents/Desktop/Nahuel/Projects/STS Internal Review bot/STS IR Bot Performer/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3F35D37-BFE4-4E97-B691-C8BE20145DB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="73" documentId="13_ncr:1_{7EB2D2BA-2ADF-4595-A83F-0537891C1675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{61C5E823-4B56-46FC-8D87-76E587461FB0}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="-21255" yWindow="2205" windowWidth="21600" windowHeight="11265" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -1817,7 +1817,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z749"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
@@ -2870,7 +2870,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z989"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
WI Exceptional Case was adding to main and new workflow was created
</commit_message>
<xml_diff>
--- a/STS IR Bot Performer/Data/Config.xlsx
+++ b/STS IR Bot Performer/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\martin.martinez\Documents\github-IRBot\STS_InternalReviewBot\STS IR Bot Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA225A9C-350C-4493-A190-30E2541DCE89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7E5B9B3-85A1-4917-A8BF-003E9CFA2B8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="102">
   <si>
     <t>Name</t>
   </si>
@@ -336,6 +336,12 @@
   </si>
   <si>
     <t>name of the excel where the dispatcher process saved the necessary information</t>
+  </si>
+  <si>
+    <t>OtherDeductionsList_SheetWIExceptionalCase</t>
+  </si>
+  <si>
+    <t>WIExceptionalCase</t>
   </si>
 </sst>
 </file>
@@ -1836,12 +1842,12 @@
   <dimension ref="A1:Z751"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="41" customWidth="1"/>
+    <col min="1" max="1" width="44.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="89.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="75.42578125" customWidth="1"/>
     <col min="4" max="26" width="8.5703125" customWidth="1"/>
@@ -2189,7 +2195,14 @@
         <v>92</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="42" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A42" t="s">
+        <v>100</v>
+      </c>
+      <c r="B42" t="s">
+        <v>101</v>
+      </c>
+    </row>
     <row r="43" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="44" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="45" spans="1:3" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Change in setting of parameters in process within main and config file.
</commit_message>
<xml_diff>
--- a/STS IR Bot Performer/Data/Config.xlsx
+++ b/STS IR Bot Performer/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\martin.martinez\Documents\github-IRBot\STS_InternalReviewBot\STS IR Bot Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7E5B9B3-85A1-4917-A8BF-003E9CFA2B8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A22A375C-FE54-40F8-A840-F290BFAF03B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="100">
   <si>
     <t>Name</t>
   </si>
@@ -255,12 +255,6 @@
   </si>
   <si>
     <t>Any return which name ends with this word, must be skipped or ignored.</t>
-  </si>
-  <si>
-    <t>ReviewSheet_WorksheetName</t>
-  </si>
-  <si>
-    <t>Template</t>
   </si>
   <si>
     <t>ReviewSheet_StartCellReturnsFailedTable</t>
@@ -1839,10 +1833,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z751"/>
+  <dimension ref="A1:Z750"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2030,68 +2024,68 @@
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B19" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B20" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B21" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" t="s">
+        <v>92</v>
+      </c>
+      <c r="B22" t="s">
+        <v>93</v>
+      </c>
+      <c r="C22" t="s">
         <v>94</v>
-      </c>
-      <c r="B22" t="s">
-        <v>95</v>
-      </c>
-      <c r="C22" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" t="s">
+        <v>83</v>
+      </c>
+      <c r="B24" t="s">
+        <v>84</v>
+      </c>
+      <c r="C24" t="s">
         <v>85</v>
-      </c>
-      <c r="B24" t="s">
-        <v>86</v>
-      </c>
-      <c r="C24" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
       <c r="A25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B25" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
       <c r="A26" t="s">
+        <v>95</v>
+      </c>
+      <c r="B26" t="s">
+        <v>96</v>
+      </c>
+      <c r="C26" t="s">
         <v>97</v>
-      </c>
-      <c r="B26" t="s">
-        <v>98</v>
-      </c>
-      <c r="C26" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2120,89 +2114,82 @@
         <v>75</v>
       </c>
       <c r="B31" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1">
       <c r="A32" t="s">
+        <v>76</v>
+      </c>
+      <c r="B32" t="s">
         <v>77</v>
       </c>
-      <c r="B32" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A33" t="s">
-        <v>78</v>
-      </c>
-      <c r="B33" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="14.25" customHeight="1"/>
+    </row>
+    <row r="33" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="34" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A34" t="s">
+        <v>54</v>
+      </c>
+      <c r="B34" t="s">
+        <v>55</v>
+      </c>
+    </row>
     <row r="35" spans="1:3" ht="14.25" customHeight="1">
       <c r="A35" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B35" t="s">
-        <v>55</v>
+        <v>57</v>
+      </c>
+      <c r="C35" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="14.25" customHeight="1">
       <c r="A36" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B36" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C36" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A37" t="s">
-        <v>59</v>
-      </c>
-      <c r="B37" t="s">
-        <v>60</v>
-      </c>
-      <c r="C37" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="37" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="38" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A38" t="s">
+        <v>64</v>
+      </c>
+      <c r="B38" t="s">
+        <v>65</v>
+      </c>
+    </row>
     <row r="39" spans="1:3" ht="14.25" customHeight="1">
       <c r="A39" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B39" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="14.25" customHeight="1">
       <c r="A40" t="s">
-        <v>66</v>
+        <v>89</v>
       </c>
       <c r="B40" t="s">
-        <v>67</v>
+        <v>90</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="14.25" customHeight="1">
       <c r="A41" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="B41" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A42" t="s">
-        <v>100</v>
-      </c>
-      <c r="B42" t="s">
-        <v>101</v>
-      </c>
-    </row>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="43" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="44" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="45" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2911,7 +2898,6 @@
     <row r="748" ht="14.25" customHeight="1"/>
     <row r="749" ht="14.25" customHeight="1"/>
     <row r="750" ht="14.25" customHeight="1"/>
-    <row r="751" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
CA and WA state balancing
</commit_message>
<xml_diff>
--- a/STS IR Bot Performer/Data/Config.xlsx
+++ b/STS IR Bot Performer/Data/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\martin.martinez\Documents\github-IRBot\STS_InternalReviewBot\STS IR Bot Performer\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://taxwarellc-my.sharepoint.com/personal/nahuel_delacruz_sovos_com/Documents/Desktop/Nahuel/Projects/STS Internal Review bot/STS IR Bot Performer/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A22A375C-FE54-40F8-A840-F290BFAF03B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{A22A375C-FE54-40F8-A840-F290BFAF03B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C0C5C9EC-3041-4DCD-868E-F21734284AB6}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="111">
   <si>
     <t>Name</t>
   </si>
@@ -336,6 +336,39 @@
   </si>
   <si>
     <t>WIExceptionalCase</t>
+  </si>
+  <si>
+    <t>StateBalancing_TN_TabName</t>
+  </si>
+  <si>
+    <t>Filing Options</t>
+  </si>
+  <si>
+    <t>StateBalancing_TN_RegexGetCheckbox</t>
+  </si>
+  <si>
+    <t>\w+(?=.*Select to Balance Schedule E Only)</t>
+  </si>
+  <si>
+    <t>StateBalancing_ReturnNamesPossibilities</t>
+  </si>
+  <si>
+    <t>TN,CO DR-0100 XML,LA R-1029,HI,WA,GA,OK,CA,SC</t>
+  </si>
+  <si>
+    <t>StateBalancing_TN_TextCompareCheckbox</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>StateBalancing_WA_ReturnNameForCheckOtherDeductions</t>
+  </si>
+  <si>
+    <t>WA CHECK BALANCING STATE</t>
+  </si>
+  <si>
+    <t>This is a special return name and it is used to check if the values in the Detail tab are 0 or not</t>
   </si>
 </sst>
 </file>
@@ -1833,10 +1866,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z750"/>
+  <dimension ref="A1:Z751"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2190,12 +2223,50 @@
       </c>
     </row>
     <row r="42" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="43" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="43" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A43" t="s">
+        <v>104</v>
+      </c>
+      <c r="B43" t="s">
+        <v>105</v>
+      </c>
+    </row>
     <row r="44" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="45" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="46" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="47" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="48" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="45" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A45" t="s">
+        <v>100</v>
+      </c>
+      <c r="B45" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A46" t="s">
+        <v>102</v>
+      </c>
+      <c r="B46" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A47" t="s">
+        <v>106</v>
+      </c>
+      <c r="B47" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A48" t="s">
+        <v>108</v>
+      </c>
+      <c r="B48" t="s">
+        <v>109</v>
+      </c>
+      <c r="C48" t="s">
+        <v>110</v>
+      </c>
+    </row>
     <row r="49" ht="14.25" customHeight="1"/>
     <row r="50" ht="14.25" customHeight="1"/>
     <row r="51" ht="14.25" customHeight="1"/>
@@ -2898,6 +2969,7 @@
     <row r="748" ht="14.25" customHeight="1"/>
     <row r="749" ht="14.25" customHeight="1"/>
     <row r="750" ht="14.25" customHeight="1"/>
+    <row r="751" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Hawaii case State Balancing is finished. Need more testing
</commit_message>
<xml_diff>
--- a/STS IR Bot Performer/Data/Config.xlsx
+++ b/STS IR Bot Performer/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://taxwarellc-my.sharepoint.com/personal/nahuel_delacruz_sovos_com/Documents/Desktop/Nahuel/Projects/STS Internal Review bot/STS IR Bot Performer/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="40" documentId="13_ncr:1_{8B7C0F14-F936-4E5A-BAB7-938310E89832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4247658E-F81D-4EB0-BB8C-FFD8D45785AA}"/>
+  <xr:revisionPtr revIDLastSave="99" documentId="13_ncr:1_{8B7C0F14-F936-4E5A-BAB7-938310E89832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4FDB7EB6-3ACA-45CD-A4F5-5490CC656863}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="194">
   <si>
     <t>Name</t>
   </si>
@@ -317,9 +317,6 @@
     <t>PathTempDirectory</t>
   </si>
   <si>
-    <t>C:\Users\martin.martinez\Documents\UiPath\temp</t>
-  </si>
-  <si>
     <t>path where the dispatcher process saved the temporary file with the information</t>
   </si>
   <si>
@@ -341,9 +338,6 @@
     <t>PathTempToPDF</t>
   </si>
   <si>
-    <t>C:\Users\martin.martinez\Desktop\filesForTesting\pdfTemp.pdf</t>
-  </si>
-  <si>
     <t>path of the temporary pdf that the bot will create when downloading it from Tax Solver for the case of Jefferson County.</t>
   </si>
   <si>
@@ -438,6 +432,192 @@
   </si>
   <si>
     <t>More info about special hotkeys: https://stackoverflow.com/questions/53170614/rpa-uipath-regarding-special-keystrokes</t>
+  </si>
+  <si>
+    <t>StateBalancing_HI_PartII_RegexOahu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(?&lt;=Oahu Taxation District.NET TAX\n.Retailing.)[\d\.\,]+(?=.\n) </t>
+  </si>
+  <si>
+    <t>StateBalancing_HI_PartII_RegexHawaii</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(?&lt;=Hawaii Taxation District.NET TAX\n.Retailing.)[\d\.\,]+(?=.\n) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(?&lt;=Kauai Taxation District.NET TAX\n.Retailing.)[\d\.\,]+(?=.\n) </t>
+  </si>
+  <si>
+    <t>StateBalancing_HI_PartII_RegexKauai</t>
+  </si>
+  <si>
+    <t>StateBalancing_HI_PartII_HotkeysKauai</t>
+  </si>
+  <si>
+    <t>StateBalancing_HI_PartII_Position</t>
+  </si>
+  <si>
+    <t>StateBalancing_HI_PagePartII</t>
+  </si>
+  <si>
+    <t>Part II - Current</t>
+  </si>
+  <si>
+    <t>StateBalancing_HI_PagePartIII</t>
+  </si>
+  <si>
+    <t>Part III thru V</t>
+  </si>
+  <si>
+    <t>Regex to get text (multiline) between two substrings: (\n|.)*?</t>
+  </si>
+  <si>
+    <t>(?&lt;=Part IV Current Period \- County Surcharge.*)(\n|.)*?(?=PART V Current Period \- SCHEDULE OF ASSIGNMENT OF TAXES BY DISTRICT)</t>
+  </si>
+  <si>
+    <t>StateBalancing_HI_RegexExtractTableText</t>
+  </si>
+  <si>
+    <t>(?&lt;=(Oahu|Hawaii|Kauai)\sTaxation\sDistrict\s+[\d\.\,]+\s+[\d\.\,]+\s+)[\d\.\,]+</t>
+  </si>
+  <si>
+    <t>Regex to get the numbers of the TAXABLE column. Must have 3 results</t>
+  </si>
+  <si>
+    <t>StateBalancing_HI_RegexGetTaxableColumnData</t>
+  </si>
+  <si>
+    <t>P:\TaxReturnOutSourcing\Preparer\UIPathPublish\IR Bot Temp Files</t>
+  </si>
+  <si>
+    <t>P:\TaxReturnOutSourcing\Preparer\UIPathPublish\IR Bot Temp Files\pdfTemp.pdf</t>
+  </si>
+  <si>
+    <t>ExportWorksheet_TempCsvFilename</t>
+  </si>
+  <si>
+    <t>TempCsvFile.csv</t>
+  </si>
+  <si>
+    <t>ExportWorksheet_ListCells_CO</t>
+  </si>
+  <si>
+    <t>DR-0100 XML Y1,AM1</t>
+  </si>
+  <si>
+    <t>CheckCreditHeld_ColumnName</t>
+  </si>
+  <si>
+    <t>Credit Held</t>
+  </si>
+  <si>
+    <t>StateBalancing_OK_TextToCompareInDT</t>
+  </si>
+  <si>
+    <t>No errors were found</t>
+  </si>
+  <si>
+    <t>text that the bot compares in the 'Pre Creation Check' table provided by TaxSolver.</t>
+  </si>
+  <si>
+    <t>StateBalancing_GA_TabName</t>
+  </si>
+  <si>
+    <t>Detail</t>
+  </si>
+  <si>
+    <t>StateBalancing_GA_RegexGetStateTotals</t>
+  </si>
+  <si>
+    <t>(?&lt;=State Totals \&gt;\s+)(\d+).*</t>
+  </si>
+  <si>
+    <t>StateBalancing_GA_RegexGetCountyTotals</t>
+  </si>
+  <si>
+    <t>(?&lt;=County Totals \&gt;\s+)(\d+).*</t>
+  </si>
+  <si>
+    <t>StateBalancing_GA_RegexToSplit</t>
+  </si>
+  <si>
+    <t>\s{3,}</t>
+  </si>
+  <si>
+    <t>StateBalancing_GA_ExpectedMatches</t>
+  </si>
+  <si>
+    <t>StateBalancing_GA_ExpectedSplitMatches</t>
+  </si>
+  <si>
+    <t>StateBalancing_GA_PositionInList</t>
+  </si>
+  <si>
+    <t>StateBalancing_CO_TabName</t>
+  </si>
+  <si>
+    <t>StateBalancing_CO_PathCsvTemp</t>
+  </si>
+  <si>
+    <t>P:\TaxReturnOutSourcing\Preparer\UIPathPublish\IR Bot Temp Files\tempCoCsv.csv</t>
+  </si>
+  <si>
+    <t>StateBalancing_CO_SheetnameCsvTemp</t>
+  </si>
+  <si>
+    <t>tempCoCsv</t>
+  </si>
+  <si>
+    <t>StateBalancing_CO_PathCOTool</t>
+  </si>
+  <si>
+    <t>C:\Users\martin.martinez\Desktop\filesForTesting\CO DR-0100 XML tool.xlsm</t>
+  </si>
+  <si>
+    <t>StateBalancing_CO_SelectForm</t>
+  </si>
+  <si>
+    <t>Information Sheet</t>
+  </si>
+  <si>
+    <t>StateBalancing_CO_urlWebsite</t>
+  </si>
+  <si>
+    <t>https://www.colorado.gov/revenueonline/</t>
+  </si>
+  <si>
+    <t>StateBalancing_CO_RegexGetStateRegistrationID</t>
+  </si>
+  <si>
+    <t>(?&lt;=State Registration ID\s+)(\d+).*</t>
+  </si>
+  <si>
+    <t>StateBalancing_CO_RegexToSplit</t>
+  </si>
+  <si>
+    <t>StateBalancing_CO_ExpectedMatches</t>
+  </si>
+  <si>
+    <t>StateBalancing_CO_ExpectedSplitMatches</t>
+  </si>
+  <si>
+    <t>StateBalancing_CO_PositionInList</t>
+  </si>
+  <si>
+    <t>StateBalancing_CO_MaximumColumn</t>
+  </si>
+  <si>
+    <t>StateBalancing_CO_SheetnameWebCOTool</t>
+  </si>
+  <si>
+    <t>Website</t>
+  </si>
+  <si>
+    <t>StateBalancing_CO_pathTXTCOWeb</t>
+  </si>
+  <si>
+    <t>P:\TaxReturnOutSourcing\Preparer\UIPathPublish\IR Bot Temp Files\txttemp.txt</t>
   </si>
 </sst>
 </file>
@@ -1935,10 +2115,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z755"/>
+  <dimension ref="A1:Z757"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2153,21 +2333,21 @@
         <v>92</v>
       </c>
       <c r="B22" t="s">
+        <v>150</v>
+      </c>
+      <c r="C22" t="s">
         <v>93</v>
-      </c>
-      <c r="C22" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" t="s">
+        <v>99</v>
+      </c>
+      <c r="B23" t="s">
+        <v>151</v>
+      </c>
+      <c r="C23" t="s">
         <v>100</v>
-      </c>
-      <c r="B23" t="s">
-        <v>101</v>
-      </c>
-      <c r="C23" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2192,13 +2372,13 @@
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
       <c r="A27" t="s">
+        <v>94</v>
+      </c>
+      <c r="B27" t="s">
         <v>95</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>96</v>
-      </c>
-      <c r="C27" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2272,863 +2452,1112 @@
     <row r="38" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="39" spans="1:3" ht="14.25" customHeight="1">
       <c r="A39" t="s">
-        <v>64</v>
+        <v>152</v>
       </c>
       <c r="B39" t="s">
-        <v>65</v>
+        <v>153</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="14.25" customHeight="1">
       <c r="A40" t="s">
-        <v>66</v>
+        <v>154</v>
       </c>
       <c r="B40" t="s">
-        <v>67</v>
+        <v>155</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="14.25" customHeight="1">
       <c r="A41" t="s">
-        <v>89</v>
+        <v>156</v>
       </c>
       <c r="B41" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A42" t="s">
-        <v>118</v>
-      </c>
-      <c r="B42" t="s">
-        <v>119</v>
-      </c>
-    </row>
+        <v>157</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="43" spans="1:3" ht="14.25" customHeight="1">
       <c r="A43" t="s">
-        <v>98</v>
+        <v>64</v>
       </c>
       <c r="B43" t="s">
-        <v>99</v>
+        <v>65</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="14.25" customHeight="1">
       <c r="A44" t="s">
-        <v>103</v>
+        <v>66</v>
       </c>
       <c r="B44" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="14.25" customHeight="1"/>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A45" t="s">
+        <v>89</v>
+      </c>
+      <c r="B45" t="s">
+        <v>90</v>
+      </c>
+    </row>
     <row r="46" spans="1:3" ht="14.25" customHeight="1">
       <c r="A46" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="B46" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="14.25" customHeight="1"/>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A47" t="s">
+        <v>97</v>
+      </c>
+      <c r="B47" t="s">
+        <v>98</v>
+      </c>
+    </row>
     <row r="48" spans="1:3" ht="14.25" customHeight="1">
       <c r="A48" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B48" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A49" t="s">
-        <v>109</v>
-      </c>
-      <c r="B49" t="s">
-        <v>110</v>
-      </c>
-    </row>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="50" spans="1:3" ht="14.25" customHeight="1">
       <c r="A50" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="B50" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A51" t="s">
-        <v>113</v>
-      </c>
-      <c r="B51" t="s">
-        <v>114</v>
-      </c>
-      <c r="C51" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" ht="14.25" customHeight="1"/>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="52" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A52" t="s">
+        <v>105</v>
+      </c>
+      <c r="B52" t="s">
+        <v>106</v>
+      </c>
+    </row>
     <row r="53" spans="1:3" ht="14.25" customHeight="1">
       <c r="A53" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="B53" t="s">
-        <v>117</v>
-      </c>
-      <c r="C53" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="14.25" customHeight="1">
       <c r="A54" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="B54" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A55" t="s">
-        <v>125</v>
-      </c>
-      <c r="B55">
-        <v>1</v>
-      </c>
-    </row>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="56" spans="1:3" ht="14.25" customHeight="1">
       <c r="A56" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="B56" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A57" t="s">
-        <v>124</v>
-      </c>
-      <c r="B57">
-        <v>1</v>
-      </c>
-    </row>
+        <v>112</v>
+      </c>
+      <c r="C56" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="58" spans="1:3" ht="14.25" customHeight="1">
       <c r="A58" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="B58" t="s">
-        <v>128</v>
+        <v>115</v>
+      </c>
+      <c r="C58" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="14.25" customHeight="1">
       <c r="A59" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="B59" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="14.25" customHeight="1">
       <c r="A60" t="s">
+        <v>123</v>
+      </c>
+      <c r="B60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A61" t="s">
+        <v>121</v>
+      </c>
+      <c r="B61" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A62" t="s">
+        <v>122</v>
+      </c>
+      <c r="B62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A63" t="s">
+        <v>124</v>
+      </c>
+      <c r="B63" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A64" t="s">
+        <v>125</v>
+      </c>
+      <c r="B64" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A65" t="s">
+        <v>128</v>
+      </c>
+      <c r="B65" t="s">
         <v>130</v>
       </c>
-      <c r="B60" t="s">
+      <c r="C65" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="67" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A67" t="s">
+        <v>158</v>
+      </c>
+      <c r="B67" t="s">
+        <v>159</v>
+      </c>
+      <c r="C67" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="69" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A69" t="s">
+        <v>161</v>
+      </c>
+      <c r="B69" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A70" t="s">
+        <v>163</v>
+      </c>
+      <c r="B70" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A71" t="s">
+        <v>165</v>
+      </c>
+      <c r="B71" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A72" t="s">
+        <v>167</v>
+      </c>
+      <c r="B72" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A73" t="s">
+        <v>169</v>
+      </c>
+      <c r="B73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A74" t="s">
+        <v>170</v>
+      </c>
+      <c r="B74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A75" t="s">
+        <v>171</v>
+      </c>
+      <c r="B75">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="77" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A77" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B77" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A78" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A79" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B79" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A80" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A81" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A82" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="B82" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A83" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B83" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A84" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B84" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A85" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A86" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A87" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A88" t="s">
+        <v>189</v>
+      </c>
+      <c r="B88">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A89" t="s">
+        <v>190</v>
+      </c>
+      <c r="B89" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A90" t="s">
+        <v>192</v>
+      </c>
+      <c r="B90" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="92" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A92" t="s">
         <v>132</v>
       </c>
-      <c r="C60" t="s">
+      <c r="B92" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="62" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="63" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="64" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="65" ht="14.25" customHeight="1"/>
-    <row r="66" ht="14.25" customHeight="1"/>
-    <row r="67" ht="14.25" customHeight="1"/>
-    <row r="68" ht="14.25" customHeight="1"/>
-    <row r="69" ht="14.25" customHeight="1"/>
-    <row r="70" ht="14.25" customHeight="1"/>
-    <row r="71" ht="14.25" customHeight="1"/>
-    <row r="72" ht="14.25" customHeight="1"/>
-    <row r="73" ht="14.25" customHeight="1"/>
-    <row r="74" ht="14.25" customHeight="1"/>
-    <row r="75" ht="14.25" customHeight="1"/>
-    <row r="76" ht="14.25" customHeight="1"/>
-    <row r="77" ht="14.25" customHeight="1"/>
-    <row r="78" ht="14.25" customHeight="1"/>
-    <row r="79" ht="14.25" customHeight="1"/>
-    <row r="80" ht="14.25" customHeight="1"/>
-    <row r="81" ht="14.25" customHeight="1"/>
-    <row r="82" ht="14.25" customHeight="1"/>
-    <row r="83" ht="14.25" customHeight="1"/>
-    <row r="84" ht="14.25" customHeight="1"/>
-    <row r="85" ht="14.25" customHeight="1"/>
-    <row r="86" ht="14.25" customHeight="1"/>
-    <row r="87" ht="14.25" customHeight="1"/>
-    <row r="88" ht="14.25" customHeight="1"/>
-    <row r="89" ht="14.25" customHeight="1"/>
-    <row r="90" ht="14.25" customHeight="1"/>
-    <row r="91" ht="14.25" customHeight="1"/>
-    <row r="92" ht="14.25" customHeight="1"/>
-    <row r="93" ht="14.25" customHeight="1"/>
-    <row r="94" ht="14.25" customHeight="1"/>
-    <row r="95" ht="14.25" customHeight="1"/>
-    <row r="96" ht="14.25" customHeight="1"/>
-    <row r="97" ht="14.25" customHeight="1"/>
-    <row r="98" ht="14.25" customHeight="1"/>
-    <row r="99" ht="14.25" customHeight="1"/>
-    <row r="100" ht="14.25" customHeight="1"/>
-    <row r="101" ht="14.25" customHeight="1"/>
-    <row r="102" ht="14.25" customHeight="1"/>
-    <row r="103" ht="14.25" customHeight="1"/>
-    <row r="104" ht="14.25" customHeight="1"/>
-    <row r="105" ht="14.25" customHeight="1"/>
-    <row r="106" ht="14.25" customHeight="1"/>
-    <row r="107" ht="14.25" customHeight="1"/>
-    <row r="108" ht="14.25" customHeight="1"/>
-    <row r="109" ht="14.25" customHeight="1"/>
-    <row r="110" ht="14.25" customHeight="1"/>
-    <row r="111" ht="14.25" customHeight="1"/>
-    <row r="112" ht="14.25" customHeight="1"/>
-    <row r="113" ht="14.25" customHeight="1"/>
-    <row r="114" ht="14.25" customHeight="1"/>
-    <row r="115" ht="14.25" customHeight="1"/>
-    <row r="116" ht="14.25" customHeight="1"/>
-    <row r="117" ht="14.25" customHeight="1"/>
-    <row r="118" ht="14.25" customHeight="1"/>
-    <row r="119" ht="14.25" customHeight="1"/>
-    <row r="120" ht="14.25" customHeight="1"/>
-    <row r="121" ht="14.25" customHeight="1"/>
-    <row r="122" ht="14.25" customHeight="1"/>
-    <row r="123" ht="14.25" customHeight="1"/>
-    <row r="124" ht="14.25" customHeight="1"/>
-    <row r="125" ht="14.25" customHeight="1"/>
-    <row r="126" ht="14.25" customHeight="1"/>
-    <row r="127" ht="14.25" customHeight="1"/>
-    <row r="128" ht="14.25" customHeight="1"/>
-    <row r="129" ht="14.25" customHeight="1"/>
-    <row r="130" ht="14.25" customHeight="1"/>
-    <row r="131" ht="14.25" customHeight="1"/>
-    <row r="132" ht="14.25" customHeight="1"/>
-    <row r="133" ht="14.25" customHeight="1"/>
-    <row r="134" ht="14.25" customHeight="1"/>
-    <row r="135" ht="14.25" customHeight="1"/>
-    <row r="136" ht="14.25" customHeight="1"/>
-    <row r="137" ht="14.25" customHeight="1"/>
-    <row r="138" ht="14.25" customHeight="1"/>
-    <row r="139" ht="14.25" customHeight="1"/>
-    <row r="140" ht="14.25" customHeight="1"/>
-    <row r="141" ht="14.25" customHeight="1"/>
-    <row r="142" ht="14.25" customHeight="1"/>
-    <row r="143" ht="14.25" customHeight="1"/>
-    <row r="144" ht="14.25" customHeight="1"/>
-    <row r="145" ht="14.25" customHeight="1"/>
-    <row r="146" ht="14.25" customHeight="1"/>
-    <row r="147" ht="14.25" customHeight="1"/>
-    <row r="148" ht="14.25" customHeight="1"/>
-    <row r="149" ht="14.25" customHeight="1"/>
-    <row r="150" ht="14.25" customHeight="1"/>
-    <row r="151" ht="14.25" customHeight="1"/>
-    <row r="152" ht="14.25" customHeight="1"/>
-    <row r="153" ht="14.25" customHeight="1"/>
-    <row r="154" ht="14.25" customHeight="1"/>
-    <row r="155" ht="14.25" customHeight="1"/>
-    <row r="156" ht="14.25" customHeight="1"/>
-    <row r="157" ht="14.25" customHeight="1"/>
-    <row r="158" ht="14.25" customHeight="1"/>
-    <row r="159" ht="14.25" customHeight="1"/>
-    <row r="160" ht="14.25" customHeight="1"/>
-    <row r="161" ht="14.25" customHeight="1"/>
-    <row r="162" ht="14.25" customHeight="1"/>
-    <row r="163" ht="14.25" customHeight="1"/>
-    <row r="164" ht="14.25" customHeight="1"/>
-    <row r="165" ht="14.25" customHeight="1"/>
-    <row r="166" ht="14.25" customHeight="1"/>
-    <row r="167" ht="14.25" customHeight="1"/>
-    <row r="168" ht="14.25" customHeight="1"/>
-    <row r="169" ht="14.25" customHeight="1"/>
-    <row r="170" ht="14.25" customHeight="1"/>
-    <row r="171" ht="14.25" customHeight="1"/>
-    <row r="172" ht="14.25" customHeight="1"/>
-    <row r="173" ht="14.25" customHeight="1"/>
-    <row r="174" ht="14.25" customHeight="1"/>
-    <row r="175" ht="14.25" customHeight="1"/>
-    <row r="176" ht="14.25" customHeight="1"/>
-    <row r="177" ht="14.25" customHeight="1"/>
-    <row r="178" ht="14.25" customHeight="1"/>
-    <row r="179" ht="14.25" customHeight="1"/>
-    <row r="180" ht="14.25" customHeight="1"/>
-    <row r="181" ht="14.25" customHeight="1"/>
-    <row r="182" ht="14.25" customHeight="1"/>
-    <row r="183" ht="14.25" customHeight="1"/>
-    <row r="184" ht="14.25" customHeight="1"/>
-    <row r="185" ht="14.25" customHeight="1"/>
-    <row r="186" ht="14.25" customHeight="1"/>
-    <row r="187" ht="14.25" customHeight="1"/>
-    <row r="188" ht="14.25" customHeight="1"/>
-    <row r="189" ht="14.25" customHeight="1"/>
-    <row r="190" ht="14.25" customHeight="1"/>
-    <row r="191" ht="14.25" customHeight="1"/>
-    <row r="192" ht="14.25" customHeight="1"/>
-    <row r="193" ht="14.25" customHeight="1"/>
-    <row r="194" ht="14.25" customHeight="1"/>
-    <row r="195" ht="14.25" customHeight="1"/>
-    <row r="196" ht="14.25" customHeight="1"/>
-    <row r="197" ht="14.25" customHeight="1"/>
-    <row r="198" ht="14.25" customHeight="1"/>
-    <row r="199" ht="14.25" customHeight="1"/>
-    <row r="200" ht="14.25" customHeight="1"/>
-    <row r="201" ht="14.25" customHeight="1"/>
-    <row r="202" ht="14.25" customHeight="1"/>
-    <row r="203" ht="14.25" customHeight="1"/>
-    <row r="204" ht="14.25" customHeight="1"/>
-    <row r="205" ht="14.25" customHeight="1"/>
-    <row r="206" ht="14.25" customHeight="1"/>
-    <row r="207" ht="14.25" customHeight="1"/>
-    <row r="208" ht="14.25" customHeight="1"/>
-    <row r="209" ht="14.25" customHeight="1"/>
-    <row r="210" ht="14.25" customHeight="1"/>
-    <row r="211" ht="14.25" customHeight="1"/>
-    <row r="212" ht="14.25" customHeight="1"/>
-    <row r="213" ht="14.25" customHeight="1"/>
-    <row r="214" ht="14.25" customHeight="1"/>
-    <row r="215" ht="14.25" customHeight="1"/>
-    <row r="216" ht="14.25" customHeight="1"/>
-    <row r="217" ht="14.25" customHeight="1"/>
-    <row r="218" ht="14.25" customHeight="1"/>
-    <row r="219" ht="14.25" customHeight="1"/>
-    <row r="220" ht="14.25" customHeight="1"/>
-    <row r="221" ht="14.25" customHeight="1"/>
-    <row r="222" ht="14.25" customHeight="1"/>
-    <row r="223" ht="14.25" customHeight="1"/>
-    <row r="224" ht="14.25" customHeight="1"/>
-    <row r="225" ht="14.25" customHeight="1"/>
-    <row r="226" ht="14.25" customHeight="1"/>
-    <row r="227" ht="14.25" customHeight="1"/>
-    <row r="228" ht="14.25" customHeight="1"/>
-    <row r="229" ht="14.25" customHeight="1"/>
-    <row r="230" ht="14.25" customHeight="1"/>
-    <row r="231" ht="14.25" customHeight="1"/>
-    <row r="232" ht="14.25" customHeight="1"/>
-    <row r="233" ht="14.25" customHeight="1"/>
-    <row r="234" ht="14.25" customHeight="1"/>
-    <row r="235" ht="14.25" customHeight="1"/>
-    <row r="236" ht="14.25" customHeight="1"/>
-    <row r="237" ht="14.25" customHeight="1"/>
-    <row r="238" ht="14.25" customHeight="1"/>
-    <row r="239" ht="14.25" customHeight="1"/>
-    <row r="240" ht="14.25" customHeight="1"/>
-    <row r="241" ht="14.25" customHeight="1"/>
-    <row r="242" ht="14.25" customHeight="1"/>
-    <row r="243" ht="14.25" customHeight="1"/>
-    <row r="244" ht="14.25" customHeight="1"/>
-    <row r="245" ht="14.25" customHeight="1"/>
-    <row r="246" ht="14.25" customHeight="1"/>
-    <row r="247" ht="14.25" customHeight="1"/>
-    <row r="248" ht="14.25" customHeight="1"/>
-    <row r="249" ht="14.25" customHeight="1"/>
-    <row r="250" ht="14.25" customHeight="1"/>
-    <row r="251" ht="14.25" customHeight="1"/>
-    <row r="252" ht="14.25" customHeight="1"/>
-    <row r="253" ht="14.25" customHeight="1"/>
-    <row r="254" ht="14.25" customHeight="1"/>
-    <row r="255" ht="14.25" customHeight="1"/>
-    <row r="256" ht="14.25" customHeight="1"/>
-    <row r="257" ht="14.25" customHeight="1"/>
-    <row r="258" ht="14.25" customHeight="1"/>
-    <row r="259" ht="14.25" customHeight="1"/>
-    <row r="260" ht="14.25" customHeight="1"/>
-    <row r="261" ht="14.25" customHeight="1"/>
-    <row r="262" ht="14.25" customHeight="1"/>
-    <row r="263" ht="14.25" customHeight="1"/>
-    <row r="264" ht="14.25" customHeight="1"/>
-    <row r="265" ht="14.25" customHeight="1"/>
-    <row r="266" ht="14.25" customHeight="1"/>
-    <row r="267" ht="14.25" customHeight="1"/>
-    <row r="268" ht="14.25" customHeight="1"/>
-    <row r="269" ht="14.25" customHeight="1"/>
-    <row r="270" ht="14.25" customHeight="1"/>
-    <row r="271" ht="14.25" customHeight="1"/>
-    <row r="272" ht="14.25" customHeight="1"/>
-    <row r="273" ht="14.25" customHeight="1"/>
-    <row r="274" ht="14.25" customHeight="1"/>
-    <row r="275" ht="14.25" customHeight="1"/>
-    <row r="276" ht="14.25" customHeight="1"/>
-    <row r="277" ht="14.25" customHeight="1"/>
-    <row r="278" ht="14.25" customHeight="1"/>
-    <row r="279" ht="14.25" customHeight="1"/>
-    <row r="280" ht="14.25" customHeight="1"/>
-    <row r="281" ht="14.25" customHeight="1"/>
-    <row r="282" ht="14.25" customHeight="1"/>
-    <row r="283" ht="14.25" customHeight="1"/>
-    <row r="284" ht="14.25" customHeight="1"/>
-    <row r="285" ht="14.25" customHeight="1"/>
-    <row r="286" ht="14.25" customHeight="1"/>
-    <row r="287" ht="14.25" customHeight="1"/>
-    <row r="288" ht="14.25" customHeight="1"/>
-    <row r="289" ht="14.25" customHeight="1"/>
-    <row r="290" ht="14.25" customHeight="1"/>
-    <row r="291" ht="14.25" customHeight="1"/>
-    <row r="292" ht="14.25" customHeight="1"/>
-    <row r="293" ht="14.25" customHeight="1"/>
-    <row r="294" ht="14.25" customHeight="1"/>
-    <row r="295" ht="14.25" customHeight="1"/>
-    <row r="296" ht="14.25" customHeight="1"/>
-    <row r="297" ht="14.25" customHeight="1"/>
-    <row r="298" ht="14.25" customHeight="1"/>
-    <row r="299" ht="14.25" customHeight="1"/>
-    <row r="300" ht="14.25" customHeight="1"/>
-    <row r="301" ht="14.25" customHeight="1"/>
-    <row r="302" ht="14.25" customHeight="1"/>
-    <row r="303" ht="14.25" customHeight="1"/>
-    <row r="304" ht="14.25" customHeight="1"/>
-    <row r="305" ht="14.25" customHeight="1"/>
-    <row r="306" ht="14.25" customHeight="1"/>
-    <row r="307" ht="14.25" customHeight="1"/>
-    <row r="308" ht="14.25" customHeight="1"/>
-    <row r="309" ht="14.25" customHeight="1"/>
-    <row r="310" ht="14.25" customHeight="1"/>
-    <row r="311" ht="14.25" customHeight="1"/>
-    <row r="312" ht="14.25" customHeight="1"/>
-    <row r="313" ht="14.25" customHeight="1"/>
-    <row r="314" ht="14.25" customHeight="1"/>
-    <row r="315" ht="14.25" customHeight="1"/>
-    <row r="316" ht="14.25" customHeight="1"/>
-    <row r="317" ht="14.25" customHeight="1"/>
-    <row r="318" ht="14.25" customHeight="1"/>
-    <row r="319" ht="14.25" customHeight="1"/>
-    <row r="320" ht="14.25" customHeight="1"/>
-    <row r="321" ht="14.25" customHeight="1"/>
-    <row r="322" ht="14.25" customHeight="1"/>
-    <row r="323" ht="14.25" customHeight="1"/>
-    <row r="324" ht="14.25" customHeight="1"/>
-    <row r="325" ht="14.25" customHeight="1"/>
-    <row r="326" ht="14.25" customHeight="1"/>
-    <row r="327" ht="14.25" customHeight="1"/>
-    <row r="328" ht="14.25" customHeight="1"/>
-    <row r="329" ht="14.25" customHeight="1"/>
-    <row r="330" ht="14.25" customHeight="1"/>
-    <row r="331" ht="14.25" customHeight="1"/>
-    <row r="332" ht="14.25" customHeight="1"/>
-    <row r="333" ht="14.25" customHeight="1"/>
-    <row r="334" ht="14.25" customHeight="1"/>
-    <row r="335" ht="14.25" customHeight="1"/>
-    <row r="336" ht="14.25" customHeight="1"/>
-    <row r="337" ht="14.25" customHeight="1"/>
-    <row r="338" ht="14.25" customHeight="1"/>
-    <row r="339" ht="14.25" customHeight="1"/>
-    <row r="340" ht="14.25" customHeight="1"/>
-    <row r="341" ht="14.25" customHeight="1"/>
-    <row r="342" ht="14.25" customHeight="1"/>
-    <row r="343" ht="14.25" customHeight="1"/>
-    <row r="344" ht="14.25" customHeight="1"/>
-    <row r="345" ht="14.25" customHeight="1"/>
-    <row r="346" ht="14.25" customHeight="1"/>
-    <row r="347" ht="14.25" customHeight="1"/>
-    <row r="348" ht="14.25" customHeight="1"/>
-    <row r="349" ht="14.25" customHeight="1"/>
-    <row r="350" ht="14.25" customHeight="1"/>
-    <row r="351" ht="14.25" customHeight="1"/>
-    <row r="352" ht="14.25" customHeight="1"/>
-    <row r="353" ht="14.25" customHeight="1"/>
-    <row r="354" ht="14.25" customHeight="1"/>
-    <row r="355" ht="14.25" customHeight="1"/>
-    <row r="356" ht="14.25" customHeight="1"/>
-    <row r="357" ht="14.25" customHeight="1"/>
-    <row r="358" ht="14.25" customHeight="1"/>
-    <row r="359" ht="14.25" customHeight="1"/>
-    <row r="360" ht="14.25" customHeight="1"/>
-    <row r="361" ht="14.25" customHeight="1"/>
-    <row r="362" ht="14.25" customHeight="1"/>
-    <row r="363" ht="14.25" customHeight="1"/>
-    <row r="364" ht="14.25" customHeight="1"/>
-    <row r="365" ht="14.25" customHeight="1"/>
-    <row r="366" ht="14.25" customHeight="1"/>
-    <row r="367" ht="14.25" customHeight="1"/>
-    <row r="368" ht="14.25" customHeight="1"/>
-    <row r="369" ht="14.25" customHeight="1"/>
-    <row r="370" ht="14.25" customHeight="1"/>
-    <row r="371" ht="14.25" customHeight="1"/>
-    <row r="372" ht="14.25" customHeight="1"/>
-    <row r="373" ht="14.25" customHeight="1"/>
-    <row r="374" ht="14.25" customHeight="1"/>
-    <row r="375" ht="14.25" customHeight="1"/>
-    <row r="376" ht="14.25" customHeight="1"/>
-    <row r="377" ht="14.25" customHeight="1"/>
-    <row r="378" ht="14.25" customHeight="1"/>
-    <row r="379" ht="14.25" customHeight="1"/>
-    <row r="380" ht="14.25" customHeight="1"/>
-    <row r="381" ht="14.25" customHeight="1"/>
-    <row r="382" ht="14.25" customHeight="1"/>
-    <row r="383" ht="14.25" customHeight="1"/>
-    <row r="384" ht="14.25" customHeight="1"/>
-    <row r="385" ht="14.25" customHeight="1"/>
-    <row r="386" ht="14.25" customHeight="1"/>
-    <row r="387" ht="14.25" customHeight="1"/>
-    <row r="388" ht="14.25" customHeight="1"/>
-    <row r="389" ht="14.25" customHeight="1"/>
-    <row r="390" ht="14.25" customHeight="1"/>
-    <row r="391" ht="14.25" customHeight="1"/>
-    <row r="392" ht="14.25" customHeight="1"/>
-    <row r="393" ht="14.25" customHeight="1"/>
-    <row r="394" ht="14.25" customHeight="1"/>
-    <row r="395" ht="14.25" customHeight="1"/>
-    <row r="396" ht="14.25" customHeight="1"/>
-    <row r="397" ht="14.25" customHeight="1"/>
-    <row r="398" ht="14.25" customHeight="1"/>
-    <row r="399" ht="14.25" customHeight="1"/>
-    <row r="400" ht="14.25" customHeight="1"/>
-    <row r="401" ht="14.25" customHeight="1"/>
-    <row r="402" ht="14.25" customHeight="1"/>
-    <row r="403" ht="14.25" customHeight="1"/>
-    <row r="404" ht="14.25" customHeight="1"/>
-    <row r="405" ht="14.25" customHeight="1"/>
-    <row r="406" ht="14.25" customHeight="1"/>
-    <row r="407" ht="14.25" customHeight="1"/>
-    <row r="408" ht="14.25" customHeight="1"/>
-    <row r="409" ht="14.25" customHeight="1"/>
-    <row r="410" ht="14.25" customHeight="1"/>
-    <row r="411" ht="14.25" customHeight="1"/>
-    <row r="412" ht="14.25" customHeight="1"/>
-    <row r="413" ht="14.25" customHeight="1"/>
-    <row r="414" ht="14.25" customHeight="1"/>
-    <row r="415" ht="14.25" customHeight="1"/>
-    <row r="416" ht="14.25" customHeight="1"/>
-    <row r="417" ht="14.25" customHeight="1"/>
-    <row r="418" ht="14.25" customHeight="1"/>
-    <row r="419" ht="14.25" customHeight="1"/>
-    <row r="420" ht="14.25" customHeight="1"/>
-    <row r="421" ht="14.25" customHeight="1"/>
-    <row r="422" ht="14.25" customHeight="1"/>
-    <row r="423" ht="14.25" customHeight="1"/>
-    <row r="424" ht="14.25" customHeight="1"/>
-    <row r="425" ht="14.25" customHeight="1"/>
-    <row r="426" ht="14.25" customHeight="1"/>
-    <row r="427" ht="14.25" customHeight="1"/>
-    <row r="428" ht="14.25" customHeight="1"/>
-    <row r="429" ht="14.25" customHeight="1"/>
-    <row r="430" ht="14.25" customHeight="1"/>
-    <row r="431" ht="14.25" customHeight="1"/>
-    <row r="432" ht="14.25" customHeight="1"/>
-    <row r="433" ht="14.25" customHeight="1"/>
-    <row r="434" ht="14.25" customHeight="1"/>
-    <row r="435" ht="14.25" customHeight="1"/>
-    <row r="436" ht="14.25" customHeight="1"/>
-    <row r="437" ht="14.25" customHeight="1"/>
-    <row r="438" ht="14.25" customHeight="1"/>
-    <row r="439" ht="14.25" customHeight="1"/>
-    <row r="440" ht="14.25" customHeight="1"/>
-    <row r="441" ht="14.25" customHeight="1"/>
-    <row r="442" ht="14.25" customHeight="1"/>
-    <row r="443" ht="14.25" customHeight="1"/>
-    <row r="444" ht="14.25" customHeight="1"/>
-    <row r="445" ht="14.25" customHeight="1"/>
-    <row r="446" ht="14.25" customHeight="1"/>
-    <row r="447" ht="14.25" customHeight="1"/>
-    <row r="448" ht="14.25" customHeight="1"/>
-    <row r="449" ht="14.25" customHeight="1"/>
-    <row r="450" ht="14.25" customHeight="1"/>
-    <row r="451" ht="14.25" customHeight="1"/>
-    <row r="452" ht="14.25" customHeight="1"/>
-    <row r="453" ht="14.25" customHeight="1"/>
-    <row r="454" ht="14.25" customHeight="1"/>
-    <row r="455" ht="14.25" customHeight="1"/>
-    <row r="456" ht="14.25" customHeight="1"/>
-    <row r="457" ht="14.25" customHeight="1"/>
-    <row r="458" ht="14.25" customHeight="1"/>
-    <row r="459" ht="14.25" customHeight="1"/>
-    <row r="460" ht="14.25" customHeight="1"/>
-    <row r="461" ht="14.25" customHeight="1"/>
-    <row r="462" ht="14.25" customHeight="1"/>
-    <row r="463" ht="14.25" customHeight="1"/>
-    <row r="464" ht="14.25" customHeight="1"/>
-    <row r="465" ht="14.25" customHeight="1"/>
-    <row r="466" ht="14.25" customHeight="1"/>
-    <row r="467" ht="14.25" customHeight="1"/>
-    <row r="468" ht="14.25" customHeight="1"/>
-    <row r="469" ht="14.25" customHeight="1"/>
-    <row r="470" ht="14.25" customHeight="1"/>
-    <row r="471" ht="14.25" customHeight="1"/>
-    <row r="472" ht="14.25" customHeight="1"/>
-    <row r="473" ht="14.25" customHeight="1"/>
-    <row r="474" ht="14.25" customHeight="1"/>
-    <row r="475" ht="14.25" customHeight="1"/>
-    <row r="476" ht="14.25" customHeight="1"/>
-    <row r="477" ht="14.25" customHeight="1"/>
-    <row r="478" ht="14.25" customHeight="1"/>
-    <row r="479" ht="14.25" customHeight="1"/>
-    <row r="480" ht="14.25" customHeight="1"/>
-    <row r="481" ht="14.25" customHeight="1"/>
-    <row r="482" ht="14.25" customHeight="1"/>
-    <row r="483" ht="14.25" customHeight="1"/>
-    <row r="484" ht="14.25" customHeight="1"/>
-    <row r="485" ht="14.25" customHeight="1"/>
-    <row r="486" ht="14.25" customHeight="1"/>
-    <row r="487" ht="14.25" customHeight="1"/>
-    <row r="488" ht="14.25" customHeight="1"/>
-    <row r="489" ht="14.25" customHeight="1"/>
-    <row r="490" ht="14.25" customHeight="1"/>
-    <row r="491" ht="14.25" customHeight="1"/>
-    <row r="492" ht="14.25" customHeight="1"/>
-    <row r="493" ht="14.25" customHeight="1"/>
-    <row r="494" ht="14.25" customHeight="1"/>
-    <row r="495" ht="14.25" customHeight="1"/>
-    <row r="496" ht="14.25" customHeight="1"/>
-    <row r="497" ht="14.25" customHeight="1"/>
-    <row r="498" ht="14.25" customHeight="1"/>
-    <row r="499" ht="14.25" customHeight="1"/>
-    <row r="500" ht="14.25" customHeight="1"/>
-    <row r="501" ht="14.25" customHeight="1"/>
-    <row r="502" ht="14.25" customHeight="1"/>
-    <row r="503" ht="14.25" customHeight="1"/>
-    <row r="504" ht="14.25" customHeight="1"/>
-    <row r="505" ht="14.25" customHeight="1"/>
-    <row r="506" ht="14.25" customHeight="1"/>
-    <row r="507" ht="14.25" customHeight="1"/>
-    <row r="508" ht="14.25" customHeight="1"/>
-    <row r="509" ht="14.25" customHeight="1"/>
-    <row r="510" ht="14.25" customHeight="1"/>
-    <row r="511" ht="14.25" customHeight="1"/>
-    <row r="512" ht="14.25" customHeight="1"/>
-    <row r="513" ht="14.25" customHeight="1"/>
-    <row r="514" ht="14.25" customHeight="1"/>
-    <row r="515" ht="14.25" customHeight="1"/>
-    <row r="516" ht="14.25" customHeight="1"/>
-    <row r="517" ht="14.25" customHeight="1"/>
-    <row r="518" ht="14.25" customHeight="1"/>
-    <row r="519" ht="14.25" customHeight="1"/>
-    <row r="520" ht="14.25" customHeight="1"/>
-    <row r="521" ht="14.25" customHeight="1"/>
-    <row r="522" ht="14.25" customHeight="1"/>
-    <row r="523" ht="14.25" customHeight="1"/>
-    <row r="524" ht="14.25" customHeight="1"/>
-    <row r="525" ht="14.25" customHeight="1"/>
-    <row r="526" ht="14.25" customHeight="1"/>
-    <row r="527" ht="14.25" customHeight="1"/>
-    <row r="528" ht="14.25" customHeight="1"/>
-    <row r="529" ht="14.25" customHeight="1"/>
-    <row r="530" ht="14.25" customHeight="1"/>
-    <row r="531" ht="14.25" customHeight="1"/>
-    <row r="532" ht="14.25" customHeight="1"/>
-    <row r="533" ht="14.25" customHeight="1"/>
-    <row r="534" ht="14.25" customHeight="1"/>
-    <row r="535" ht="14.25" customHeight="1"/>
-    <row r="536" ht="14.25" customHeight="1"/>
-    <row r="537" ht="14.25" customHeight="1"/>
-    <row r="538" ht="14.25" customHeight="1"/>
-    <row r="539" ht="14.25" customHeight="1"/>
-    <row r="540" ht="14.25" customHeight="1"/>
-    <row r="541" ht="14.25" customHeight="1"/>
-    <row r="542" ht="14.25" customHeight="1"/>
-    <row r="543" ht="14.25" customHeight="1"/>
-    <row r="544" ht="14.25" customHeight="1"/>
-    <row r="545" ht="14.25" customHeight="1"/>
-    <row r="546" ht="14.25" customHeight="1"/>
-    <row r="547" ht="14.25" customHeight="1"/>
-    <row r="548" ht="14.25" customHeight="1"/>
-    <row r="549" ht="14.25" customHeight="1"/>
-    <row r="550" ht="14.25" customHeight="1"/>
-    <row r="551" ht="14.25" customHeight="1"/>
-    <row r="552" ht="14.25" customHeight="1"/>
-    <row r="553" ht="14.25" customHeight="1"/>
-    <row r="554" ht="14.25" customHeight="1"/>
-    <row r="555" ht="14.25" customHeight="1"/>
-    <row r="556" ht="14.25" customHeight="1"/>
-    <row r="557" ht="14.25" customHeight="1"/>
-    <row r="558" ht="14.25" customHeight="1"/>
-    <row r="559" ht="14.25" customHeight="1"/>
-    <row r="560" ht="14.25" customHeight="1"/>
-    <row r="561" ht="14.25" customHeight="1"/>
-    <row r="562" ht="14.25" customHeight="1"/>
-    <row r="563" ht="14.25" customHeight="1"/>
-    <row r="564" ht="14.25" customHeight="1"/>
-    <row r="565" ht="14.25" customHeight="1"/>
-    <row r="566" ht="14.25" customHeight="1"/>
-    <row r="567" ht="14.25" customHeight="1"/>
-    <row r="568" ht="14.25" customHeight="1"/>
-    <row r="569" ht="14.25" customHeight="1"/>
-    <row r="570" ht="14.25" customHeight="1"/>
-    <row r="571" ht="14.25" customHeight="1"/>
-    <row r="572" ht="14.25" customHeight="1"/>
-    <row r="573" ht="14.25" customHeight="1"/>
-    <row r="574" ht="14.25" customHeight="1"/>
-    <row r="575" ht="14.25" customHeight="1"/>
-    <row r="576" ht="14.25" customHeight="1"/>
-    <row r="577" ht="14.25" customHeight="1"/>
-    <row r="578" ht="14.25" customHeight="1"/>
-    <row r="579" ht="14.25" customHeight="1"/>
-    <row r="580" ht="14.25" customHeight="1"/>
-    <row r="581" ht="14.25" customHeight="1"/>
-    <row r="582" ht="14.25" customHeight="1"/>
-    <row r="583" ht="14.25" customHeight="1"/>
-    <row r="584" ht="14.25" customHeight="1"/>
-    <row r="585" ht="14.25" customHeight="1"/>
-    <row r="586" ht="14.25" customHeight="1"/>
-    <row r="587" ht="14.25" customHeight="1"/>
-    <row r="588" ht="14.25" customHeight="1"/>
-    <row r="589" ht="14.25" customHeight="1"/>
-    <row r="590" ht="14.25" customHeight="1"/>
-    <row r="591" ht="14.25" customHeight="1"/>
-    <row r="592" ht="14.25" customHeight="1"/>
-    <row r="593" ht="14.25" customHeight="1"/>
-    <row r="594" ht="14.25" customHeight="1"/>
-    <row r="595" ht="14.25" customHeight="1"/>
-    <row r="596" ht="14.25" customHeight="1"/>
-    <row r="597" ht="14.25" customHeight="1"/>
-    <row r="598" ht="14.25" customHeight="1"/>
-    <row r="599" ht="14.25" customHeight="1"/>
-    <row r="600" ht="14.25" customHeight="1"/>
-    <row r="601" ht="14.25" customHeight="1"/>
-    <row r="602" ht="14.25" customHeight="1"/>
-    <row r="603" ht="14.25" customHeight="1"/>
-    <row r="604" ht="14.25" customHeight="1"/>
-    <row r="605" ht="14.25" customHeight="1"/>
-    <row r="606" ht="14.25" customHeight="1"/>
-    <row r="607" ht="14.25" customHeight="1"/>
-    <row r="608" ht="14.25" customHeight="1"/>
-    <row r="609" ht="14.25" customHeight="1"/>
-    <row r="610" ht="14.25" customHeight="1"/>
-    <row r="611" ht="14.25" customHeight="1"/>
-    <row r="612" ht="14.25" customHeight="1"/>
-    <row r="613" ht="14.25" customHeight="1"/>
-    <row r="614" ht="14.25" customHeight="1"/>
-    <row r="615" ht="14.25" customHeight="1"/>
-    <row r="616" ht="14.25" customHeight="1"/>
-    <row r="617" ht="14.25" customHeight="1"/>
-    <row r="618" ht="14.25" customHeight="1"/>
-    <row r="619" ht="14.25" customHeight="1"/>
-    <row r="620" ht="14.25" customHeight="1"/>
-    <row r="621" ht="14.25" customHeight="1"/>
-    <row r="622" ht="14.25" customHeight="1"/>
-    <row r="623" ht="14.25" customHeight="1"/>
-    <row r="624" ht="14.25" customHeight="1"/>
-    <row r="625" ht="14.25" customHeight="1"/>
-    <row r="626" ht="14.25" customHeight="1"/>
-    <row r="627" ht="14.25" customHeight="1"/>
-    <row r="628" ht="14.25" customHeight="1"/>
-    <row r="629" ht="14.25" customHeight="1"/>
-    <row r="630" ht="14.25" customHeight="1"/>
-    <row r="631" ht="14.25" customHeight="1"/>
-    <row r="632" ht="14.25" customHeight="1"/>
-    <row r="633" ht="14.25" customHeight="1"/>
-    <row r="634" ht="14.25" customHeight="1"/>
-    <row r="635" ht="14.25" customHeight="1"/>
-    <row r="636" ht="14.25" customHeight="1"/>
-    <row r="637" ht="14.25" customHeight="1"/>
-    <row r="638" ht="14.25" customHeight="1"/>
-    <row r="639" ht="14.25" customHeight="1"/>
-    <row r="640" ht="14.25" customHeight="1"/>
-    <row r="641" ht="14.25" customHeight="1"/>
-    <row r="642" ht="14.25" customHeight="1"/>
-    <row r="643" ht="14.25" customHeight="1"/>
-    <row r="644" ht="14.25" customHeight="1"/>
-    <row r="645" ht="14.25" customHeight="1"/>
-    <row r="646" ht="14.25" customHeight="1"/>
-    <row r="647" ht="14.25" customHeight="1"/>
-    <row r="648" ht="14.25" customHeight="1"/>
-    <row r="649" ht="14.25" customHeight="1"/>
-    <row r="650" ht="14.25" customHeight="1"/>
-    <row r="651" ht="14.25" customHeight="1"/>
-    <row r="652" ht="14.25" customHeight="1"/>
-    <row r="653" ht="14.25" customHeight="1"/>
-    <row r="654" ht="14.25" customHeight="1"/>
-    <row r="655" ht="14.25" customHeight="1"/>
-    <row r="656" ht="14.25" customHeight="1"/>
-    <row r="657" ht="14.25" customHeight="1"/>
-    <row r="658" ht="14.25" customHeight="1"/>
-    <row r="659" ht="14.25" customHeight="1"/>
-    <row r="660" ht="14.25" customHeight="1"/>
-    <row r="661" ht="14.25" customHeight="1"/>
-    <row r="662" ht="14.25" customHeight="1"/>
-    <row r="663" ht="14.25" customHeight="1"/>
-    <row r="664" ht="14.25" customHeight="1"/>
-    <row r="665" ht="14.25" customHeight="1"/>
-    <row r="666" ht="14.25" customHeight="1"/>
-    <row r="667" ht="14.25" customHeight="1"/>
-    <row r="668" ht="14.25" customHeight="1"/>
-    <row r="669" ht="14.25" customHeight="1"/>
-    <row r="670" ht="14.25" customHeight="1"/>
-    <row r="671" ht="14.25" customHeight="1"/>
-    <row r="672" ht="14.25" customHeight="1"/>
-    <row r="673" ht="14.25" customHeight="1"/>
-    <row r="674" ht="14.25" customHeight="1"/>
-    <row r="675" ht="14.25" customHeight="1"/>
-    <row r="676" ht="14.25" customHeight="1"/>
-    <row r="677" ht="14.25" customHeight="1"/>
-    <row r="678" ht="14.25" customHeight="1"/>
-    <row r="679" ht="14.25" customHeight="1"/>
-    <row r="680" ht="14.25" customHeight="1"/>
-    <row r="681" ht="14.25" customHeight="1"/>
-    <row r="682" ht="14.25" customHeight="1"/>
-    <row r="683" ht="14.25" customHeight="1"/>
-    <row r="684" ht="14.25" customHeight="1"/>
-    <row r="685" ht="14.25" customHeight="1"/>
-    <row r="686" ht="14.25" customHeight="1"/>
-    <row r="687" ht="14.25" customHeight="1"/>
-    <row r="688" ht="14.25" customHeight="1"/>
-    <row r="689" ht="14.25" customHeight="1"/>
-    <row r="690" ht="14.25" customHeight="1"/>
-    <row r="691" ht="14.25" customHeight="1"/>
-    <row r="692" ht="14.25" customHeight="1"/>
-    <row r="693" ht="14.25" customHeight="1"/>
-    <row r="694" ht="14.25" customHeight="1"/>
-    <row r="695" ht="14.25" customHeight="1"/>
-    <row r="696" ht="14.25" customHeight="1"/>
-    <row r="697" ht="14.25" customHeight="1"/>
-    <row r="698" ht="14.25" customHeight="1"/>
-    <row r="699" ht="14.25" customHeight="1"/>
-    <row r="700" ht="14.25" customHeight="1"/>
-    <row r="701" ht="14.25" customHeight="1"/>
-    <row r="702" ht="14.25" customHeight="1"/>
-    <row r="703" ht="14.25" customHeight="1"/>
-    <row r="704" ht="14.25" customHeight="1"/>
-    <row r="705" ht="14.25" customHeight="1"/>
-    <row r="706" ht="14.25" customHeight="1"/>
-    <row r="707" ht="14.25" customHeight="1"/>
-    <row r="708" ht="14.25" customHeight="1"/>
-    <row r="709" ht="14.25" customHeight="1"/>
-    <row r="710" ht="14.25" customHeight="1"/>
-    <row r="711" ht="14.25" customHeight="1"/>
-    <row r="712" ht="14.25" customHeight="1"/>
-    <row r="713" ht="14.25" customHeight="1"/>
-    <row r="714" ht="14.25" customHeight="1"/>
-    <row r="715" ht="14.25" customHeight="1"/>
-    <row r="716" ht="14.25" customHeight="1"/>
-    <row r="717" ht="14.25" customHeight="1"/>
-    <row r="718" ht="14.25" customHeight="1"/>
-    <row r="719" ht="14.25" customHeight="1"/>
-    <row r="720" ht="14.25" customHeight="1"/>
-    <row r="721" ht="14.25" customHeight="1"/>
-    <row r="722" ht="14.25" customHeight="1"/>
-    <row r="723" ht="14.25" customHeight="1"/>
-    <row r="724" ht="14.25" customHeight="1"/>
-    <row r="725" ht="14.25" customHeight="1"/>
-    <row r="726" ht="14.25" customHeight="1"/>
-    <row r="727" ht="14.25" customHeight="1"/>
-    <row r="728" ht="14.25" customHeight="1"/>
-    <row r="729" ht="14.25" customHeight="1"/>
-    <row r="730" ht="14.25" customHeight="1"/>
-    <row r="731" ht="14.25" customHeight="1"/>
-    <row r="732" ht="14.25" customHeight="1"/>
-    <row r="733" ht="14.25" customHeight="1"/>
-    <row r="734" ht="14.25" customHeight="1"/>
-    <row r="735" ht="14.25" customHeight="1"/>
-    <row r="736" ht="14.25" customHeight="1"/>
-    <row r="737" ht="14.25" customHeight="1"/>
-    <row r="738" ht="14.25" customHeight="1"/>
-    <row r="739" ht="14.25" customHeight="1"/>
-    <row r="740" ht="14.25" customHeight="1"/>
-    <row r="741" ht="14.25" customHeight="1"/>
-    <row r="742" ht="14.25" customHeight="1"/>
-    <row r="743" ht="14.25" customHeight="1"/>
-    <row r="744" ht="14.25" customHeight="1"/>
-    <row r="745" ht="14.25" customHeight="1"/>
-    <row r="746" ht="14.25" customHeight="1"/>
-    <row r="747" ht="14.25" customHeight="1"/>
-    <row r="748" ht="14.25" customHeight="1"/>
-    <row r="749" ht="14.25" customHeight="1"/>
-    <row r="750" ht="14.25" customHeight="1"/>
-    <row r="751" ht="14.25" customHeight="1"/>
-    <row r="752" ht="14.25" customHeight="1"/>
-    <row r="753" ht="14.25" customHeight="1"/>
-    <row r="754" ht="14.25" customHeight="1"/>
-    <row r="755" ht="14.25" customHeight="1"/>
+    <row r="93" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A93" t="s">
+        <v>134</v>
+      </c>
+      <c r="B93" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A94" t="s">
+        <v>137</v>
+      </c>
+      <c r="B94" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A95" t="s">
+        <v>138</v>
+      </c>
+      <c r="B95" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A96" t="s">
+        <v>139</v>
+      </c>
+      <c r="B96">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A97" t="s">
+        <v>140</v>
+      </c>
+      <c r="B97" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A98" t="s">
+        <v>142</v>
+      </c>
+      <c r="B98" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A99" t="s">
+        <v>146</v>
+      </c>
+      <c r="B99" t="s">
+        <v>145</v>
+      </c>
+      <c r="C99" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A100" t="s">
+        <v>149</v>
+      </c>
+      <c r="B100" t="s">
+        <v>147</v>
+      </c>
+      <c r="C100" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="102" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="103" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="104" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="105" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="106" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="107" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="108" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="109" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="110" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="111" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="112" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="113" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="114" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="115" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="116" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="117" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="118" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="119" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="120" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="121" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="122" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="123" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="124" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="125" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="126" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="127" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="128" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="129" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="130" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="131" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="132" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="133" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="134" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="135" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="136" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="137" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="138" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="139" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="140" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="141" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="142" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="143" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="144" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="145" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="146" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="147" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="148" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="149" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="150" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="151" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="152" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="153" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="154" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="155" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="156" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="157" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="158" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="159" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="160" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="161" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="162" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="163" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="164" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="165" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="166" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="167" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="168" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="169" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="170" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="171" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="172" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="173" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="174" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="175" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="176" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="177" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="178" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="179" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="180" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="181" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="182" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="183" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="184" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="185" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="186" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="187" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="188" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="189" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="190" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="191" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="192" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="193" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="194" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="195" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="196" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="197" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="198" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="199" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="200" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="201" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="202" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="203" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="204" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="205" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="206" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="207" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="208" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="209" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="210" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="211" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="212" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="213" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="214" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="215" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="216" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="217" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="218" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="219" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="220" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="221" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="222" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="223" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="224" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="225" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="226" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="227" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="228" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="229" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="230" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="231" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="232" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="233" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="234" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="235" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="236" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="237" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="238" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="239" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="240" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="241" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="242" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="243" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="244" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="245" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="246" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="247" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="248" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="249" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="250" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="251" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="252" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="253" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="254" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="255" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="256" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="257" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="258" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="259" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="260" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="261" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="262" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="263" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="264" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="265" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="266" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="267" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="268" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="269" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="270" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="271" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="272" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="273" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="274" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="275" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="276" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="277" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="278" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="279" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="280" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="281" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="282" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="283" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="284" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="285" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="286" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="287" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="288" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="289" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="290" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="291" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="292" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="293" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="294" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="295" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="296" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="297" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="298" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="299" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="300" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="301" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="302" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="303" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="304" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="305" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="306" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="307" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="308" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="309" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="310" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="311" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="312" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="313" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="314" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="315" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="316" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="317" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="318" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="319" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="320" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="321" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="322" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="323" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="324" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="325" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="326" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="327" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="328" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="329" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="330" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="331" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="332" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="333" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="334" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="335" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="336" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="337" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="338" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="339" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="340" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="341" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="342" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="343" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="344" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="345" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="346" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="347" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="348" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="349" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="350" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="351" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="352" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="353" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="354" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="355" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="356" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="357" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="358" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="359" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="360" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="361" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="362" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="363" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="364" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="365" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="366" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="367" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="368" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="369" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="370" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="371" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="372" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="373" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="374" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="375" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="376" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="377" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="378" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="379" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="380" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="381" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="382" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="383" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="384" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="385" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="386" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="387" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="388" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="389" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="390" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="391" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="392" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="393" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="394" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="395" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="396" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="397" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="398" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="399" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="400" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="401" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="402" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="403" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="404" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="405" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="406" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="407" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="408" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="409" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="410" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="411" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="412" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="413" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="414" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="415" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="416" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="417" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="418" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="419" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="420" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="421" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="422" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="423" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="424" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="425" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="426" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="427" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="428" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="429" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="430" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="431" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="432" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="433" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="434" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="435" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="436" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="437" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="438" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="439" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="440" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="441" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="442" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="443" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="444" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="445" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="446" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="447" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="448" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="449" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="450" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="451" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="452" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="453" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="454" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="455" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="456" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="457" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="458" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="459" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="460" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="461" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="462" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="463" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="464" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="465" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="466" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="467" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="468" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="469" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="470" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="471" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="472" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="473" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="474" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="475" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="476" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="477" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="478" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="479" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="480" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="481" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="482" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="483" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="484" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="485" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="486" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="487" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="488" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="489" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="490" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="491" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="492" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="493" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="494" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="495" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="496" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="497" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="498" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="499" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="500" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="501" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="502" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="503" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="504" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="505" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="506" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="507" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="508" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="509" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="510" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="511" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="512" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="513" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="514" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="515" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="516" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="517" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="518" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="519" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="520" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="521" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="522" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="523" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="524" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="525" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="526" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="527" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="528" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="529" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="530" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="531" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="532" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="533" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="534" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="535" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="536" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="537" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="538" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="539" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="540" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="541" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="542" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="543" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="544" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="545" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="546" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="547" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="548" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="549" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="550" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="551" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="552" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="553" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="554" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="555" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="556" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="557" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="558" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="559" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="560" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="561" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="562" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="563" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="564" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="565" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="566" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="567" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="568" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="569" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="570" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="571" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="572" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="573" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="574" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="575" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="576" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="577" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="578" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="579" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="580" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="581" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="582" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="583" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="584" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="585" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="586" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="587" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="588" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="589" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="590" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="591" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="592" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="593" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="594" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="595" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="596" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="597" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="598" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="599" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="600" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="601" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="602" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="603" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="604" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="605" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="606" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="607" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="608" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="609" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="610" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="611" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="612" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="613" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="614" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="615" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="616" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="617" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="618" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="619" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="620" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="621" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="622" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="623" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="624" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="625" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="626" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="627" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="628" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="629" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="630" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="631" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="632" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="633" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="634" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="635" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="636" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="637" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="638" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="639" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="640" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="641" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="642" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="643" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="644" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="645" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="646" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="647" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="648" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="649" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="650" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="651" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="652" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="653" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="654" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="655" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="656" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="657" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="658" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="659" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="660" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="661" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="662" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="663" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="664" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="665" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="666" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="667" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="668" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="669" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="670" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="671" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="672" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="673" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="674" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="675" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="676" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="677" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="678" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="679" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="680" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="681" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="682" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="683" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="684" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="685" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="686" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="687" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="688" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="689" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="690" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="691" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="692" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="693" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="694" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="695" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="696" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="697" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="698" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="699" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="700" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="701" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="702" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="703" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="704" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="705" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="706" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="707" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="708" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="709" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="710" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="711" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="712" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="713" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="714" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="715" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="716" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="717" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="718" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="719" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="720" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="721" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="722" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="723" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="724" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="725" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="726" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="727" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="728" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="729" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="730" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="731" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="732" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="733" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="734" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="735" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="736" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="737" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="738" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="739" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="740" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="741" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="742" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="743" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="744" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="745" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="746" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="747" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="748" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="749" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="750" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="751" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="752" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="753" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="754" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="755" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="756" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="757" customFormat="1" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Changes in performer due to some tests for the demo.
</commit_message>
<xml_diff>
--- a/STS IR Bot Performer/Data/Config.xlsx
+++ b/STS IR Bot Performer/Data/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://taxwarellc-my.sharepoint.com/personal/martin_martinez_sovos_com/Documents/Other Deductions/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://taxwarellc-my.sharepoint.com/personal/nahuel_delacruz_sovos_com/Documents/Desktop/Nahuel/Projects/STS Internal Review bot/STS IR Bot Performer/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="115" documentId="13_ncr:1_{8B7C0F14-F936-4E5A-BAB7-938310E89832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6C71827B-8691-461A-B721-7370455C9928}"/>
+  <xr:revisionPtr revIDLastSave="118" documentId="13_ncr:1_{8B7C0F14-F936-4E5A-BAB7-938310E89832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{69970AB7-8563-4E44-A596-0225DD175B54}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -482,15 +482,9 @@
     <t>StateBalancing_CO_PathCsvTemp</t>
   </si>
   <si>
-    <t>P:\TaxReturnOutSourcing\Preparer\UIPathPublish\IR Bot Temp Files</t>
-  </si>
-  <si>
     <t>P:\TaxReturnOutSourcing\Preparer\UIPathPublish\IR Bot Temp Files\tempCoCsv.csv</t>
   </si>
   <si>
-    <t>P:\TaxReturnOutSourcing\Preparer\UIPathPublish\IR Bot Temp Files\pdfTemp.pdf</t>
-  </si>
-  <si>
     <t>tempCoCsv</t>
   </si>
   <si>
@@ -618,6 +612,12 @@
   </si>
   <si>
     <t>Credit Held</t>
+  </si>
+  <si>
+    <t>P:\TaxReturnOutSourcing\Preparer\UIPathPublish\IR Bot Temp Files\pdfTemp &lt;USERNAME&gt;.pdf</t>
+  </si>
+  <si>
+    <t>C:\Users\&lt;USERNAME&gt;\Documents\UiPath\temp</t>
   </si>
 </sst>
 </file>
@@ -695,10 +695,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2121,8 +2117,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z757"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2337,7 +2333,7 @@
         <v>92</v>
       </c>
       <c r="B22" t="s">
-        <v>148</v>
+        <v>193</v>
       </c>
       <c r="C22" t="s">
         <v>93</v>
@@ -2348,7 +2344,7 @@
         <v>99</v>
       </c>
       <c r="B23" t="s">
-        <v>150</v>
+        <v>192</v>
       </c>
       <c r="C23" t="s">
         <v>100</v>
@@ -2456,26 +2452,26 @@
     <row r="38" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="39" spans="1:3" ht="14.25" customHeight="1">
       <c r="A39" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B39" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="14.25" customHeight="1">
       <c r="A40" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B40" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="14.25" customHeight="1">
       <c r="A41" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B41" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2727,52 +2723,52 @@
         <v>147</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="14.25" customHeight="1">
       <c r="A79" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B79" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="14.25" customHeight="1">
       <c r="A80" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="14.25" customHeight="1">
       <c r="A81" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="14.25" customHeight="1">
       <c r="A82" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B82" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="14.25" customHeight="1">
       <c r="A83" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B83" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="14.25" customHeight="1">
       <c r="A84" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B84" t="s">
         <v>142</v>
@@ -2780,7 +2776,7 @@
     </row>
     <row r="85" spans="1:2" ht="14.25" customHeight="1">
       <c r="A85" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B85">
         <v>1</v>
@@ -2788,7 +2784,7 @@
     </row>
     <row r="86" spans="1:2" ht="14.25" customHeight="1">
       <c r="A86" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B86">
         <v>0</v>
@@ -2796,7 +2792,7 @@
     </row>
     <row r="87" spans="1:2" ht="14.25" customHeight="1">
       <c r="A87" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B87">
         <v>1</v>
@@ -2804,7 +2800,7 @@
     </row>
     <row r="88" spans="1:2" ht="14.25" customHeight="1">
       <c r="A88" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B88">
         <v>35</v>
@@ -2812,48 +2808,48 @@
     </row>
     <row r="89" spans="1:2" ht="14.25" customHeight="1">
       <c r="A89" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B89" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="14.25" customHeight="1">
       <c r="A90" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B90" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="92" spans="1:2" ht="14.25" customHeight="1">
       <c r="A92" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B92" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="14.25" customHeight="1">
       <c r="A93" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B93" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="14.25" customHeight="1">
       <c r="A94" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B94" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="14.25" customHeight="1">
       <c r="A95" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B95" t="s">
         <v>130</v>
@@ -2861,7 +2857,7 @@
     </row>
     <row r="96" spans="1:2" ht="14.25" customHeight="1">
       <c r="A96" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B96">
         <v>2</v>
@@ -2869,40 +2865,40 @@
     </row>
     <row r="97" spans="1:3" ht="14.25" customHeight="1">
       <c r="A97" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B97" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="14.25" customHeight="1">
       <c r="A98" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B98" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="14.25" customHeight="1">
       <c r="A99" t="s">
+        <v>180</v>
+      </c>
+      <c r="B99" t="s">
+        <v>181</v>
+      </c>
+      <c r="C99" t="s">
         <v>182</v>
-      </c>
-      <c r="B99" t="s">
-        <v>183</v>
-      </c>
-      <c r="C99" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="14.25" customHeight="1">
       <c r="A100" t="s">
+        <v>183</v>
+      </c>
+      <c r="B100" t="s">
+        <v>184</v>
+      </c>
+      <c r="C100" t="s">
         <v>185</v>
-      </c>
-      <c r="B100" t="s">
-        <v>186</v>
-      </c>
-      <c r="C100" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Hawaii done - Some fixes while running the demo.
</commit_message>
<xml_diff>
--- a/STS IR Bot Performer/Data/Config.xlsx
+++ b/STS IR Bot Performer/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://taxwarellc-my.sharepoint.com/personal/nahuel_delacruz_sovos_com/Documents/Desktop/Nahuel/Projects/STS Internal Review bot/STS IR Bot Performer/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="118" documentId="13_ncr:1_{8B7C0F14-F936-4E5A-BAB7-938310E89832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{69970AB7-8563-4E44-A596-0225DD175B54}"/>
+  <xr:revisionPtr revIDLastSave="131" documentId="13_ncr:1_{8B7C0F14-F936-4E5A-BAB7-938310E89832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BCDC09DB-F96F-4C38-8212-B756ABBA7291}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="195">
   <si>
     <t>Name</t>
   </si>
@@ -545,21 +545,12 @@
     <t>StateBalancing_HI_PartII_RegexOahu</t>
   </si>
   <si>
-    <t xml:space="preserve">(?&lt;=Oahu Taxation District.NET TAX\n.Retailing.)[\d\.\,]+(?=.\n) </t>
-  </si>
-  <si>
     <t>StateBalancing_HI_PartII_RegexHawaii</t>
   </si>
   <si>
-    <t xml:space="preserve">(?&lt;=Hawaii Taxation District.NET TAX\n.Retailing.)[\d\.\,]+(?=.\n) </t>
-  </si>
-  <si>
     <t>StateBalancing_HI_PartII_RegexKauai</t>
   </si>
   <si>
-    <t xml:space="preserve">(?&lt;=Kauai Taxation District.NET TAX\n.Retailing.)[\d\.\,]+(?=.\n) </t>
-  </si>
-  <si>
     <t>StateBalancing_HI_PartII_HotkeysKauai</t>
   </si>
   <si>
@@ -599,15 +590,6 @@
     <t>ExportWorksheet_TempCsvFilename</t>
   </si>
   <si>
-    <t>TempCsvFile.csv</t>
-  </si>
-  <si>
-    <t>ExportWorksheet_ListCells_CO</t>
-  </si>
-  <si>
-    <t>DR-0100 XML Y1,AM1</t>
-  </si>
-  <si>
     <t>CheckCreditHeld_ColumnName</t>
   </si>
   <si>
@@ -618,6 +600,27 @@
   </si>
   <si>
     <t>C:\Users\&lt;USERNAME&gt;\Documents\UiPath\temp</t>
+  </si>
+  <si>
+    <t>(?&lt;=Oahu\sTaxation\sDistrict.*NET\sTAX.*\n.*Retailing.*)[\d\.\,]+(?=.*\n)</t>
+  </si>
+  <si>
+    <t>(?&lt;=Hawaii\sTaxation\sDistrict.*NET\sTAX.*\n.*Retailing.*)[\d\.\,]+(?=.*\n)</t>
+  </si>
+  <si>
+    <t>(?&lt;=Kauai\sTaxation\sDistrict.*NET\sTAX.*\n.*Retailing.*)[\d\.\,]+(?=.*\n)</t>
+  </si>
+  <si>
+    <t>StateBalancing_HI_PartII_ExpectedMatches</t>
+  </si>
+  <si>
+    <t>Y1,AM1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ExportWorksheet_ListCells_CO_DR0100 XML </t>
+  </si>
+  <si>
+    <t>P:\TaxReturnOutSourcing\Preparer\UIPathPublish\IR Bot Temp Files\DetailWorksheetFile &lt;USERNAME&gt;.csv</t>
   </si>
 </sst>
 </file>
@@ -2115,10 +2118,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z757"/>
+  <dimension ref="A1:Z758"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2333,7 +2336,7 @@
         <v>92</v>
       </c>
       <c r="B22" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="C22" t="s">
         <v>93</v>
@@ -2344,7 +2347,7 @@
         <v>99</v>
       </c>
       <c r="B23" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="C23" t="s">
         <v>100</v>
@@ -2452,26 +2455,26 @@
     <row r="38" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="39" spans="1:3" ht="14.25" customHeight="1">
       <c r="A39" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B39" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="14.25" customHeight="1">
       <c r="A40" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="B40" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="14.25" customHeight="1">
       <c r="A41" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="B41" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2828,80 +2831,87 @@
         <v>168</v>
       </c>
       <c r="B92" t="s">
-        <v>169</v>
+        <v>188</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="14.25" customHeight="1">
       <c r="A93" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B93" t="s">
-        <v>171</v>
+        <v>189</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="14.25" customHeight="1">
       <c r="A94" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B94" t="s">
-        <v>173</v>
+        <v>190</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="14.25" customHeight="1">
       <c r="A95" t="s">
-        <v>174</v>
-      </c>
-      <c r="B95" t="s">
-        <v>130</v>
+        <v>191</v>
+      </c>
+      <c r="B95">
+        <v>7</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="14.25" customHeight="1">
       <c r="A96" t="s">
-        <v>175</v>
-      </c>
-      <c r="B96">
-        <v>2</v>
+        <v>171</v>
+      </c>
+      <c r="B96" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="14.25" customHeight="1">
       <c r="A97" t="s">
-        <v>176</v>
-      </c>
-      <c r="B97" t="s">
-        <v>177</v>
+        <v>172</v>
+      </c>
+      <c r="B97">
+        <v>2</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="14.25" customHeight="1">
       <c r="A98" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="B98" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="14.25" customHeight="1">
       <c r="A99" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="B99" t="s">
-        <v>181</v>
-      </c>
-      <c r="C99" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="14.25" customHeight="1">
       <c r="A100" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="B100" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="C100" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" ht="14.25" customHeight="1"/>
+        <v>179</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A101" t="s">
+        <v>180</v>
+      </c>
+      <c r="B101" t="s">
+        <v>181</v>
+      </c>
+      <c r="C101" t="s">
+        <v>182</v>
+      </c>
+    </row>
     <row r="102" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="103" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="104" spans="1:3" ht="14.25" customHeight="1"/>
@@ -3558,6 +3568,7 @@
     <row r="755" ht="14.25" customHeight="1"/>
     <row r="756" ht="14.25" customHeight="1"/>
     <row r="757" ht="14.25" customHeight="1"/>
+    <row r="758" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Delete old files. Fixes after the demo with Jaime. Click on Return was improved. Transaction reference: Legal entity was added
</commit_message>
<xml_diff>
--- a/STS IR Bot Performer/Data/Config.xlsx
+++ b/STS IR Bot Performer/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\martin.martinez\Documents\github-IRBot\STS_InternalReviewBot\STS IR Bot Performer\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://taxwarellc-my.sharepoint.com/personal/nahuel_delacruz_sovos_com/Documents/Desktop/Nahuel/Projects/STS Internal Review bot/STS IR Bot Performer/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6168EBD1-1BEF-415E-8C0A-5B125435311F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{6168EBD1-1BEF-415E-8C0A-5B125435311F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6C59714C-B305-42B8-A7A7-F68172EB3DB6}"/>
   <bookViews>
-    <workbookView xWindow="-28410" yWindow="480" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="197">
   <si>
     <t>Name</t>
   </si>
@@ -621,6 +621,12 @@
   </si>
   <si>
     <t>Data\Input\Other Deductions List.xlsx</t>
+  </si>
+  <si>
+    <t>OtherDeductionsList_NonLocalStates</t>
+  </si>
+  <si>
+    <t>Non-Local State Forms</t>
   </si>
 </sst>
 </file>
@@ -2118,10 +2124,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z758"/>
+  <dimension ref="A1:Z759"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2526,393 +2532,400 @@
         <v>101</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="50" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A50" t="s">
+    <row r="49" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A49" t="s">
+        <v>195</v>
+      </c>
+      <c r="B49" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="51" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A51" t="s">
         <v>102</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B51" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="52" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A52" t="s">
-        <v>104</v>
-      </c>
-      <c r="B52" t="s">
-        <v>105</v>
-      </c>
-    </row>
+    <row r="52" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="53" spans="1:3" ht="14.25" customHeight="1">
       <c r="A53" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B53" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="14.25" customHeight="1">
       <c r="A54" t="s">
+        <v>106</v>
+      </c>
+      <c r="B54" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A55" t="s">
         <v>108</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B55" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="56" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A56" t="s">
+    <row r="56" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="57" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A57" t="s">
         <v>110</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B57" t="s">
         <v>111</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C57" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="58" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A58" t="s">
-        <v>113</v>
-      </c>
-      <c r="B58" t="s">
-        <v>114</v>
-      </c>
-      <c r="C58" t="s">
-        <v>117</v>
-      </c>
-    </row>
+    <row r="58" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="59" spans="1:3" ht="14.25" customHeight="1">
       <c r="A59" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B59" t="s">
-        <v>119</v>
+        <v>114</v>
+      </c>
+      <c r="C59" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="14.25" customHeight="1">
       <c r="A60" t="s">
-        <v>120</v>
-      </c>
-      <c r="B60">
-        <v>1</v>
+        <v>118</v>
+      </c>
+      <c r="B60" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="14.25" customHeight="1">
       <c r="A61" t="s">
-        <v>121</v>
-      </c>
-      <c r="B61" t="s">
-        <v>122</v>
+        <v>120</v>
+      </c>
+      <c r="B61">
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="14.25" customHeight="1">
       <c r="A62" t="s">
-        <v>123</v>
-      </c>
-      <c r="B62">
-        <v>1</v>
+        <v>121</v>
+      </c>
+      <c r="B62" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="14.25" customHeight="1">
       <c r="A63" t="s">
-        <v>124</v>
-      </c>
-      <c r="B63" t="s">
-        <v>125</v>
+        <v>123</v>
+      </c>
+      <c r="B63">
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="14.25" customHeight="1">
       <c r="A64" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B64" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="14.25" customHeight="1">
       <c r="A65" t="s">
+        <v>126</v>
+      </c>
+      <c r="B65" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A66" t="s">
         <v>128</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B66" t="s">
         <v>129</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C66" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="67" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A67" t="s">
+    <row r="67" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="68" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A68" t="s">
         <v>131</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B68" t="s">
         <v>132</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C68" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="69" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A69" t="s">
-        <v>134</v>
-      </c>
-      <c r="B69" t="s">
-        <v>135</v>
-      </c>
-    </row>
+    <row r="69" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="70" spans="1:3" ht="14.25" customHeight="1">
       <c r="A70" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B70" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="14.25" customHeight="1">
       <c r="A71" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B71" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="14.25" customHeight="1">
       <c r="A72" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B72" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="14.25" customHeight="1">
       <c r="A73" t="s">
-        <v>142</v>
-      </c>
-      <c r="B73">
-        <v>1</v>
+        <v>140</v>
+      </c>
+      <c r="B73" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="14.25" customHeight="1">
       <c r="A74" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B74">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="14.25" customHeight="1">
       <c r="A75" t="s">
+        <v>143</v>
+      </c>
+      <c r="B75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A76" t="s">
         <v>144</v>
       </c>
-      <c r="B75">
+      <c r="B76">
         <v>2</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="77" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A77" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="B77" t="s">
-        <v>135</v>
-      </c>
-    </row>
+    <row r="77" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="78" spans="1:3" ht="14.25" customHeight="1">
       <c r="A78" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
+      </c>
+      <c r="B78" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="14.25" customHeight="1">
       <c r="A79" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="B79" t="s">
-        <v>148</v>
+        <v>146</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="14.25" customHeight="1">
       <c r="A80" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
+      </c>
+      <c r="B80" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="14.25" customHeight="1">
       <c r="A81" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="14.25" customHeight="1">
       <c r="A82" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="B82" t="s">
-        <v>155</v>
+        <v>152</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="14.25" customHeight="1">
       <c r="A83" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B83" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="14.25" customHeight="1">
       <c r="A84" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B84" t="s">
-        <v>141</v>
+        <v>156</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="14.25" customHeight="1">
       <c r="A85" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="B85">
-        <v>1</v>
+        <v>158</v>
+      </c>
+      <c r="B85" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="14.25" customHeight="1">
       <c r="A86" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B86">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="14.25" customHeight="1">
       <c r="A87" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A88" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="B87">
+      <c r="B88">
         <v>1</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A88" t="s">
-        <v>162</v>
-      </c>
-      <c r="B88">
-        <v>35</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="14.25" customHeight="1">
       <c r="A89" t="s">
-        <v>164</v>
-      </c>
-      <c r="B89" t="s">
-        <v>163</v>
+        <v>162</v>
+      </c>
+      <c r="B89">
+        <v>35</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="14.25" customHeight="1">
       <c r="A90" t="s">
+        <v>164</v>
+      </c>
+      <c r="B90" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A91" t="s">
         <v>166</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B91" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="91" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="92" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A92" t="s">
-        <v>167</v>
-      </c>
-      <c r="B92" t="s">
-        <v>187</v>
-      </c>
-    </row>
+    <row r="92" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="93" spans="1:2" ht="14.25" customHeight="1">
       <c r="A93" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B93" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="14.25" customHeight="1">
       <c r="A94" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B94" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="14.25" customHeight="1">
       <c r="A95" t="s">
-        <v>190</v>
-      </c>
-      <c r="B95">
-        <v>7</v>
+        <v>169</v>
+      </c>
+      <c r="B95" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="14.25" customHeight="1">
       <c r="A96" t="s">
-        <v>170</v>
-      </c>
-      <c r="B96" t="s">
-        <v>129</v>
+        <v>190</v>
+      </c>
+      <c r="B96">
+        <v>7</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="14.25" customHeight="1">
       <c r="A97" t="s">
-        <v>171</v>
-      </c>
-      <c r="B97">
-        <v>2</v>
+        <v>170</v>
+      </c>
+      <c r="B97" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="14.25" customHeight="1">
       <c r="A98" t="s">
-        <v>172</v>
-      </c>
-      <c r="B98" t="s">
-        <v>173</v>
+        <v>171</v>
+      </c>
+      <c r="B98">
+        <v>2</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="14.25" customHeight="1">
       <c r="A99" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B99" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="14.25" customHeight="1">
       <c r="A100" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B100" t="s">
-        <v>177</v>
-      </c>
-      <c r="C100" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="14.25" customHeight="1">
       <c r="A101" t="s">
+        <v>176</v>
+      </c>
+      <c r="B101" t="s">
+        <v>177</v>
+      </c>
+      <c r="C101" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A102" t="s">
         <v>179</v>
       </c>
-      <c r="B101" t="s">
+      <c r="B102" t="s">
         <v>180</v>
       </c>
-      <c r="C101" t="s">
+      <c r="C102" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="102" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="103" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="104" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="105" spans="1:3" ht="14.25" customHeight="1"/>
@@ -3569,6 +3582,7 @@
     <row r="756" ht="14.25" customHeight="1"/>
     <row r="757" ht="14.25" customHeight="1"/>
     <row r="758" ht="14.25" customHeight="1"/>
+    <row r="759" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Performer. Hawaii error amended. ScreenScraping matches: now it checks if there is empty matches and remove them from the list. OpenReturn timeout was changed. OtherDeductionsList was changed.
</commit_message>
<xml_diff>
--- a/STS IR Bot Performer/Data/Config.xlsx
+++ b/STS IR Bot Performer/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://taxwarellc-my.sharepoint.com/personal/nahuel_delacruz_sovos_com/Documents/Desktop/Nahuel/Projects/STS Internal Review bot/STS IR Bot Performer/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{6168EBD1-1BEF-415E-8C0A-5B125435311F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6C59714C-B305-42B8-A7A7-F68172EB3DB6}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{6168EBD1-1BEF-415E-8C0A-5B125435311F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CE9FEAB3-D6D5-4662-BB5F-45768AE8D6A2}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="211">
   <si>
     <t>Name</t>
   </si>
@@ -479,21 +479,12 @@
     <t>StateBalancing_CO_PathCsvTemp</t>
   </si>
   <si>
-    <t>P:\TaxReturnOutSourcing\Preparer\UIPathPublish\IR Bot Temp Files\tempCoCsv.csv</t>
-  </si>
-  <si>
     <t>tempCoCsv</t>
   </si>
   <si>
     <t>StateBalancing_CO_SheetnameCsvTemp</t>
   </si>
   <si>
-    <t>StateBalancing_CO_PathCOTool</t>
-  </si>
-  <si>
-    <t>C:\Users\martin.martinez\Desktop\filesForTesting\CO DR-0100 XML tool.xlsm</t>
-  </si>
-  <si>
     <t>StateBalancing_CO_SelectForm</t>
   </si>
   <si>
@@ -614,9 +605,6 @@
     <t>Y1,AM1</t>
   </si>
   <si>
-    <t xml:space="preserve">ExportWorksheet_ListCells_CO_DR0100 XML </t>
-  </si>
-  <si>
     <t>P:\TaxReturnOutSourcing\Preparer\UIPathPublish\IR Bot Temp Files\DetailWorksheetFile &lt;USERNAME&gt;.csv</t>
   </si>
   <si>
@@ -627,6 +615,60 @@
   </si>
   <si>
     <t>Non-Local State Forms</t>
+  </si>
+  <si>
+    <t>ExportWorksheet_ListCells_CO_DR0100_XML</t>
+  </si>
+  <si>
+    <t>StateBalancing_CO_PathCOToolTemplate</t>
+  </si>
+  <si>
+    <t>Data\Input\CO DR-0100 XML tool.xlsm</t>
+  </si>
+  <si>
+    <t>StateBalancing_CO_PathCOToolCopy</t>
+  </si>
+  <si>
+    <t>Data\Output\CO DR-0100 XML tool.xlsm</t>
+  </si>
+  <si>
+    <t>StateBalancing_CO_firstSheetCOTool</t>
+  </si>
+  <si>
+    <t>Hide-Unhide</t>
+  </si>
+  <si>
+    <t>StateBalancing_CO_DifferenceSheetCOTool</t>
+  </si>
+  <si>
+    <t>Rates-Service Fees</t>
+  </si>
+  <si>
+    <t>StateBalancing_CO_BalancingSheetCOTool</t>
+  </si>
+  <si>
+    <t>Balancing Sheet</t>
+  </si>
+  <si>
+    <t>StateBalancing_CO_firstCellCOTool</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>StateBalancing_CO_firstCellBalancingCOTool</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>StateBalancing_CO_secondCellBalancingCOTool</t>
+  </si>
+  <si>
+    <t>U6</t>
+  </si>
+  <si>
+    <t>P:\TaxReturnOutSourcing\Preparer\UIPathPublish\IR Bot Temp Files\tempCoCsv &lt;USERNAME&gt;.csv</t>
   </si>
 </sst>
 </file>
@@ -2124,10 +2166,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z759"/>
+  <dimension ref="A1:Z766"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B80" sqref="B80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2302,7 +2344,7 @@
         <v>62</v>
       </c>
       <c r="B17" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
@@ -2342,7 +2384,7 @@
         <v>91</v>
       </c>
       <c r="B22" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C22" t="s">
         <v>92</v>
@@ -2353,7 +2395,7 @@
         <v>98</v>
       </c>
       <c r="B23" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C23" t="s">
         <v>99</v>
@@ -2461,26 +2503,26 @@
     <row r="38" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="39" spans="1:3" ht="14.25" customHeight="1">
       <c r="A39" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B39" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="14.25" customHeight="1">
       <c r="A40" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B40" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="14.25" customHeight="1">
       <c r="A41" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B41" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2534,10 +2576,10 @@
     </row>
     <row r="49" spans="1:3" ht="14.25" customHeight="1">
       <c r="A49" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B49" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2740,199 +2782,248 @@
         <v>146</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>147</v>
+        <v>210</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="14.25" customHeight="1">
       <c r="A80" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B80" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="14.25" customHeight="1">
       <c r="A81" s="2" t="s">
-        <v>150</v>
+        <v>194</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>151</v>
+        <v>195</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="14.25" customHeight="1">
       <c r="A82" s="2" t="s">
-        <v>152</v>
+        <v>196</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>153</v>
+        <v>197</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="14.25" customHeight="1">
       <c r="A83" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="B83" t="s">
-        <v>155</v>
+        <v>149</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="14.25" customHeight="1">
       <c r="A84" s="2" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="B84" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="14.25" customHeight="1">
       <c r="A85" s="2" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B85" t="s">
-        <v>141</v>
+        <v>153</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="14.25" customHeight="1">
       <c r="A86" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="B86">
-        <v>1</v>
+        <v>155</v>
+      </c>
+      <c r="B86" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="14.25" customHeight="1">
       <c r="A87" s="2" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B87">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="14.25" customHeight="1">
       <c r="A88" s="2" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A89" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B89">
         <v>1</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A89" t="s">
-        <v>162</v>
-      </c>
-      <c r="B89">
-        <v>35</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="14.25" customHeight="1">
       <c r="A90" t="s">
-        <v>164</v>
-      </c>
-      <c r="B90" t="s">
-        <v>163</v>
+        <v>159</v>
+      </c>
+      <c r="B90">
+        <v>35</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="14.25" customHeight="1">
       <c r="A91" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="B91" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" ht="14.25" customHeight="1"/>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A92" t="s">
+        <v>163</v>
+      </c>
+      <c r="B92" t="s">
+        <v>162</v>
+      </c>
+    </row>
     <row r="93" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A93" t="s">
-        <v>167</v>
+      <c r="A93" s="2" t="s">
+        <v>198</v>
       </c>
       <c r="B93" t="s">
-        <v>187</v>
+        <v>199</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A94" t="s">
-        <v>168</v>
-      </c>
-      <c r="B94" t="s">
-        <v>188</v>
+      <c r="A94" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A95" t="s">
-        <v>169</v>
-      </c>
-      <c r="B95" t="s">
-        <v>189</v>
+      <c r="A95" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A96" t="s">
-        <v>190</v>
-      </c>
-      <c r="B96">
-        <v>7</v>
+      <c r="A96" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A97" t="s">
-        <v>170</v>
-      </c>
-      <c r="B97" t="s">
-        <v>129</v>
+      <c r="A97" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A98" t="s">
-        <v>171</v>
-      </c>
-      <c r="B98">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A99" t="s">
-        <v>172</v>
-      </c>
-      <c r="B99" t="s">
-        <v>173</v>
-      </c>
-    </row>
+      <c r="A98" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="100" spans="1:3" ht="14.25" customHeight="1">
       <c r="A100" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="B100" t="s">
-        <v>175</v>
+        <v>184</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="14.25" customHeight="1">
       <c r="A101" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="B101" t="s">
-        <v>177</v>
-      </c>
-      <c r="C101" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="14.25" customHeight="1">
       <c r="A102" t="s">
-        <v>179</v>
+        <v>166</v>
       </c>
       <c r="B102" t="s">
-        <v>180</v>
-      </c>
-      <c r="C102" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="104" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="105" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="106" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="107" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="108" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="109" spans="1:3" ht="14.25" customHeight="1"/>
+        <v>186</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A103" t="s">
+        <v>187</v>
+      </c>
+      <c r="B103">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A104" t="s">
+        <v>167</v>
+      </c>
+      <c r="B104" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A105" t="s">
+        <v>168</v>
+      </c>
+      <c r="B105">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A106" t="s">
+        <v>169</v>
+      </c>
+      <c r="B106" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A107" t="s">
+        <v>171</v>
+      </c>
+      <c r="B107" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A108" t="s">
+        <v>173</v>
+      </c>
+      <c r="B108" t="s">
+        <v>174</v>
+      </c>
+      <c r="C108" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A109" t="s">
+        <v>176</v>
+      </c>
+      <c r="B109" t="s">
+        <v>177</v>
+      </c>
+      <c r="C109" t="s">
+        <v>178</v>
+      </c>
+    </row>
     <row r="110" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="111" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="112" spans="1:3" ht="14.25" customHeight="1"/>
@@ -3583,6 +3674,13 @@
     <row r="757" ht="14.25" customHeight="1"/>
     <row r="758" ht="14.25" customHeight="1"/>
     <row r="759" ht="14.25" customHeight="1"/>
+    <row r="760" ht="14.25" customHeight="1"/>
+    <row r="761" ht="14.25" customHeight="1"/>
+    <row r="762" ht="14.25" customHeight="1"/>
+    <row r="763" ht="14.25" customHeight="1"/>
+    <row r="764" ht="14.25" customHeight="1"/>
+    <row r="765" ht="14.25" customHeight="1"/>
+    <row r="766" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Config with LA values. LA was changed in switch
</commit_message>
<xml_diff>
--- a/STS IR Bot Performer/Data/Config.xlsx
+++ b/STS IR Bot Performer/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://taxwarellc-my.sharepoint.com/personal/nahuel_delacruz_sovos_com/Documents/Desktop/Nahuel/Projects/STS Internal Review bot/STS IR Bot Performer/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{6168EBD1-1BEF-415E-8C0A-5B125435311F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CE9FEAB3-D6D5-4662-BB5F-45768AE8D6A2}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{6168EBD1-1BEF-415E-8C0A-5B125435311F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BD5D2072-0B29-47FD-9C21-F01C3CC80D3B}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="219">
   <si>
     <t>Name</t>
   </si>
@@ -347,9 +347,6 @@
     <t>StateBalancing_ReturnNamesPossibilities</t>
   </si>
   <si>
-    <t>TN,CO DR-0100 XML,LA R-1029,HI,WA,GA,OK,CA,SC</t>
-  </si>
-  <si>
     <t>StateBalancing_TN_TabName</t>
   </si>
   <si>
@@ -669,6 +666,33 @@
   </si>
   <si>
     <t>P:\TaxReturnOutSourcing\Preparer\UIPathPublish\IR Bot Temp Files\tempCoCsv &lt;USERNAME&gt;.csv</t>
+  </si>
+  <si>
+    <t>TN,CO DR-0100 XML,LA,HI,WA,GA,OK,CA,SC</t>
+  </si>
+  <si>
+    <t>StateBalancing_LA_SecondSelectTab</t>
+  </si>
+  <si>
+    <t>StateBalancing_LA_RegexToApply</t>
+  </si>
+  <si>
+    <t>(?&lt;=Monthly)(\s+(\d{1,3}(,\d{3})*(\.\d+)?))</t>
+  </si>
+  <si>
+    <t>StateBalancing_LA_ExpectedMatches</t>
+  </si>
+  <si>
+    <t>StateBalancing_LA_SplitRegex</t>
+  </si>
+  <si>
+    <t>\s+</t>
+  </si>
+  <si>
+    <t>StateBalancing_LA_ExpectedSplitElements</t>
+  </si>
+  <si>
+    <t>StateBalancing_LA_PositionInList</t>
   </si>
 </sst>
 </file>
@@ -2168,8 +2192,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z766"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B80" sqref="B80"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A116" sqref="A116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2344,7 +2368,7 @@
         <v>62</v>
       </c>
       <c r="B17" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
@@ -2384,7 +2408,7 @@
         <v>91</v>
       </c>
       <c r="B22" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C22" t="s">
         <v>92</v>
@@ -2395,7 +2419,7 @@
         <v>98</v>
       </c>
       <c r="B23" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C23" t="s">
         <v>99</v>
@@ -2503,26 +2527,26 @@
     <row r="38" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="39" spans="1:3" ht="14.25" customHeight="1">
       <c r="A39" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B39" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="14.25" customHeight="1">
       <c r="A40" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B40" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="14.25" customHeight="1">
       <c r="A41" t="s">
+        <v>179</v>
+      </c>
+      <c r="B41" t="s">
         <v>180</v>
-      </c>
-      <c r="B41" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2552,10 +2576,10 @@
     </row>
     <row r="46" spans="1:3" ht="14.25" customHeight="1">
       <c r="A46" t="s">
+        <v>114</v>
+      </c>
+      <c r="B46" t="s">
         <v>115</v>
-      </c>
-      <c r="B46" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="14.25" customHeight="1">
@@ -2576,10 +2600,10 @@
     </row>
     <row r="49" spans="1:3" ht="14.25" customHeight="1">
       <c r="A49" t="s">
+        <v>190</v>
+      </c>
+      <c r="B49" t="s">
         <v>191</v>
-      </c>
-      <c r="B49" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2588,69 +2612,69 @@
         <v>102</v>
       </c>
       <c r="B51" t="s">
-        <v>103</v>
+        <v>210</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="53" spans="1:3" ht="14.25" customHeight="1">
       <c r="A53" t="s">
+        <v>103</v>
+      </c>
+      <c r="B53" t="s">
         <v>104</v>
-      </c>
-      <c r="B53" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="14.25" customHeight="1">
       <c r="A54" t="s">
+        <v>105</v>
+      </c>
+      <c r="B54" t="s">
         <v>106</v>
-      </c>
-      <c r="B54" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="14.25" customHeight="1">
       <c r="A55" t="s">
+        <v>107</v>
+      </c>
+      <c r="B55" t="s">
         <v>108</v>
-      </c>
-      <c r="B55" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="57" spans="1:3" ht="14.25" customHeight="1">
       <c r="A57" t="s">
+        <v>109</v>
+      </c>
+      <c r="B57" t="s">
         <v>110</v>
       </c>
-      <c r="B57" t="s">
+      <c r="C57" t="s">
         <v>111</v>
-      </c>
-      <c r="C57" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="59" spans="1:3" ht="14.25" customHeight="1">
       <c r="A59" t="s">
+        <v>112</v>
+      </c>
+      <c r="B59" t="s">
         <v>113</v>
       </c>
-      <c r="B59" t="s">
-        <v>114</v>
-      </c>
       <c r="C59" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="14.25" customHeight="1">
       <c r="A60" t="s">
+        <v>117</v>
+      </c>
+      <c r="B60" t="s">
         <v>118</v>
-      </c>
-      <c r="B60" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="14.25" customHeight="1">
       <c r="A61" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B61">
         <v>1</v>
@@ -2658,15 +2682,15 @@
     </row>
     <row r="62" spans="1:3" ht="14.25" customHeight="1">
       <c r="A62" t="s">
+        <v>120</v>
+      </c>
+      <c r="B62" t="s">
         <v>121</v>
-      </c>
-      <c r="B62" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="14.25" customHeight="1">
       <c r="A63" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B63">
         <v>1</v>
@@ -2674,79 +2698,79 @@
     </row>
     <row r="64" spans="1:3" ht="14.25" customHeight="1">
       <c r="A64" t="s">
+        <v>123</v>
+      </c>
+      <c r="B64" t="s">
         <v>124</v>
-      </c>
-      <c r="B64" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="14.25" customHeight="1">
       <c r="A65" t="s">
+        <v>125</v>
+      </c>
+      <c r="B65" t="s">
         <v>126</v>
-      </c>
-      <c r="B65" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="14.25" customHeight="1">
       <c r="A66" t="s">
+        <v>127</v>
+      </c>
+      <c r="B66" t="s">
         <v>128</v>
       </c>
-      <c r="B66" t="s">
+      <c r="C66" t="s">
         <v>129</v>
-      </c>
-      <c r="C66" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="68" spans="1:3" ht="14.25" customHeight="1">
       <c r="A68" t="s">
+        <v>130</v>
+      </c>
+      <c r="B68" t="s">
         <v>131</v>
       </c>
-      <c r="B68" t="s">
+      <c r="C68" t="s">
         <v>132</v>
-      </c>
-      <c r="C68" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="70" spans="1:3" ht="14.25" customHeight="1">
       <c r="A70" t="s">
+        <v>133</v>
+      </c>
+      <c r="B70" t="s">
         <v>134</v>
-      </c>
-      <c r="B70" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="14.25" customHeight="1">
       <c r="A71" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B71" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="14.25" customHeight="1">
       <c r="A72" t="s">
+        <v>136</v>
+      </c>
+      <c r="B72" t="s">
         <v>137</v>
-      </c>
-      <c r="B72" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="14.25" customHeight="1">
       <c r="A73" t="s">
+        <v>139</v>
+      </c>
+      <c r="B73" t="s">
         <v>140</v>
-      </c>
-      <c r="B73" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="14.25" customHeight="1">
       <c r="A74" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B74">
         <v>1</v>
@@ -2754,7 +2778,7 @@
     </row>
     <row r="75" spans="1:3" ht="14.25" customHeight="1">
       <c r="A75" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B75">
         <v>0</v>
@@ -2762,7 +2786,7 @@
     </row>
     <row r="76" spans="1:3" ht="14.25" customHeight="1">
       <c r="A76" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B76">
         <v>2</v>
@@ -2771,79 +2795,79 @@
     <row r="77" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="78" spans="1:3" ht="14.25" customHeight="1">
       <c r="A78" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B78" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="14.25" customHeight="1">
       <c r="A79" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="14.25" customHeight="1">
       <c r="A80" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B80" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="14.25" customHeight="1">
       <c r="A81" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B81" s="2" t="s">
         <v>194</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="14.25" customHeight="1">
       <c r="A82" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B82" s="2" t="s">
         <v>196</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="14.25" customHeight="1">
       <c r="A83" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B83" s="2" t="s">
         <v>149</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="14.25" customHeight="1">
       <c r="A84" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B84" t="s">
         <v>151</v>
-      </c>
-      <c r="B84" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="14.25" customHeight="1">
       <c r="A85" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B85" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="14.25" customHeight="1">
       <c r="A86" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B86" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="14.25" customHeight="1">
       <c r="A87" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B87">
         <v>1</v>
@@ -2851,7 +2875,7 @@
     </row>
     <row r="88" spans="1:2" ht="14.25" customHeight="1">
       <c r="A88" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B88">
         <v>0</v>
@@ -2859,7 +2883,7 @@
     </row>
     <row r="89" spans="1:2" ht="14.25" customHeight="1">
       <c r="A89" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B89">
         <v>1</v>
@@ -2867,7 +2891,7 @@
     </row>
     <row r="90" spans="1:2" ht="14.25" customHeight="1">
       <c r="A90" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B90">
         <v>35</v>
@@ -2875,96 +2899,96 @@
     </row>
     <row r="91" spans="1:2" ht="14.25" customHeight="1">
       <c r="A91" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B91" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="14.25" customHeight="1">
       <c r="A92" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B92" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="14.25" customHeight="1">
       <c r="A93" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B93" t="s">
         <v>198</v>
-      </c>
-      <c r="B93" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="14.25" customHeight="1">
       <c r="A94" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="B94" s="2" t="s">
         <v>200</v>
-      </c>
-      <c r="B94" s="2" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="14.25" customHeight="1">
       <c r="A95" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B95" s="2" t="s">
         <v>202</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="14.25" customHeight="1">
       <c r="A96" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B96" s="2" t="s">
         <v>204</v>
-      </c>
-      <c r="B96" s="2" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="14.25" customHeight="1">
       <c r="A97" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="B97" s="2" t="s">
         <v>206</v>
-      </c>
-      <c r="B97" s="2" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="14.25" customHeight="1">
       <c r="A98" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="B98" s="2" t="s">
         <v>208</v>
-      </c>
-      <c r="B98" s="2" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="100" spans="1:3" ht="14.25" customHeight="1">
       <c r="A100" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B100" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="14.25" customHeight="1">
       <c r="A101" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B101" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="14.25" customHeight="1">
       <c r="A102" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B102" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="14.25" customHeight="1">
       <c r="A103" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B103">
         <v>7</v>
@@ -2972,15 +2996,15 @@
     </row>
     <row r="104" spans="1:3" ht="14.25" customHeight="1">
       <c r="A104" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B104" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="14.25" customHeight="1">
       <c r="A105" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B105">
         <v>2</v>
@@ -2988,61 +3012,103 @@
     </row>
     <row r="106" spans="1:3" ht="14.25" customHeight="1">
       <c r="A106" t="s">
+        <v>168</v>
+      </c>
+      <c r="B106" t="s">
         <v>169</v>
-      </c>
-      <c r="B106" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="14.25" customHeight="1">
       <c r="A107" t="s">
+        <v>170</v>
+      </c>
+      <c r="B107" t="s">
         <v>171</v>
-      </c>
-      <c r="B107" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="14.25" customHeight="1">
       <c r="A108" t="s">
+        <v>172</v>
+      </c>
+      <c r="B108" t="s">
         <v>173</v>
       </c>
-      <c r="B108" t="s">
+      <c r="C108" t="s">
         <v>174</v>
-      </c>
-      <c r="C108" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="14.25" customHeight="1">
       <c r="A109" t="s">
+        <v>175</v>
+      </c>
+      <c r="B109" t="s">
         <v>176</v>
       </c>
-      <c r="B109" t="s">
+      <c r="C109" t="s">
         <v>177</v>
       </c>
-      <c r="C109" t="s">
-        <v>178</v>
-      </c>
     </row>
     <row r="110" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="111" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="112" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="113" ht="14.25" customHeight="1"/>
-    <row r="114" ht="14.25" customHeight="1"/>
-    <row r="115" ht="14.25" customHeight="1"/>
-    <row r="116" ht="14.25" customHeight="1"/>
-    <row r="117" ht="14.25" customHeight="1"/>
-    <row r="118" ht="14.25" customHeight="1"/>
-    <row r="119" ht="14.25" customHeight="1"/>
-    <row r="120" ht="14.25" customHeight="1"/>
-    <row r="121" ht="14.25" customHeight="1"/>
-    <row r="122" ht="14.25" customHeight="1"/>
-    <row r="123" ht="14.25" customHeight="1"/>
-    <row r="124" ht="14.25" customHeight="1"/>
-    <row r="125" ht="14.25" customHeight="1"/>
-    <row r="126" ht="14.25" customHeight="1"/>
-    <row r="127" ht="14.25" customHeight="1"/>
-    <row r="128" ht="14.25" customHeight="1"/>
+    <row r="111" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A111" t="s">
+        <v>211</v>
+      </c>
+      <c r="B111" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A112" t="s">
+        <v>212</v>
+      </c>
+      <c r="B112" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A113" t="s">
+        <v>214</v>
+      </c>
+      <c r="B113">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A114" t="s">
+        <v>215</v>
+      </c>
+      <c r="B114" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A115" t="s">
+        <v>217</v>
+      </c>
+      <c r="B115">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A116" t="s">
+        <v>218</v>
+      </c>
+      <c r="B116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="118" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="119" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="120" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="121" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="122" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="123" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="124" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="125" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="126" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="127" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="128" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="129" ht="14.25" customHeight="1"/>
     <row r="130" ht="14.25" customHeight="1"/>
     <row r="131" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Hawaii State Balancing was amended. New hotkey added in the config file for Hawaii case. Click on Data Entry Type column in Taxsolver was changed. Now it clicks in State column instead. Invoke Workflow CopyInputFiles in Main. Moved before open the user form. CopyInputFiles workflow added in the dispatcher.
</commit_message>
<xml_diff>
--- a/STS IR Bot Performer/Data/Config.xlsx
+++ b/STS IR Bot Performer/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://taxwarellc-my.sharepoint.com/personal/nahuel_delacruz_sovos_com/Documents/Desktop/Nahuel/Projects/STS Internal Review bot/STS IR Bot Performer/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="40" documentId="13_ncr:1_{6168EBD1-1BEF-415E-8C0A-5B125435311F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{938C29CE-FE24-44CF-8129-1B249895933C}"/>
+  <xr:revisionPtr revIDLastSave="47" documentId="13_ncr:1_{6168EBD1-1BEF-415E-8C0A-5B125435311F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{812A0497-1243-4089-AE4F-684B254C161E}"/>
   <bookViews>
-    <workbookView xWindow="7125" yWindow="4335" windowWidth="21600" windowHeight="11265" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="224">
   <si>
     <t>Name</t>
   </si>
@@ -587,15 +587,6 @@
     <t>C:\Users\&lt;USERNAME&gt;\Documents\UiPath\temp</t>
   </si>
   <si>
-    <t>(?&lt;=Oahu\sTaxation\sDistrict.*NET\sTAX.*\n.*Retailing.*)[\d\.\,]+(?=.*\n)</t>
-  </si>
-  <si>
-    <t>(?&lt;=Hawaii\sTaxation\sDistrict.*NET\sTAX.*\n.*Retailing.*)[\d\.\,]+(?=.*\n)</t>
-  </si>
-  <si>
-    <t>(?&lt;=Kauai\sTaxation\sDistrict.*NET\sTAX.*\n.*Retailing.*)[\d\.\,]+(?=.*\n)</t>
-  </si>
-  <si>
     <t>StateBalancing_HI_PartII_ExpectedMatches</t>
   </si>
   <si>
@@ -705,6 +696,18 @@
   </si>
   <si>
     <t>\\somproddfs1.prod.sovos.org\depts\TaxReturnOutSourcing\Preparer\UIPathPublish\IR Bot Temp Files\InputFiles</t>
+  </si>
+  <si>
+    <t>(?&lt;=Kauai\sTaxation\sDistrict.*)[\d\.\,]+(?=.*\n)</t>
+  </si>
+  <si>
+    <t>(?&lt;=Hawaii\sTaxation\sDistrict.*)[\d\.\,]+(?=.*\n)</t>
+  </si>
+  <si>
+    <t>(?&lt;=Oahu\sTaxation\sDistrict.*)[\d\.\,]+(?=.*\n)</t>
+  </si>
+  <si>
+    <t>StateBalancing_HI_PartII_HotkeysHawaii</t>
   </si>
 </sst>
 </file>
@@ -2216,10 +2219,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z767"/>
+  <dimension ref="A1:Z768"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
+      <selection activeCell="A105" sqref="A105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2391,13 +2394,13 @@
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" spans="1:3" s="5" customFormat="1" ht="14.25" customHeight="1">
       <c r="A17" s="5" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="18" spans="1:3" s="6" customFormat="1" ht="14.25" customHeight="1">
@@ -2405,7 +2408,7 @@
         <v>62</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="19" spans="1:3" s="5" customFormat="1" ht="14.25" customHeight="1">
@@ -2413,7 +2416,7 @@
         <v>67</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>68</v>
@@ -2570,15 +2573,15 @@
         <v>178</v>
       </c>
       <c r="B40" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="14.25" customHeight="1">
       <c r="A41" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B41" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="14.25" customHeight="1">
@@ -2640,10 +2643,10 @@
     </row>
     <row r="50" spans="1:3" ht="14.25" customHeight="1">
       <c r="A50" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B50" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2652,7 +2655,7 @@
         <v>102</v>
       </c>
       <c r="B52" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2846,7 +2849,7 @@
         <v>145</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="14.25" customHeight="1">
@@ -2859,18 +2862,18 @@
     </row>
     <row r="82" spans="1:2" ht="14.25" customHeight="1">
       <c r="A82" s="2" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="14.25" customHeight="1">
       <c r="A83" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="14.25" customHeight="1">
@@ -2955,50 +2958,50 @@
     </row>
     <row r="94" spans="1:2" ht="14.25" customHeight="1">
       <c r="A94" s="2" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B94" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="14.25" customHeight="1">
       <c r="A95" s="2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="14.25" customHeight="1">
       <c r="A96" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="14.25" customHeight="1">
       <c r="A97" s="2" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="14.25" customHeight="1">
       <c r="A98" s="2" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="14.25" customHeight="1">
       <c r="A99" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="14.25" customHeight="1"/>
@@ -3007,7 +3010,7 @@
         <v>163</v>
       </c>
       <c r="B101" t="s">
-        <v>183</v>
+        <v>222</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="14.25" customHeight="1">
@@ -3015,7 +3018,7 @@
         <v>164</v>
       </c>
       <c r="B102" t="s">
-        <v>184</v>
+        <v>221</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="14.25" customHeight="1">
@@ -3023,20 +3026,20 @@
         <v>165</v>
       </c>
       <c r="B103" t="s">
-        <v>185</v>
+        <v>220</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="14.25" customHeight="1">
       <c r="A104" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B104">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="14.25" customHeight="1">
       <c r="A105" t="s">
-        <v>166</v>
+        <v>223</v>
       </c>
       <c r="B105" t="s">
         <v>128</v>
@@ -3044,100 +3047,107 @@
     </row>
     <row r="106" spans="1:3" ht="14.25" customHeight="1">
       <c r="A106" t="s">
-        <v>167</v>
-      </c>
-      <c r="B106">
-        <v>2</v>
+        <v>166</v>
+      </c>
+      <c r="B106" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="14.25" customHeight="1">
       <c r="A107" t="s">
-        <v>168</v>
-      </c>
-      <c r="B107" t="s">
-        <v>169</v>
+        <v>167</v>
+      </c>
+      <c r="B107">
+        <v>2</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="14.25" customHeight="1">
       <c r="A108" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B108" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="14.25" customHeight="1">
       <c r="A109" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B109" t="s">
-        <v>173</v>
-      </c>
-      <c r="C109" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="14.25" customHeight="1">
       <c r="A110" t="s">
+        <v>172</v>
+      </c>
+      <c r="B110" t="s">
+        <v>173</v>
+      </c>
+      <c r="C110" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A111" t="s">
         <v>175</v>
       </c>
-      <c r="B110" t="s">
+      <c r="B111" t="s">
         <v>176</v>
       </c>
-      <c r="C110" t="s">
+      <c r="C111" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="111" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="112" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A112" t="s">
-        <v>210</v>
-      </c>
-      <c r="B112" t="s">
-        <v>104</v>
-      </c>
-    </row>
+    <row r="112" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="113" spans="1:2" ht="14.25" customHeight="1">
       <c r="A113" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="B113" t="s">
-        <v>212</v>
+        <v>104</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="14.25" customHeight="1">
       <c r="A114" t="s">
-        <v>213</v>
-      </c>
-      <c r="B114">
-        <v>1</v>
+        <v>208</v>
+      </c>
+      <c r="B114" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="14.25" customHeight="1">
       <c r="A115" t="s">
-        <v>214</v>
-      </c>
-      <c r="B115" t="s">
-        <v>215</v>
+        <v>210</v>
+      </c>
+      <c r="B115">
+        <v>1</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="14.25" customHeight="1">
       <c r="A116" t="s">
-        <v>216</v>
-      </c>
-      <c r="B116">
-        <v>1</v>
+        <v>211</v>
+      </c>
+      <c r="B116" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="14.25" customHeight="1">
       <c r="A117" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="B117">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A118" t="s">
+        <v>214</v>
+      </c>
+      <c r="B118">
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="119" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="120" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="121" spans="1:2" ht="14.25" customHeight="1"/>
@@ -3787,6 +3797,7 @@
     <row r="765" ht="14.25" customHeight="1"/>
     <row r="766" ht="14.25" customHeight="1"/>
     <row r="767" ht="14.25" customHeight="1"/>
+    <row r="768" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
South California State balancing completed.
</commit_message>
<xml_diff>
--- a/STS IR Bot Performer/Data/Config.xlsx
+++ b/STS IR Bot Performer/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://taxwarellc-my.sharepoint.com/personal/nahuel_delacruz_sovos_com/Documents/Desktop/Nahuel/Projects/STS Internal Review bot/STS IR Bot Performer/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="47" documentId="13_ncr:1_{6168EBD1-1BEF-415E-8C0A-5B125435311F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{812A0497-1243-4089-AE4F-684B254C161E}"/>
+  <xr:revisionPtr revIDLastSave="90" documentId="13_ncr:1_{6168EBD1-1BEF-415E-8C0A-5B125435311F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3B141E85-259D-4176-BA32-CBA6E31C5934}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="245">
   <si>
     <t>Name</t>
   </si>
@@ -708,6 +708,69 @@
   </si>
   <si>
     <t>StateBalancing_HI_PartII_HotkeysHawaii</t>
+  </si>
+  <si>
+    <t>StateBalancing_SC_PathCsvTemp</t>
+  </si>
+  <si>
+    <t>P:\TaxReturnOutSourcing\Preparer\UIPathPublish\IR Bot Temp Files\tempScCsv &lt;USERNAME&gt;.csv</t>
+  </si>
+  <si>
+    <t>StateBalancing_SC_FormName</t>
+  </si>
+  <si>
+    <t>StateBalancing_SC_PathTool</t>
+  </si>
+  <si>
+    <t>StateBalancing_SC_Tool_DetailWorksheet</t>
+  </si>
+  <si>
+    <t>detail</t>
+  </si>
+  <si>
+    <t>Data\Input\SC ST 389 tool.xlsx</t>
+  </si>
+  <si>
+    <t>StateBalancing_SC_Tool_MainWorksheet</t>
+  </si>
+  <si>
+    <t>SC ST-389</t>
+  </si>
+  <si>
+    <t>SC ST-389 tool</t>
+  </si>
+  <si>
+    <t>StateBalancing_SC_DetailPageName</t>
+  </si>
+  <si>
+    <t>StateBalancing_SC_LocalTaxesPageName</t>
+  </si>
+  <si>
+    <t>Local Taxes</t>
+  </si>
+  <si>
+    <t>StateBalancing_SC_CountyList</t>
+  </si>
+  <si>
+    <t>The list of all county names that can appear in TaxSolver - LocalTaxes tab</t>
+  </si>
+  <si>
+    <t>StateBalancing_SC_GetLocalTaxesCounty</t>
+  </si>
+  <si>
+    <t>Regex to get county of each local tax in Taxsolver</t>
+  </si>
+  <si>
+    <t>StateBalancing_SC_Tool_StartCell</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>(&lt;COUNTY_LIST&gt;)\s+[\d\.\,]+\s+[\d\.\,]+</t>
+  </si>
+  <si>
+    <t>AIKEN|ALLENDALE|ANDERSON|BAMBERG|BARNWELL|BERKELEY|CALHOUN|CHARLESTON|CHEROKEE|CHESTER|CHESTERFIELD|CLARENDON|COLLETON|DARLINGTON|DILLON|EDGEFIELD|FLORENCE|GREENWOOD|HORRY|JASPER|KERSHAW|LANCASTER|LAURENS|LEE|LEXINGTON|MARION|MARLBORO|MCCORMICK|NEWBERRY|ORANGEBURG|RICHLAND|SALUDA|SPARTANBURG|SUMTER|WILLIAMSBURG|YORK</t>
   </si>
 </sst>
 </file>
@@ -2219,10 +2282,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z768"/>
+  <dimension ref="A1:Z769"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
-      <selection activeCell="A105" sqref="A105"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="B128" sqref="B128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3100,7 +3163,7 @@
       </c>
     </row>
     <row r="112" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="113" spans="1:2" ht="14.25" customHeight="1">
+    <row r="113" spans="1:3" ht="14.25" customHeight="1">
       <c r="A113" t="s">
         <v>207</v>
       </c>
@@ -3108,7 +3171,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="114" spans="1:2" ht="14.25" customHeight="1">
+    <row r="114" spans="1:3" ht="14.25" customHeight="1">
       <c r="A114" t="s">
         <v>208</v>
       </c>
@@ -3116,7 +3179,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="115" spans="1:2" ht="14.25" customHeight="1">
+    <row r="115" spans="1:3" ht="14.25" customHeight="1">
       <c r="A115" t="s">
         <v>210</v>
       </c>
@@ -3124,7 +3187,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:2" ht="14.25" customHeight="1">
+    <row r="116" spans="1:3" ht="14.25" customHeight="1">
       <c r="A116" t="s">
         <v>211</v>
       </c>
@@ -3132,7 +3195,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="117" spans="1:2" ht="14.25" customHeight="1">
+    <row r="117" spans="1:3" ht="14.25" customHeight="1">
       <c r="A117" t="s">
         <v>213</v>
       </c>
@@ -3140,7 +3203,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:2" ht="14.25" customHeight="1">
+    <row r="118" spans="1:3" ht="14.25" customHeight="1">
       <c r="A118" t="s">
         <v>214</v>
       </c>
@@ -3148,32 +3211,108 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="120" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="121" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="122" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="123" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="124" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="125" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="126" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="127" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="128" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="129" ht="14.25" customHeight="1"/>
-    <row r="130" ht="14.25" customHeight="1"/>
-    <row r="131" ht="14.25" customHeight="1"/>
-    <row r="132" ht="14.25" customHeight="1"/>
-    <row r="133" ht="14.25" customHeight="1"/>
-    <row r="134" ht="14.25" customHeight="1"/>
-    <row r="135" ht="14.25" customHeight="1"/>
-    <row r="136" ht="14.25" customHeight="1"/>
-    <row r="137" ht="14.25" customHeight="1"/>
-    <row r="138" ht="14.25" customHeight="1"/>
-    <row r="139" ht="14.25" customHeight="1"/>
-    <row r="140" ht="14.25" customHeight="1"/>
-    <row r="141" ht="14.25" customHeight="1"/>
-    <row r="142" ht="14.25" customHeight="1"/>
-    <row r="143" ht="14.25" customHeight="1"/>
-    <row r="144" ht="14.25" customHeight="1"/>
+    <row r="119" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="120" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A120" t="s">
+        <v>224</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A121" t="s">
+        <v>234</v>
+      </c>
+      <c r="B121" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A122" t="s">
+        <v>235</v>
+      </c>
+      <c r="B122" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A123" t="s">
+        <v>226</v>
+      </c>
+      <c r="B123" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A124" t="s">
+        <v>227</v>
+      </c>
+      <c r="B124" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A125" t="s">
+        <v>228</v>
+      </c>
+      <c r="B125" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A126" t="s">
+        <v>231</v>
+      </c>
+      <c r="B126" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A127" t="s">
+        <v>237</v>
+      </c>
+      <c r="B127" t="s">
+        <v>244</v>
+      </c>
+      <c r="C127" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A128" t="s">
+        <v>239</v>
+      </c>
+      <c r="B128" t="s">
+        <v>243</v>
+      </c>
+      <c r="C128" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A129" t="s">
+        <v>241</v>
+      </c>
+      <c r="B129" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="131" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="132" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="133" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="134" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="135" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="136" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="137" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="138" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="139" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="140" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="141" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="142" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="143" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="144" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="145" ht="14.25" customHeight="1"/>
     <row r="146" ht="14.25" customHeight="1"/>
     <row r="147" ht="14.25" customHeight="1"/>
@@ -3798,6 +3937,7 @@
     <row r="766" ht="14.25" customHeight="1"/>
     <row r="767" ht="14.25" customHeight="1"/>
     <row r="768" ht="14.25" customHeight="1"/>
+    <row r="769" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Performer. Click on OpenReturn was improved. Organized worfklows. LA State Balancing second version.
</commit_message>
<xml_diff>
--- a/STS IR Bot Performer/Data/Config.xlsx
+++ b/STS IR Bot Performer/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://taxwarellc-my.sharepoint.com/personal/nahuel_delacruz_sovos_com/Documents/Desktop/Nahuel/Projects/STS Internal Review bot/STS IR Bot Performer/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="90" documentId="13_ncr:1_{6168EBD1-1BEF-415E-8C0A-5B125435311F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3B141E85-259D-4176-BA32-CBA6E31C5934}"/>
+  <xr:revisionPtr revIDLastSave="124" documentId="13_ncr:1_{6168EBD1-1BEF-415E-8C0A-5B125435311F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{97A4B112-C99F-4ECC-B8FE-437F333941C3}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3465" yWindow="3465" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="259">
   <si>
     <t>Name</t>
   </si>
@@ -771,6 +771,48 @@
   </si>
   <si>
     <t>AIKEN|ALLENDALE|ANDERSON|BAMBERG|BARNWELL|BERKELEY|CALHOUN|CHARLESTON|CHEROKEE|CHESTER|CHESTERFIELD|CLARENDON|COLLETON|DARLINGTON|DILLON|EDGEFIELD|FLORENCE|GREENWOOD|HORRY|JASPER|KERSHAW|LANCASTER|LAURENS|LEE|LEXINGTON|MARION|MARLBORO|MCCORMICK|NEWBERRY|ORANGEBURG|RICHLAND|SALUDA|SPARTANBURG|SUMTER|WILLIAMSBURG|YORK</t>
+  </si>
+  <si>
+    <t>StateBalancing_LA_GrossSalesClickOnText</t>
+  </si>
+  <si>
+    <t>GROSS SALES OF TANGIBLE###Gross Sales of Tangible###Gross sales of tangible###Gross Sales of tangible</t>
+  </si>
+  <si>
+    <t>StateBalancing_LA_RegexGetMonthlyCheckbox</t>
+  </si>
+  <si>
+    <t>(?&lt;=\n.*)\w+(?=.*Monthly)</t>
+  </si>
+  <si>
+    <t>StateBalancing_LA_ListNonLocalStates</t>
+  </si>
+  <si>
+    <t>LA R-1029,LA R-1029E,LA R-1031</t>
+  </si>
+  <si>
+    <t>StateBalancing_LA_TableColumns</t>
+  </si>
+  <si>
+    <t>StateBalancing_LA_TemporalCsvFile</t>
+  </si>
+  <si>
+    <t>Data\TemporalFileLAStateBalancing.csv</t>
+  </si>
+  <si>
+    <t>StateBalancing_LA_ExceptionMessageQuarterlyReturn</t>
+  </si>
+  <si>
+    <t>This return is Quarterly. Gross Sales are:</t>
+  </si>
+  <si>
+    <t>ReturnType,FilingType,LegalEntity,ReturnName,CustomerName,GrossSales</t>
+  </si>
+  <si>
+    <t>For LA State Balancing 2nd version</t>
+  </si>
+  <si>
+    <t>StateBalancing_LA_GrossSalesTab</t>
   </si>
 </sst>
 </file>
@@ -2282,10 +2324,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z769"/>
+  <dimension ref="A1:Z776"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="B128" sqref="B128"/>
+      <selection activeCell="A119" sqref="A119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3211,108 +3253,160 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="119" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A119" t="s">
+        <v>258</v>
+      </c>
+      <c r="B119">
+        <v>1</v>
+      </c>
+    </row>
     <row r="120" spans="1:3" ht="14.25" customHeight="1">
       <c r="A120" t="s">
-        <v>224</v>
-      </c>
-      <c r="B120" s="2" t="s">
-        <v>225</v>
+        <v>245</v>
+      </c>
+      <c r="B120" t="s">
+        <v>246</v>
+      </c>
+      <c r="C120" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="14.25" customHeight="1">
       <c r="A121" t="s">
-        <v>234</v>
+        <v>247</v>
       </c>
       <c r="B121" t="s">
-        <v>134</v>
+        <v>248</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="14.25" customHeight="1">
       <c r="A122" t="s">
-        <v>235</v>
+        <v>249</v>
       </c>
       <c r="B122" t="s">
-        <v>236</v>
+        <v>250</v>
       </c>
     </row>
     <row r="123" spans="1:3" ht="14.25" customHeight="1">
       <c r="A123" t="s">
-        <v>226</v>
+        <v>252</v>
       </c>
       <c r="B123" t="s">
-        <v>232</v>
+        <v>253</v>
       </c>
     </row>
     <row r="124" spans="1:3" ht="14.25" customHeight="1">
       <c r="A124" t="s">
-        <v>227</v>
+        <v>251</v>
       </c>
       <c r="B124" t="s">
-        <v>230</v>
+        <v>256</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="14.25" customHeight="1">
       <c r="A125" t="s">
-        <v>228</v>
+        <v>254</v>
       </c>
       <c r="B125" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A126" t="s">
-        <v>231</v>
-      </c>
-      <c r="B126" t="s">
-        <v>233</v>
-      </c>
-    </row>
+        <v>255</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="127" spans="1:3" ht="14.25" customHeight="1">
       <c r="A127" t="s">
-        <v>237</v>
-      </c>
-      <c r="B127" t="s">
-        <v>244</v>
-      </c>
-      <c r="C127" t="s">
-        <v>238</v>
+        <v>224</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="14.25" customHeight="1">
       <c r="A128" t="s">
+        <v>234</v>
+      </c>
+      <c r="B128" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A129" t="s">
+        <v>235</v>
+      </c>
+      <c r="B129" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A130" t="s">
+        <v>226</v>
+      </c>
+      <c r="B130" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A131" t="s">
+        <v>227</v>
+      </c>
+      <c r="B131" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A132" t="s">
+        <v>228</v>
+      </c>
+      <c r="B132" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A133" t="s">
+        <v>231</v>
+      </c>
+      <c r="B133" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A134" t="s">
+        <v>237</v>
+      </c>
+      <c r="B134" t="s">
+        <v>244</v>
+      </c>
+      <c r="C134" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A135" t="s">
         <v>239</v>
       </c>
-      <c r="B128" t="s">
+      <c r="B135" t="s">
         <v>243</v>
       </c>
-      <c r="C128" t="s">
+      <c r="C135" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="129" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A129" t="s">
+    <row r="136" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A136" t="s">
         <v>241</v>
       </c>
-      <c r="B129" t="s">
+      <c r="B136" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="130" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="131" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="132" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="133" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="134" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="135" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="136" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="137" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="138" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="139" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="140" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="141" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="142" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="143" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="144" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="137" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="138" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="139" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="140" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="141" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="142" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="143" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="144" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="145" ht="14.25" customHeight="1"/>
     <row r="146" ht="14.25" customHeight="1"/>
     <row r="147" ht="14.25" customHeight="1"/>
@@ -3938,6 +4032,13 @@
     <row r="767" ht="14.25" customHeight="1"/>
     <row r="768" ht="14.25" customHeight="1"/>
     <row r="769" ht="14.25" customHeight="1"/>
+    <row r="770" ht="14.25" customHeight="1"/>
+    <row r="771" ht="14.25" customHeight="1"/>
+    <row r="772" ht="14.25" customHeight="1"/>
+    <row r="773" ht="14.25" customHeight="1"/>
+    <row r="774" ht="14.25" customHeight="1"/>
+    <row r="775" ht="14.25" customHeight="1"/>
+    <row r="776" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
commit all fixes with relation to last TFR procesed
</commit_message>
<xml_diff>
--- a/STS IR Bot Performer/Data/Config.xlsx
+++ b/STS IR Bot Performer/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://taxwarellc-my.sharepoint.com/personal/nahuel_delacruz_sovos_com/Documents/Desktop/Nahuel/Projects/STS Internal Review bot/STS IR Bot Performer/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\martin.martinez\Documents\github-IRBot\STS_InternalReviewBot\STS IR Bot Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="124" documentId="13_ncr:1_{6168EBD1-1BEF-415E-8C0A-5B125435311F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{97A4B112-C99F-4ECC-B8FE-437F333941C3}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BCC80F2-0D7A-49A5-9796-A6CF90867F37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3465" yWindow="3465" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="261">
   <si>
     <t>Name</t>
   </si>
@@ -776,9 +776,6 @@
     <t>StateBalancing_LA_GrossSalesClickOnText</t>
   </si>
   <si>
-    <t>GROSS SALES OF TANGIBLE###Gross Sales of Tangible###Gross sales of tangible###Gross Sales of tangible</t>
-  </si>
-  <si>
     <t>StateBalancing_LA_RegexGetMonthlyCheckbox</t>
   </si>
   <si>
@@ -813,6 +810,15 @@
   </si>
   <si>
     <t>StateBalancing_LA_GrossSalesTab</t>
+  </si>
+  <si>
+    <t>RENTALS AND SERVICES AS REPORTED TO THE STATE OF LOUISIANA###and services as reported to the State of LA###SERVICES AS REPORTED TO THE STATE OF LOUISIANA###GROSS SALES OF TANGIBLE###Gross Sales of Tangible###Gross sales of tangible###Gross Sales of tangible###Gross sales of Tangible###GROSS SALES OF THE TANGIBLE</t>
+  </si>
+  <si>
+    <t>CheckTFR_ReturnName</t>
+  </si>
+  <si>
+    <t>WA Rev-40</t>
   </si>
 </sst>
 </file>
@@ -2324,10 +2330,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z776"/>
+  <dimension ref="A1:Z777"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="A119" sqref="A119"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2697,462 +2703,462 @@
         <v>180</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="44" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A44" t="s">
-        <v>63</v>
-      </c>
-      <c r="B44" t="s">
-        <v>64</v>
-      </c>
-    </row>
+    <row r="43" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A43" t="s">
+        <v>259</v>
+      </c>
+      <c r="B43" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="45" spans="1:3" ht="14.25" customHeight="1">
       <c r="A45" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B45" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="14.25" customHeight="1">
       <c r="A46" t="s">
-        <v>88</v>
+        <v>65</v>
       </c>
       <c r="B46" t="s">
-        <v>89</v>
+        <v>66</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="14.25" customHeight="1">
       <c r="A47" t="s">
-        <v>114</v>
+        <v>88</v>
       </c>
       <c r="B47" t="s">
-        <v>115</v>
+        <v>89</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="14.25" customHeight="1">
       <c r="A48" t="s">
-        <v>96</v>
+        <v>114</v>
       </c>
       <c r="B48" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="14.25" customHeight="1">
       <c r="A49" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B49" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="14.25" customHeight="1">
       <c r="A50" t="s">
+        <v>100</v>
+      </c>
+      <c r="B50" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A51" t="s">
         <v>186</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B51" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="52" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A52" t="s">
+    <row r="52" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="53" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A53" t="s">
         <v>102</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B53" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="54" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A54" t="s">
-        <v>103</v>
-      </c>
-      <c r="B54" t="s">
-        <v>104</v>
-      </c>
-    </row>
+    <row r="54" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="55" spans="1:3" ht="14.25" customHeight="1">
       <c r="A55" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B55" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="14.25" customHeight="1">
       <c r="A56" t="s">
+        <v>105</v>
+      </c>
+      <c r="B56" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A57" t="s">
         <v>107</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B57" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="58" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A58" t="s">
+    <row r="58" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="59" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A59" t="s">
         <v>109</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B59" t="s">
         <v>110</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C59" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="60" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A60" t="s">
-        <v>112</v>
-      </c>
-      <c r="B60" t="s">
-        <v>113</v>
-      </c>
-      <c r="C60" t="s">
-        <v>116</v>
-      </c>
-    </row>
+    <row r="60" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="61" spans="1:3" ht="14.25" customHeight="1">
       <c r="A61" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B61" t="s">
-        <v>118</v>
+        <v>113</v>
+      </c>
+      <c r="C61" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="14.25" customHeight="1">
       <c r="A62" t="s">
-        <v>119</v>
-      </c>
-      <c r="B62">
-        <v>1</v>
+        <v>117</v>
+      </c>
+      <c r="B62" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="14.25" customHeight="1">
       <c r="A63" t="s">
-        <v>120</v>
-      </c>
-      <c r="B63" t="s">
-        <v>121</v>
+        <v>119</v>
+      </c>
+      <c r="B63">
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="14.25" customHeight="1">
       <c r="A64" t="s">
-        <v>122</v>
-      </c>
-      <c r="B64">
-        <v>1</v>
+        <v>120</v>
+      </c>
+      <c r="B64" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="14.25" customHeight="1">
       <c r="A65" t="s">
-        <v>123</v>
-      </c>
-      <c r="B65" t="s">
-        <v>124</v>
+        <v>122</v>
+      </c>
+      <c r="B65">
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="14.25" customHeight="1">
       <c r="A66" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B66" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="14.25" customHeight="1">
       <c r="A67" t="s">
+        <v>125</v>
+      </c>
+      <c r="B67" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A68" t="s">
         <v>127</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B68" t="s">
         <v>128</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C68" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="69" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A69" t="s">
+    <row r="69" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="70" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A70" t="s">
         <v>130</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B70" t="s">
         <v>131</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C70" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="71" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A71" t="s">
-        <v>133</v>
-      </c>
-      <c r="B71" t="s">
-        <v>134</v>
-      </c>
-    </row>
+    <row r="71" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="72" spans="1:3" ht="14.25" customHeight="1">
       <c r="A72" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B72" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="14.25" customHeight="1">
       <c r="A73" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B73" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="14.25" customHeight="1">
       <c r="A74" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B74" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="14.25" customHeight="1">
       <c r="A75" t="s">
-        <v>141</v>
-      </c>
-      <c r="B75">
-        <v>1</v>
+        <v>139</v>
+      </c>
+      <c r="B75" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="14.25" customHeight="1">
       <c r="A76" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B76">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="14.25" customHeight="1">
       <c r="A77" t="s">
+        <v>142</v>
+      </c>
+      <c r="B77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A78" t="s">
         <v>143</v>
       </c>
-      <c r="B77">
+      <c r="B78">
         <v>2</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="79" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A79" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="B79" t="s">
-        <v>134</v>
-      </c>
-    </row>
+    <row r="79" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="80" spans="1:3" ht="14.25" customHeight="1">
       <c r="A80" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>205</v>
+        <v>144</v>
+      </c>
+      <c r="B80" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="14.25" customHeight="1">
       <c r="A81" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="B81" t="s">
-        <v>146</v>
+        <v>145</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="14.25" customHeight="1">
       <c r="A82" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>190</v>
+        <v>147</v>
+      </c>
+      <c r="B82" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="14.25" customHeight="1">
       <c r="A83" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="14.25" customHeight="1">
       <c r="A84" s="2" t="s">
-        <v>148</v>
+        <v>191</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>149</v>
+        <v>192</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="14.25" customHeight="1">
       <c r="A85" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="B85" t="s">
-        <v>151</v>
+        <v>148</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="14.25" customHeight="1">
       <c r="A86" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B86" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="14.25" customHeight="1">
       <c r="A87" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B87" t="s">
-        <v>140</v>
+        <v>152</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="14.25" customHeight="1">
       <c r="A88" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="B88">
-        <v>1</v>
+        <v>154</v>
+      </c>
+      <c r="B88" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="14.25" customHeight="1">
       <c r="A89" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B89">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="14.25" customHeight="1">
       <c r="A90" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A91" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="B90">
+      <c r="B91">
         <v>1</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A91" t="s">
-        <v>158</v>
-      </c>
-      <c r="B91">
-        <v>35</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="14.25" customHeight="1">
       <c r="A92" t="s">
-        <v>160</v>
-      </c>
-      <c r="B92" t="s">
-        <v>159</v>
+        <v>158</v>
+      </c>
+      <c r="B92">
+        <v>35</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="14.25" customHeight="1">
       <c r="A93" t="s">
+        <v>160</v>
+      </c>
+      <c r="B93" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A94" t="s">
         <v>162</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B94" t="s">
         <v>161</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A94" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="B94" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="14.25" customHeight="1">
       <c r="A95" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>196</v>
+        <v>193</v>
+      </c>
+      <c r="B95" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="14.25" customHeight="1">
       <c r="A96" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="14.25" customHeight="1">
       <c r="A97" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="14.25" customHeight="1">
       <c r="A98" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="14.25" customHeight="1">
       <c r="A99" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A100" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="B99" s="2" t="s">
+      <c r="B100" s="2" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="100" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="101" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A101" t="s">
-        <v>163</v>
-      </c>
-      <c r="B101" t="s">
-        <v>222</v>
-      </c>
-    </row>
+    <row r="101" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="102" spans="1:3" ht="14.25" customHeight="1">
       <c r="A102" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B102" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="14.25" customHeight="1">
       <c r="A103" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B103" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="14.25" customHeight="1">
       <c r="A104" t="s">
-        <v>183</v>
-      </c>
-      <c r="B104">
-        <v>6</v>
+        <v>165</v>
+      </c>
+      <c r="B104" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="14.25" customHeight="1">
       <c r="A105" t="s">
-        <v>223</v>
-      </c>
-      <c r="B105" t="s">
-        <v>128</v>
+        <v>183</v>
+      </c>
+      <c r="B105">
+        <v>6</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="14.25" customHeight="1">
       <c r="A106" t="s">
-        <v>166</v>
+        <v>223</v>
       </c>
       <c r="B106" t="s">
         <v>128</v>
@@ -3160,140 +3166,140 @@
     </row>
     <row r="107" spans="1:3" ht="14.25" customHeight="1">
       <c r="A107" t="s">
-        <v>167</v>
-      </c>
-      <c r="B107">
-        <v>2</v>
+        <v>166</v>
+      </c>
+      <c r="B107" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="14.25" customHeight="1">
       <c r="A108" t="s">
-        <v>168</v>
-      </c>
-      <c r="B108" t="s">
-        <v>169</v>
+        <v>167</v>
+      </c>
+      <c r="B108">
+        <v>2</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="14.25" customHeight="1">
       <c r="A109" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B109" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="14.25" customHeight="1">
       <c r="A110" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B110" t="s">
-        <v>173</v>
-      </c>
-      <c r="C110" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="14.25" customHeight="1">
       <c r="A111" t="s">
+        <v>172</v>
+      </c>
+      <c r="B111" t="s">
+        <v>173</v>
+      </c>
+      <c r="C111" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A112" t="s">
         <v>175</v>
       </c>
-      <c r="B111" t="s">
+      <c r="B112" t="s">
         <v>176</v>
       </c>
-      <c r="C111" t="s">
+      <c r="C112" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="112" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="113" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A113" t="s">
-        <v>207</v>
-      </c>
-      <c r="B113" t="s">
-        <v>104</v>
-      </c>
-    </row>
+    <row r="113" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="114" spans="1:3" ht="14.25" customHeight="1">
       <c r="A114" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B114" t="s">
-        <v>209</v>
+        <v>104</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="14.25" customHeight="1">
       <c r="A115" t="s">
-        <v>210</v>
-      </c>
-      <c r="B115">
-        <v>1</v>
+        <v>208</v>
+      </c>
+      <c r="B115" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="14.25" customHeight="1">
       <c r="A116" t="s">
-        <v>211</v>
-      </c>
-      <c r="B116" t="s">
-        <v>212</v>
+        <v>210</v>
+      </c>
+      <c r="B116">
+        <v>1</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="14.25" customHeight="1">
       <c r="A117" t="s">
-        <v>213</v>
-      </c>
-      <c r="B117">
-        <v>1</v>
+        <v>211</v>
+      </c>
+      <c r="B117" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="14.25" customHeight="1">
       <c r="A118" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B118">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="14.25" customHeight="1">
       <c r="A119" t="s">
-        <v>258</v>
+        <v>214</v>
       </c>
       <c r="B119">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="14.25" customHeight="1">
       <c r="A120" t="s">
-        <v>245</v>
-      </c>
-      <c r="B120" t="s">
-        <v>246</v>
-      </c>
-      <c r="C120" t="s">
         <v>257</v>
+      </c>
+      <c r="B120">
+        <v>1</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="14.25" customHeight="1">
       <c r="A121" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B121" t="s">
-        <v>248</v>
+        <v>258</v>
+      </c>
+      <c r="C121" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="14.25" customHeight="1">
       <c r="A122" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B122" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="123" spans="1:3" ht="14.25" customHeight="1">
       <c r="A123" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="B123" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="124" spans="1:3" ht="14.25" customHeight="1">
@@ -3301,105 +3307,112 @@
         <v>251</v>
       </c>
       <c r="B124" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="14.25" customHeight="1">
       <c r="A125" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="B125" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="126" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="127" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A127" t="s">
-        <v>224</v>
-      </c>
-      <c r="B127" s="2" t="s">
-        <v>225</v>
-      </c>
-    </row>
+    <row r="126" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A126" t="s">
+        <v>253</v>
+      </c>
+      <c r="B126" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="128" spans="1:3" ht="14.25" customHeight="1">
       <c r="A128" t="s">
-        <v>234</v>
-      </c>
-      <c r="B128" t="s">
-        <v>134</v>
+        <v>224</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="129" spans="1:3" ht="14.25" customHeight="1">
       <c r="A129" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B129" t="s">
-        <v>236</v>
+        <v>134</v>
       </c>
     </row>
     <row r="130" spans="1:3" ht="14.25" customHeight="1">
       <c r="A130" t="s">
-        <v>226</v>
+        <v>235</v>
       </c>
       <c r="B130" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
     </row>
     <row r="131" spans="1:3" ht="14.25" customHeight="1">
       <c r="A131" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B131" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="132" spans="1:3" ht="14.25" customHeight="1">
       <c r="A132" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B132" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="133" spans="1:3" ht="14.25" customHeight="1">
       <c r="A133" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B133" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="134" spans="1:3" ht="14.25" customHeight="1">
       <c r="A134" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="B134" t="s">
-        <v>244</v>
-      </c>
-      <c r="C134" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
     </row>
     <row r="135" spans="1:3" ht="14.25" customHeight="1">
       <c r="A135" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B135" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C135" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="136" spans="1:3" ht="14.25" customHeight="1">
       <c r="A136" t="s">
+        <v>239</v>
+      </c>
+      <c r="B136" t="s">
+        <v>243</v>
+      </c>
+      <c r="C136" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A137" t="s">
         <v>241</v>
       </c>
-      <c r="B136" t="s">
+      <c r="B137" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="137" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="138" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="139" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="140" spans="1:3" ht="14.25" customHeight="1"/>
@@ -4039,6 +4052,7 @@
     <row r="774" ht="14.25" customHeight="1"/>
     <row r="775" ht="14.25" customHeight="1"/>
     <row r="776" ht="14.25" customHeight="1"/>
+    <row r="777" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add multiple customer clients and fixes in relation to the last run of the bot
</commit_message>
<xml_diff>
--- a/STS IR Bot Performer/Data/Config.xlsx
+++ b/STS IR Bot Performer/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\martin.martinez\Documents\github-IRBot\STS_InternalReviewBot\STS IR Bot Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BCC80F2-0D7A-49A5-9796-A6CF90867F37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAC2D448-160F-46A2-83E6-D962A142AE78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="263">
   <si>
     <t>Name</t>
   </si>
@@ -581,9 +581,6 @@
     <t>Credit Held</t>
   </si>
   <si>
-    <t>P:\TaxReturnOutSourcing\Preparer\UIPathPublish\IR Bot Temp Files\pdfTemp &lt;USERNAME&gt;.pdf</t>
-  </si>
-  <si>
     <t>C:\Users\&lt;USERNAME&gt;\Documents\UiPath\temp</t>
   </si>
   <si>
@@ -614,9 +611,6 @@
     <t>StateBalancing_CO_PathCOToolCopy</t>
   </si>
   <si>
-    <t>Data\Output\CO DR-0100 XML tool.xlsm</t>
-  </si>
-  <si>
     <t>StateBalancing_CO_firstSheetCOTool</t>
   </si>
   <si>
@@ -728,97 +722,109 @@
     <t>detail</t>
   </si>
   <si>
+    <t>StateBalancing_SC_Tool_MainWorksheet</t>
+  </si>
+  <si>
+    <t>SC ST-389</t>
+  </si>
+  <si>
+    <t>SC ST-389 tool</t>
+  </si>
+  <si>
+    <t>StateBalancing_SC_DetailPageName</t>
+  </si>
+  <si>
+    <t>StateBalancing_SC_LocalTaxesPageName</t>
+  </si>
+  <si>
+    <t>Local Taxes</t>
+  </si>
+  <si>
+    <t>StateBalancing_SC_CountyList</t>
+  </si>
+  <si>
+    <t>The list of all county names that can appear in TaxSolver - LocalTaxes tab</t>
+  </si>
+  <si>
+    <t>StateBalancing_SC_GetLocalTaxesCounty</t>
+  </si>
+  <si>
+    <t>Regex to get county of each local tax in Taxsolver</t>
+  </si>
+  <si>
+    <t>StateBalancing_SC_Tool_StartCell</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>(&lt;COUNTY_LIST&gt;)\s+[\d\.\,]+\s+[\d\.\,]+</t>
+  </si>
+  <si>
+    <t>AIKEN|ALLENDALE|ANDERSON|BAMBERG|BARNWELL|BERKELEY|CALHOUN|CHARLESTON|CHEROKEE|CHESTER|CHESTERFIELD|CLARENDON|COLLETON|DARLINGTON|DILLON|EDGEFIELD|FLORENCE|GREENWOOD|HORRY|JASPER|KERSHAW|LANCASTER|LAURENS|LEE|LEXINGTON|MARION|MARLBORO|MCCORMICK|NEWBERRY|ORANGEBURG|RICHLAND|SALUDA|SPARTANBURG|SUMTER|WILLIAMSBURG|YORK</t>
+  </si>
+  <si>
+    <t>StateBalancing_LA_GrossSalesClickOnText</t>
+  </si>
+  <si>
+    <t>StateBalancing_LA_RegexGetMonthlyCheckbox</t>
+  </si>
+  <si>
+    <t>(?&lt;=\n.*)\w+(?=.*Monthly)</t>
+  </si>
+  <si>
+    <t>StateBalancing_LA_ListNonLocalStates</t>
+  </si>
+  <si>
+    <t>LA R-1029,LA R-1029E,LA R-1031</t>
+  </si>
+  <si>
+    <t>StateBalancing_LA_TableColumns</t>
+  </si>
+  <si>
+    <t>StateBalancing_LA_TemporalCsvFile</t>
+  </si>
+  <si>
+    <t>Data\TemporalFileLAStateBalancing.csv</t>
+  </si>
+  <si>
+    <t>StateBalancing_LA_ExceptionMessageQuarterlyReturn</t>
+  </si>
+  <si>
+    <t>This return is Quarterly. Gross Sales are:</t>
+  </si>
+  <si>
+    <t>ReturnType,FilingType,LegalEntity,ReturnName,CustomerName,GrossSales</t>
+  </si>
+  <si>
+    <t>For LA State Balancing 2nd version</t>
+  </si>
+  <si>
+    <t>StateBalancing_LA_GrossSalesTab</t>
+  </si>
+  <si>
+    <t>CheckTFR_ReturnName</t>
+  </si>
+  <si>
+    <t>WA Rev-40</t>
+  </si>
+  <si>
+    <t>P:\TaxReturnOutSourcing\Preparer\UIPathPublish\IR Bot Temp Files\pdfTemp &lt;USERNAME&gt; &lt;CUSTOMER&gt;.pdf</t>
+  </si>
+  <si>
+    <t>Data\Output\CO DR-0100 XML tool &lt;CUSTOMER&gt;.xlsm</t>
+  </si>
+  <si>
     <t>Data\Input\SC ST 389 tool.xlsx</t>
   </si>
   <si>
-    <t>StateBalancing_SC_Tool_MainWorksheet</t>
-  </si>
-  <si>
-    <t>SC ST-389</t>
-  </si>
-  <si>
-    <t>SC ST-389 tool</t>
-  </si>
-  <si>
-    <t>StateBalancing_SC_DetailPageName</t>
-  </si>
-  <si>
-    <t>StateBalancing_SC_LocalTaxesPageName</t>
-  </si>
-  <si>
-    <t>Local Taxes</t>
-  </si>
-  <si>
-    <t>StateBalancing_SC_CountyList</t>
-  </si>
-  <si>
-    <t>The list of all county names that can appear in TaxSolver - LocalTaxes tab</t>
-  </si>
-  <si>
-    <t>StateBalancing_SC_GetLocalTaxesCounty</t>
-  </si>
-  <si>
-    <t>Regex to get county of each local tax in Taxsolver</t>
-  </si>
-  <si>
-    <t>StateBalancing_SC_Tool_StartCell</t>
-  </si>
-  <si>
-    <t>F1</t>
-  </si>
-  <si>
-    <t>(&lt;COUNTY_LIST&gt;)\s+[\d\.\,]+\s+[\d\.\,]+</t>
-  </si>
-  <si>
-    <t>AIKEN|ALLENDALE|ANDERSON|BAMBERG|BARNWELL|BERKELEY|CALHOUN|CHARLESTON|CHEROKEE|CHESTER|CHESTERFIELD|CLARENDON|COLLETON|DARLINGTON|DILLON|EDGEFIELD|FLORENCE|GREENWOOD|HORRY|JASPER|KERSHAW|LANCASTER|LAURENS|LEE|LEXINGTON|MARION|MARLBORO|MCCORMICK|NEWBERRY|ORANGEBURG|RICHLAND|SALUDA|SPARTANBURG|SUMTER|WILLIAMSBURG|YORK</t>
-  </si>
-  <si>
-    <t>StateBalancing_LA_GrossSalesClickOnText</t>
-  </si>
-  <si>
-    <t>StateBalancing_LA_RegexGetMonthlyCheckbox</t>
-  </si>
-  <si>
-    <t>(?&lt;=\n.*)\w+(?=.*Monthly)</t>
-  </si>
-  <si>
-    <t>StateBalancing_LA_ListNonLocalStates</t>
-  </si>
-  <si>
-    <t>LA R-1029,LA R-1029E,LA R-1031</t>
-  </si>
-  <si>
-    <t>StateBalancing_LA_TableColumns</t>
-  </si>
-  <si>
-    <t>StateBalancing_LA_TemporalCsvFile</t>
-  </si>
-  <si>
-    <t>Data\TemporalFileLAStateBalancing.csv</t>
-  </si>
-  <si>
-    <t>StateBalancing_LA_ExceptionMessageQuarterlyReturn</t>
-  </si>
-  <si>
-    <t>This return is Quarterly. Gross Sales are:</t>
-  </si>
-  <si>
-    <t>ReturnType,FilingType,LegalEntity,ReturnName,CustomerName,GrossSales</t>
-  </si>
-  <si>
-    <t>For LA State Balancing 2nd version</t>
-  </si>
-  <si>
-    <t>StateBalancing_LA_GrossSalesTab</t>
+    <t>StateBalancing_SC_PathToolDestination</t>
+  </si>
+  <si>
+    <t>Data\Output\SC ST 389 tool &lt;CUSTOMER&gt;.xlsx</t>
   </si>
   <si>
     <t>RENTALS AND SERVICES AS REPORTED TO THE STATE OF LOUISIANA###and services as reported to the State of LA###SERVICES AS REPORTED TO THE STATE OF LOUISIANA###GROSS SALES OF TANGIBLE###Gross Sales of Tangible###Gross sales of tangible###Gross Sales of tangible###Gross sales of Tangible###GROSS SALES OF THE TANGIBLE</t>
-  </si>
-  <si>
-    <t>CheckTFR_ReturnName</t>
-  </si>
-  <si>
-    <t>WA Rev-40</t>
   </si>
 </sst>
 </file>
@@ -2330,10 +2336,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z777"/>
+  <dimension ref="A1:Z778"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
+      <selection activeCell="B121" sqref="B121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2505,13 +2511,13 @@
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" spans="1:3" s="5" customFormat="1" ht="14.25" customHeight="1">
       <c r="A17" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>215</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="18" spans="1:3" s="6" customFormat="1" ht="14.25" customHeight="1">
@@ -2519,7 +2525,7 @@
         <v>62</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="19" spans="1:3" s="5" customFormat="1" ht="14.25" customHeight="1">
@@ -2527,7 +2533,7 @@
         <v>67</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>68</v>
@@ -2562,7 +2568,7 @@
         <v>91</v>
       </c>
       <c r="B23" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C23" t="s">
         <v>92</v>
@@ -2573,7 +2579,7 @@
         <v>98</v>
       </c>
       <c r="B24" t="s">
-        <v>181</v>
+        <v>257</v>
       </c>
       <c r="C24" t="s">
         <v>99</v>
@@ -2684,15 +2690,15 @@
         <v>178</v>
       </c>
       <c r="B40" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="14.25" customHeight="1">
       <c r="A41" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B41" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="14.25" customHeight="1">
@@ -2705,10 +2711,10 @@
     </row>
     <row r="43" spans="1:3" ht="14.25" customHeight="1">
       <c r="A43" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="B43" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2762,10 +2768,10 @@
     </row>
     <row r="51" spans="1:3" ht="14.25" customHeight="1">
       <c r="A51" t="s">
+        <v>185</v>
+      </c>
+      <c r="B51" t="s">
         <v>186</v>
-      </c>
-      <c r="B51" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2774,7 +2780,7 @@
         <v>102</v>
       </c>
       <c r="B53" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2968,7 +2974,7 @@
         <v>145</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="14.25" customHeight="1">
@@ -2981,18 +2987,18 @@
     </row>
     <row r="83" spans="1:2" ht="14.25" customHeight="1">
       <c r="A83" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B83" s="2" t="s">
         <v>189</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="14.25" customHeight="1">
       <c r="A84" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>192</v>
+        <v>258</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="14.25" customHeight="1">
@@ -3077,50 +3083,50 @@
     </row>
     <row r="95" spans="1:2" ht="14.25" customHeight="1">
       <c r="A95" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B95" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="14.25" customHeight="1">
       <c r="A96" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="14.25" customHeight="1">
       <c r="A97" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="14.25" customHeight="1">
       <c r="A98" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="14.25" customHeight="1">
       <c r="A99" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="14.25" customHeight="1">
       <c r="A100" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="14.25" customHeight="1"/>
@@ -3129,7 +3135,7 @@
         <v>163</v>
       </c>
       <c r="B102" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="14.25" customHeight="1">
@@ -3137,7 +3143,7 @@
         <v>164</v>
       </c>
       <c r="B103" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="14.25" customHeight="1">
@@ -3145,12 +3151,12 @@
         <v>165</v>
       </c>
       <c r="B104" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="14.25" customHeight="1">
       <c r="A105" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B105">
         <v>6</v>
@@ -3158,7 +3164,7 @@
     </row>
     <row r="106" spans="1:3" ht="14.25" customHeight="1">
       <c r="A106" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B106" t="s">
         <v>128</v>
@@ -3221,7 +3227,7 @@
     <row r="113" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="114" spans="1:3" ht="14.25" customHeight="1">
       <c r="A114" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B114" t="s">
         <v>104</v>
@@ -3229,15 +3235,15 @@
     </row>
     <row r="115" spans="1:3" ht="14.25" customHeight="1">
       <c r="A115" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B115" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="14.25" customHeight="1">
       <c r="A116" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B116">
         <v>1</v>
@@ -3245,15 +3251,15 @@
     </row>
     <row r="117" spans="1:3" ht="14.25" customHeight="1">
       <c r="A117" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B117" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="14.25" customHeight="1">
       <c r="A118" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B118">
         <v>1</v>
@@ -3261,7 +3267,7 @@
     </row>
     <row r="119" spans="1:3" ht="14.25" customHeight="1">
       <c r="A119" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B119">
         <v>0</v>
@@ -3269,7 +3275,7 @@
     </row>
     <row r="120" spans="1:3" ht="14.25" customHeight="1">
       <c r="A120" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B120">
         <v>1</v>
@@ -3277,67 +3283,67 @@
     </row>
     <row r="121" spans="1:3" ht="14.25" customHeight="1">
       <c r="A121" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B121" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="C121" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="14.25" customHeight="1">
       <c r="A122" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B122" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="123" spans="1:3" ht="14.25" customHeight="1">
       <c r="A123" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B123" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="124" spans="1:3" ht="14.25" customHeight="1">
       <c r="A124" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B124" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="14.25" customHeight="1">
       <c r="A125" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B125" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="14.25" customHeight="1">
       <c r="A126" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B126" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="128" spans="1:3" ht="14.25" customHeight="1">
       <c r="A128" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="129" spans="1:3" ht="14.25" customHeight="1">
       <c r="A129" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B129" t="s">
         <v>134</v>
@@ -3345,75 +3351,82 @@
     </row>
     <row r="130" spans="1:3" ht="14.25" customHeight="1">
       <c r="A130" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B130" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="131" spans="1:3" ht="14.25" customHeight="1">
       <c r="A131" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B131" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="132" spans="1:3" ht="14.25" customHeight="1">
       <c r="A132" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B132" t="s">
-        <v>230</v>
+        <v>259</v>
       </c>
     </row>
     <row r="133" spans="1:3" ht="14.25" customHeight="1">
       <c r="A133" t="s">
-        <v>228</v>
+        <v>260</v>
       </c>
       <c r="B133" t="s">
-        <v>229</v>
+        <v>261</v>
       </c>
     </row>
     <row r="134" spans="1:3" ht="14.25" customHeight="1">
       <c r="A134" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="B134" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
     </row>
     <row r="135" spans="1:3" ht="14.25" customHeight="1">
       <c r="A135" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="B135" t="s">
-        <v>244</v>
-      </c>
-      <c r="C135" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
     </row>
     <row r="136" spans="1:3" ht="14.25" customHeight="1">
       <c r="A136" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="B136" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C136" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
     </row>
     <row r="137" spans="1:3" ht="14.25" customHeight="1">
       <c r="A137" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="B137" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3" ht="14.25" customHeight="1"/>
+        <v>240</v>
+      </c>
+      <c r="C137" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A138" t="s">
+        <v>238</v>
+      </c>
+      <c r="B138" t="s">
+        <v>239</v>
+      </c>
+    </row>
     <row r="139" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="140" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="141" spans="1:3" ht="14.25" customHeight="1"/>
@@ -4053,6 +4066,7 @@
     <row r="775" ht="14.25" customHeight="1"/>
     <row r="776" ht="14.25" customHeight="1"/>
     <row r="777" ht="14.25" customHeight="1"/>
+    <row r="778" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add new path that work for specific users
</commit_message>
<xml_diff>
--- a/STS IR Bot Performer/Data/Config.xlsx
+++ b/STS IR Bot Performer/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\martin.martinez\Documents\github-IRBot\STS_InternalReviewBot\STS IR Bot Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAC2D448-160F-46A2-83E6-D962A142AE78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E05DAEBC-21DF-484D-A01E-226AC53437E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="265">
   <si>
     <t>Name</t>
   </si>
@@ -825,6 +825,12 @@
   </si>
   <si>
     <t>RENTALS AND SERVICES AS REPORTED TO THE STATE OF LOUISIANA###and services as reported to the State of LA###SERVICES AS REPORTED TO THE STATE OF LOUISIANA###GROSS SALES OF TANGIBLE###Gross Sales of Tangible###Gross sales of tangible###Gross Sales of tangible###Gross sales of Tangible###GROSS SALES OF THE TANGIBLE</t>
+  </si>
+  <si>
+    <t>\\10.250.52.158\Depts\TaxReturnOutSourcing\Preparer\UIPathPublish\IR Bot Temp Files\InputFiles</t>
+  </si>
+  <si>
+    <t>PathDifferentPDriveFolder</t>
   </si>
 </sst>
 </file>
@@ -2336,10 +2342,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z778"/>
+  <dimension ref="A1:Z779"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
-      <selection activeCell="B121" sqref="B121"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2528,651 +2534,654 @@
         <v>216</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="5" customFormat="1" ht="14.25" customHeight="1">
+    <row r="19" spans="1:3" s="6" customFormat="1" ht="14.25" customHeight="1">
       <c r="A19" s="5" t="s">
-        <v>67</v>
+        <v>264</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>217</v>
+        <v>263</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A20" t="s">
+    <row r="20" spans="1:3" s="5" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A20" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A21" t="s">
         <v>85</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>90</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" s="6" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A21" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="22" spans="1:3" s="6" customFormat="1" ht="14.25" customHeight="1">
       <c r="A22" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" s="6" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A23" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B23" s="6" t="s">
         <v>81</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A23" t="s">
-        <v>91</v>
-      </c>
-      <c r="B23" t="s">
-        <v>181</v>
-      </c>
-      <c r="C23" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" t="s">
+        <v>91</v>
+      </c>
+      <c r="B24" t="s">
+        <v>181</v>
+      </c>
+      <c r="C24" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A25" t="s">
         <v>98</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
         <v>257</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C25" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="26" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A26" t="s">
-        <v>82</v>
-      </c>
-      <c r="B26" t="s">
-        <v>83</v>
-      </c>
-      <c r="C26" t="s">
-        <v>84</v>
-      </c>
-    </row>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
       <c r="A27" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B27" t="s">
-        <v>87</v>
+        <v>83</v>
+      </c>
+      <c r="C27" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1">
       <c r="A28" t="s">
+        <v>86</v>
+      </c>
+      <c r="B28" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A29" t="s">
         <v>93</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" t="s">
         <v>94</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C29" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="30" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A30" t="s">
+    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A31" t="s">
         <v>69</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B31" t="s">
         <v>70</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C31" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="32" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A32" t="s">
-        <v>72</v>
-      </c>
-      <c r="B32" t="s">
-        <v>73</v>
-      </c>
-    </row>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="33" spans="1:3" ht="14.25" customHeight="1">
       <c r="A33" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B33" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="14.25" customHeight="1">
       <c r="A34" t="s">
+        <v>74</v>
+      </c>
+      <c r="B34" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A35" t="s">
         <v>75</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B35" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="36" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A36" t="s">
-        <v>54</v>
-      </c>
-      <c r="B36" t="s">
-        <v>55</v>
-      </c>
-    </row>
+    <row r="36" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="37" spans="1:3" ht="14.25" customHeight="1">
       <c r="A37" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B37" t="s">
-        <v>57</v>
-      </c>
-      <c r="C37" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="14.25" customHeight="1">
       <c r="A38" t="s">
+        <v>56</v>
+      </c>
+      <c r="B38" t="s">
+        <v>57</v>
+      </c>
+      <c r="C38" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A39" t="s">
         <v>59</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
         <v>60</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C39" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="40" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A40" t="s">
-        <v>178</v>
-      </c>
-      <c r="B40" t="s">
-        <v>184</v>
-      </c>
-    </row>
+    <row r="40" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="41" spans="1:3" ht="14.25" customHeight="1">
       <c r="A41" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="B41" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="14.25" customHeight="1">
       <c r="A42" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="B42" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="14.25" customHeight="1">
       <c r="A43" t="s">
+        <v>179</v>
+      </c>
+      <c r="B43" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A44" t="s">
         <v>255</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B44" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="45" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A45" t="s">
-        <v>63</v>
-      </c>
-      <c r="B45" t="s">
-        <v>64</v>
-      </c>
-    </row>
+    <row r="45" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="46" spans="1:3" ht="14.25" customHeight="1">
       <c r="A46" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B46" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="14.25" customHeight="1">
       <c r="A47" t="s">
-        <v>88</v>
+        <v>65</v>
       </c>
       <c r="B47" t="s">
-        <v>89</v>
+        <v>66</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="14.25" customHeight="1">
       <c r="A48" t="s">
-        <v>114</v>
+        <v>88</v>
       </c>
       <c r="B48" t="s">
-        <v>115</v>
+        <v>89</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="14.25" customHeight="1">
       <c r="A49" t="s">
-        <v>96</v>
+        <v>114</v>
       </c>
       <c r="B49" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="14.25" customHeight="1">
       <c r="A50" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B50" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="14.25" customHeight="1">
       <c r="A51" t="s">
+        <v>100</v>
+      </c>
+      <c r="B51" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A52" t="s">
         <v>185</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B52" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="53" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A53" t="s">
+    <row r="53" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="54" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A54" t="s">
         <v>102</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B54" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="55" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A55" t="s">
-        <v>103</v>
-      </c>
-      <c r="B55" t="s">
-        <v>104</v>
-      </c>
-    </row>
+    <row r="55" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="56" spans="1:3" ht="14.25" customHeight="1">
       <c r="A56" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B56" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="14.25" customHeight="1">
       <c r="A57" t="s">
+        <v>105</v>
+      </c>
+      <c r="B57" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A58" t="s">
         <v>107</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B58" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="59" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A59" t="s">
+    <row r="59" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="60" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A60" t="s">
         <v>109</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B60" t="s">
         <v>110</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C60" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="61" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A61" t="s">
-        <v>112</v>
-      </c>
-      <c r="B61" t="s">
-        <v>113</v>
-      </c>
-      <c r="C61" t="s">
-        <v>116</v>
-      </c>
-    </row>
+    <row r="61" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="62" spans="1:3" ht="14.25" customHeight="1">
       <c r="A62" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B62" t="s">
-        <v>118</v>
+        <v>113</v>
+      </c>
+      <c r="C62" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="14.25" customHeight="1">
       <c r="A63" t="s">
-        <v>119</v>
-      </c>
-      <c r="B63">
-        <v>1</v>
+        <v>117</v>
+      </c>
+      <c r="B63" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="14.25" customHeight="1">
       <c r="A64" t="s">
-        <v>120</v>
-      </c>
-      <c r="B64" t="s">
-        <v>121</v>
+        <v>119</v>
+      </c>
+      <c r="B64">
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="14.25" customHeight="1">
       <c r="A65" t="s">
-        <v>122</v>
-      </c>
-      <c r="B65">
-        <v>1</v>
+        <v>120</v>
+      </c>
+      <c r="B65" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="14.25" customHeight="1">
       <c r="A66" t="s">
-        <v>123</v>
-      </c>
-      <c r="B66" t="s">
-        <v>124</v>
+        <v>122</v>
+      </c>
+      <c r="B66">
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="14.25" customHeight="1">
       <c r="A67" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B67" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="14.25" customHeight="1">
       <c r="A68" t="s">
+        <v>125</v>
+      </c>
+      <c r="B68" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A69" t="s">
         <v>127</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B69" t="s">
         <v>128</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C69" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="70" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A70" t="s">
+    <row r="70" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="71" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A71" t="s">
         <v>130</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B71" t="s">
         <v>131</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C71" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="72" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A72" t="s">
-        <v>133</v>
-      </c>
-      <c r="B72" t="s">
-        <v>134</v>
-      </c>
-    </row>
+    <row r="72" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="73" spans="1:3" ht="14.25" customHeight="1">
       <c r="A73" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B73" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="14.25" customHeight="1">
       <c r="A74" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B74" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="14.25" customHeight="1">
       <c r="A75" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B75" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="14.25" customHeight="1">
       <c r="A76" t="s">
-        <v>141</v>
-      </c>
-      <c r="B76">
-        <v>1</v>
+        <v>139</v>
+      </c>
+      <c r="B76" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="14.25" customHeight="1">
       <c r="A77" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B77">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="14.25" customHeight="1">
       <c r="A78" t="s">
+        <v>142</v>
+      </c>
+      <c r="B78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A79" t="s">
         <v>143</v>
       </c>
-      <c r="B78">
+      <c r="B79">
         <v>2</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="80" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A80" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="B80" t="s">
-        <v>134</v>
-      </c>
-    </row>
+    <row r="80" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="81" spans="1:2" ht="14.25" customHeight="1">
       <c r="A81" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>203</v>
+        <v>144</v>
+      </c>
+      <c r="B81" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="14.25" customHeight="1">
       <c r="A82" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="B82" t="s">
-        <v>146</v>
+        <v>145</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="14.25" customHeight="1">
       <c r="A83" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>189</v>
+        <v>147</v>
+      </c>
+      <c r="B83" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="14.25" customHeight="1">
       <c r="A84" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>258</v>
+        <v>189</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="14.25" customHeight="1">
       <c r="A85" s="2" t="s">
-        <v>148</v>
+        <v>190</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>149</v>
+        <v>258</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="14.25" customHeight="1">
       <c r="A86" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="B86" t="s">
-        <v>151</v>
+        <v>148</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="14.25" customHeight="1">
       <c r="A87" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B87" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="14.25" customHeight="1">
       <c r="A88" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B88" t="s">
-        <v>140</v>
+        <v>152</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="14.25" customHeight="1">
       <c r="A89" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="B89">
-        <v>1</v>
+        <v>154</v>
+      </c>
+      <c r="B89" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="14.25" customHeight="1">
       <c r="A90" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B90">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="14.25" customHeight="1">
       <c r="A91" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A92" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="B91">
+      <c r="B92">
         <v>1</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A92" t="s">
-        <v>158</v>
-      </c>
-      <c r="B92">
-        <v>35</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="14.25" customHeight="1">
       <c r="A93" t="s">
-        <v>160</v>
-      </c>
-      <c r="B93" t="s">
-        <v>159</v>
+        <v>158</v>
+      </c>
+      <c r="B93">
+        <v>35</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="14.25" customHeight="1">
       <c r="A94" t="s">
+        <v>160</v>
+      </c>
+      <c r="B94" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A95" t="s">
         <v>162</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B95" t="s">
         <v>161</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A95" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="B95" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="14.25" customHeight="1">
       <c r="A96" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="B96" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
+      </c>
+      <c r="B96" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="14.25" customHeight="1">
       <c r="A97" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="14.25" customHeight="1">
       <c r="A98" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="14.25" customHeight="1">
       <c r="A99" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="14.25" customHeight="1">
       <c r="A100" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A101" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="B100" s="2" t="s">
+      <c r="B101" s="2" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="101" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="102" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A102" t="s">
-        <v>163</v>
-      </c>
-      <c r="B102" t="s">
-        <v>220</v>
-      </c>
-    </row>
+    <row r="102" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="103" spans="1:3" ht="14.25" customHeight="1">
       <c r="A103" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B103" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="14.25" customHeight="1">
       <c r="A104" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B104" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="14.25" customHeight="1">
       <c r="A105" t="s">
-        <v>182</v>
-      </c>
-      <c r="B105">
-        <v>6</v>
+        <v>165</v>
+      </c>
+      <c r="B105" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="14.25" customHeight="1">
       <c r="A106" t="s">
-        <v>221</v>
-      </c>
-      <c r="B106" t="s">
-        <v>128</v>
+        <v>182</v>
+      </c>
+      <c r="B106">
+        <v>6</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="14.25" customHeight="1">
       <c r="A107" t="s">
-        <v>166</v>
+        <v>221</v>
       </c>
       <c r="B107" t="s">
         <v>128</v>
@@ -3180,254 +3189,261 @@
     </row>
     <row r="108" spans="1:3" ht="14.25" customHeight="1">
       <c r="A108" t="s">
-        <v>167</v>
-      </c>
-      <c r="B108">
-        <v>2</v>
+        <v>166</v>
+      </c>
+      <c r="B108" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="14.25" customHeight="1">
       <c r="A109" t="s">
-        <v>168</v>
-      </c>
-      <c r="B109" t="s">
-        <v>169</v>
+        <v>167</v>
+      </c>
+      <c r="B109">
+        <v>2</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="14.25" customHeight="1">
       <c r="A110" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B110" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="14.25" customHeight="1">
       <c r="A111" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B111" t="s">
-        <v>173</v>
-      </c>
-      <c r="C111" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="14.25" customHeight="1">
       <c r="A112" t="s">
+        <v>172</v>
+      </c>
+      <c r="B112" t="s">
+        <v>173</v>
+      </c>
+      <c r="C112" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A113" t="s">
         <v>175</v>
       </c>
-      <c r="B112" t="s">
+      <c r="B113" t="s">
         <v>176</v>
       </c>
-      <c r="C112" t="s">
+      <c r="C113" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="113" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="114" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A114" t="s">
-        <v>205</v>
-      </c>
-      <c r="B114" t="s">
-        <v>104</v>
-      </c>
-    </row>
+    <row r="114" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="115" spans="1:3" ht="14.25" customHeight="1">
       <c r="A115" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B115" t="s">
-        <v>207</v>
+        <v>104</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="14.25" customHeight="1">
       <c r="A116" t="s">
-        <v>208</v>
-      </c>
-      <c r="B116">
-        <v>1</v>
+        <v>206</v>
+      </c>
+      <c r="B116" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="14.25" customHeight="1">
       <c r="A117" t="s">
-        <v>209</v>
-      </c>
-      <c r="B117" t="s">
-        <v>210</v>
+        <v>208</v>
+      </c>
+      <c r="B117">
+        <v>1</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="14.25" customHeight="1">
       <c r="A118" t="s">
-        <v>211</v>
-      </c>
-      <c r="B118">
-        <v>1</v>
+        <v>209</v>
+      </c>
+      <c r="B118" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="14.25" customHeight="1">
       <c r="A119" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B119">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="14.25" customHeight="1">
       <c r="A120" t="s">
-        <v>254</v>
+        <v>212</v>
       </c>
       <c r="B120">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="14.25" customHeight="1">
       <c r="A121" t="s">
-        <v>242</v>
-      </c>
-      <c r="B121" t="s">
-        <v>262</v>
-      </c>
-      <c r="C121" t="s">
-        <v>253</v>
+        <v>254</v>
+      </c>
+      <c r="B121">
+        <v>1</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="14.25" customHeight="1">
       <c r="A122" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B122" t="s">
-        <v>244</v>
+        <v>262</v>
+      </c>
+      <c r="C122" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="123" spans="1:3" ht="14.25" customHeight="1">
       <c r="A123" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B123" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="124" spans="1:3" ht="14.25" customHeight="1">
       <c r="A124" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B124" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="14.25" customHeight="1">
       <c r="A125" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B125" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="14.25" customHeight="1">
       <c r="A126" t="s">
+        <v>247</v>
+      </c>
+      <c r="B126" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A127" t="s">
         <v>250</v>
       </c>
-      <c r="B126" t="s">
+      <c r="B127" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="127" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="128" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A128" t="s">
-        <v>222</v>
-      </c>
-      <c r="B128" s="2" t="s">
-        <v>223</v>
-      </c>
-    </row>
+    <row r="128" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="129" spans="1:3" ht="14.25" customHeight="1">
       <c r="A129" t="s">
-        <v>231</v>
-      </c>
-      <c r="B129" t="s">
-        <v>134</v>
+        <v>222</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="130" spans="1:3" ht="14.25" customHeight="1">
       <c r="A130" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B130" t="s">
-        <v>233</v>
+        <v>134</v>
       </c>
     </row>
     <row r="131" spans="1:3" ht="14.25" customHeight="1">
       <c r="A131" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="B131" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
     </row>
     <row r="132" spans="1:3" ht="14.25" customHeight="1">
       <c r="A132" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B132" t="s">
-        <v>259</v>
+        <v>229</v>
       </c>
     </row>
     <row r="133" spans="1:3" ht="14.25" customHeight="1">
       <c r="A133" t="s">
-        <v>260</v>
+        <v>225</v>
       </c>
       <c r="B133" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="134" spans="1:3" ht="14.25" customHeight="1">
       <c r="A134" t="s">
-        <v>226</v>
+        <v>260</v>
       </c>
       <c r="B134" t="s">
-        <v>227</v>
+        <v>261</v>
       </c>
     </row>
     <row r="135" spans="1:3" ht="14.25" customHeight="1">
       <c r="A135" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B135" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="136" spans="1:3" ht="14.25" customHeight="1">
       <c r="A136" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="B136" t="s">
-        <v>241</v>
-      </c>
-      <c r="C136" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
     </row>
     <row r="137" spans="1:3" ht="14.25" customHeight="1">
       <c r="A137" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B137" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C137" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="138" spans="1:3" ht="14.25" customHeight="1">
       <c r="A138" t="s">
+        <v>236</v>
+      </c>
+      <c r="B138" t="s">
+        <v>240</v>
+      </c>
+      <c r="C138" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A139" t="s">
         <v>238</v>
       </c>
-      <c r="B138" t="s">
+      <c r="B139" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="139" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="140" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="141" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="142" spans="1:3" ht="14.25" customHeight="1"/>
@@ -4067,6 +4083,7 @@
     <row r="776" ht="14.25" customHeight="1"/>
     <row r="777" ht="14.25" customHeight="1"/>
     <row r="778" ht="14.25" customHeight="1"/>
+    <row r="779" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
commit changes for LA in Config File to Get Gross Sales
</commit_message>
<xml_diff>
--- a/STS IR Bot Performer/Data/Config.xlsx
+++ b/STS IR Bot Performer/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\martin.martinez\Documents\github-IRBot\STS_InternalReviewBot\STS IR Bot Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72D8E7AD-540D-4609-9361-0A490815926E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1F62EA7-3994-4201-92E6-5F7F55C58549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="265">
   <si>
     <t>Name</t>
   </si>
@@ -824,13 +824,13 @@
     <t>Data\Output\SC ST 389 tool &lt;CUSTOMER&gt;.xlsx</t>
   </si>
   <si>
-    <t>RENTALS AND SERVICES AS REPORTED TO THE STATE OF LOUISIANA###and services as reported to the State of LA###SERVICES AS REPORTED TO THE STATE OF LOUISIANA###GROSS SALES OF TANGIBLE###Gross Sales of Tangible###Gross sales of tangible###Gross Sales of tangible###Gross sales of Tangible###GROSS SALES OF THE TANGIBLE</t>
-  </si>
-  <si>
     <t>\\10.250.52.158\Depts\TaxReturnOutSourcing\Preparer\UIPathPublish\IR Bot Temp Files\InputFiles</t>
   </si>
   <si>
     <t>PathDifferentPDriveFolder</t>
+  </si>
+  <si>
+    <t>Monthly</t>
   </si>
 </sst>
 </file>
@@ -2344,8 +2344,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z779"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
+      <selection activeCell="C122" sqref="C122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2536,10 +2536,10 @@
     </row>
     <row r="19" spans="1:3" s="6" customFormat="1" ht="14.25" customHeight="1">
       <c r="A19" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>68</v>
@@ -3294,8 +3294,8 @@
       <c r="A121" t="s">
         <v>254</v>
       </c>
-      <c r="B121">
-        <v>1</v>
+      <c r="B121" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="14.25" customHeight="1">
@@ -3303,7 +3303,7 @@
         <v>242</v>
       </c>
       <c r="B122" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="C122" t="s">
         <v>253</v>

</xml_diff>

<commit_message>
add changes in relation to P drive validations
</commit_message>
<xml_diff>
--- a/STS IR Bot Performer/Data/Config.xlsx
+++ b/STS IR Bot Performer/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\martin.martinez\Documents\github-IRBot\STS_InternalReviewBot\STS IR Bot Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1F62EA7-3994-4201-92E6-5F7F55C58549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F7BB3FE-B7DB-47D2-A129-C4F6066C5031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24855" yWindow="2070" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="267">
   <si>
     <t>Name</t>
   </si>
@@ -809,9 +809,6 @@
     <t>WA Rev-40</t>
   </si>
   <si>
-    <t>P:\TaxReturnOutSourcing\Preparer\UIPathPublish\IR Bot Temp Files\pdfTemp &lt;USERNAME&gt; &lt;CUSTOMER&gt;.pdf</t>
-  </si>
-  <si>
     <t>Data\Output\CO DR-0100 XML tool &lt;CUSTOMER&gt;.xlsm</t>
   </si>
   <si>
@@ -831,6 +828,15 @@
   </si>
   <si>
     <t>Monthly</t>
+  </si>
+  <si>
+    <t>\\10.250.52.158\Depts\TaxReturnOutSourcing\Preparer\UIPathPublish\IR Bot Temp Files\pdfTemp &lt;USERNAME&gt; &lt;CUSTOMER&gt;.pdf</t>
+  </si>
+  <si>
+    <t>PathDifferentTempToPDF</t>
+  </si>
+  <si>
+    <t>\\somproddfs1.prod.sovos.org\depts\TaxReturnOutSourcing\Preparer\UIPathPublish\IR Bot Temp Files\pdfTemp &lt;USERNAME&gt; &lt;CUSTOMER&gt;.pdf</t>
   </si>
 </sst>
 </file>
@@ -895,7 +901,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -907,6 +913,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2342,10 +2349,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z779"/>
+  <dimension ref="A1:Z780"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
-      <selection activeCell="C122" sqref="C122"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2536,10 +2543,10 @@
     </row>
     <row r="19" spans="1:3" s="6" customFormat="1" ht="14.25" customHeight="1">
       <c r="A19" s="5" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>68</v>
@@ -2595,856 +2602,863 @@
       <c r="A25" t="s">
         <v>98</v>
       </c>
-      <c r="B25" t="s">
-        <v>257</v>
+      <c r="B25" s="7" t="s">
+        <v>264</v>
       </c>
       <c r="C25" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="27" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A27" t="s">
-        <v>82</v>
-      </c>
-      <c r="B27" t="s">
-        <v>83</v>
-      </c>
-      <c r="C27" t="s">
-        <v>84</v>
-      </c>
-    </row>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A26" t="s">
+        <v>265</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="28" spans="1:3" ht="14.25" customHeight="1">
       <c r="A28" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B28" t="s">
-        <v>87</v>
+        <v>83</v>
+      </c>
+      <c r="C28" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1">
       <c r="A29" t="s">
+        <v>86</v>
+      </c>
+      <c r="B29" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A30" t="s">
         <v>93</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B30" t="s">
         <v>94</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C30" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="31" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A31" t="s">
+    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A32" t="s">
         <v>69</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" t="s">
         <v>70</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C32" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="33" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A33" t="s">
-        <v>72</v>
-      </c>
-      <c r="B33" t="s">
-        <v>73</v>
-      </c>
-    </row>
+    <row r="33" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="34" spans="1:3" ht="14.25" customHeight="1">
       <c r="A34" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B34" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="14.25" customHeight="1">
       <c r="A35" t="s">
+        <v>74</v>
+      </c>
+      <c r="B35" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A36" t="s">
         <v>75</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B36" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="37" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A37" t="s">
-        <v>54</v>
-      </c>
-      <c r="B37" t="s">
-        <v>55</v>
-      </c>
-    </row>
+    <row r="37" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="38" spans="1:3" ht="14.25" customHeight="1">
       <c r="A38" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B38" t="s">
-        <v>57</v>
-      </c>
-      <c r="C38" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="14.25" customHeight="1">
       <c r="A39" t="s">
+        <v>56</v>
+      </c>
+      <c r="B39" t="s">
+        <v>57</v>
+      </c>
+      <c r="C39" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A40" t="s">
         <v>59</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B40" t="s">
         <v>60</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C40" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="41" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A41" t="s">
-        <v>178</v>
-      </c>
-      <c r="B41" t="s">
-        <v>184</v>
-      </c>
-    </row>
+    <row r="41" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="42" spans="1:3" ht="14.25" customHeight="1">
       <c r="A42" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="B42" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="14.25" customHeight="1">
       <c r="A43" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="B43" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="14.25" customHeight="1">
       <c r="A44" t="s">
+        <v>179</v>
+      </c>
+      <c r="B44" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A45" t="s">
         <v>255</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B45" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="46" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A46" t="s">
-        <v>63</v>
-      </c>
-      <c r="B46" t="s">
-        <v>64</v>
-      </c>
-    </row>
+    <row r="46" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="47" spans="1:3" ht="14.25" customHeight="1">
       <c r="A47" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B47" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="14.25" customHeight="1">
       <c r="A48" t="s">
-        <v>88</v>
+        <v>65</v>
       </c>
       <c r="B48" t="s">
-        <v>89</v>
+        <v>66</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="14.25" customHeight="1">
       <c r="A49" t="s">
-        <v>114</v>
+        <v>88</v>
       </c>
       <c r="B49" t="s">
-        <v>115</v>
+        <v>89</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="14.25" customHeight="1">
       <c r="A50" t="s">
-        <v>96</v>
+        <v>114</v>
       </c>
       <c r="B50" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="14.25" customHeight="1">
       <c r="A51" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B51" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="14.25" customHeight="1">
       <c r="A52" t="s">
+        <v>100</v>
+      </c>
+      <c r="B52" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A53" t="s">
         <v>185</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B53" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="54" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A54" t="s">
+    <row r="54" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="55" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A55" t="s">
         <v>102</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B55" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="56" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A56" t="s">
-        <v>103</v>
-      </c>
-      <c r="B56" t="s">
-        <v>104</v>
-      </c>
-    </row>
+    <row r="56" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="57" spans="1:3" ht="14.25" customHeight="1">
       <c r="A57" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B57" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="14.25" customHeight="1">
       <c r="A58" t="s">
+        <v>105</v>
+      </c>
+      <c r="B58" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A59" t="s">
         <v>107</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B59" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="60" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A60" t="s">
+    <row r="60" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="61" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A61" t="s">
         <v>109</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B61" t="s">
         <v>110</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C61" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="62" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A62" t="s">
-        <v>112</v>
-      </c>
-      <c r="B62" t="s">
-        <v>113</v>
-      </c>
-      <c r="C62" t="s">
-        <v>116</v>
-      </c>
-    </row>
+    <row r="62" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="63" spans="1:3" ht="14.25" customHeight="1">
       <c r="A63" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B63" t="s">
-        <v>118</v>
+        <v>113</v>
+      </c>
+      <c r="C63" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="14.25" customHeight="1">
       <c r="A64" t="s">
-        <v>119</v>
-      </c>
-      <c r="B64">
-        <v>1</v>
+        <v>117</v>
+      </c>
+      <c r="B64" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="14.25" customHeight="1">
       <c r="A65" t="s">
-        <v>120</v>
-      </c>
-      <c r="B65" t="s">
-        <v>121</v>
+        <v>119</v>
+      </c>
+      <c r="B65">
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="14.25" customHeight="1">
       <c r="A66" t="s">
-        <v>122</v>
-      </c>
-      <c r="B66">
-        <v>1</v>
+        <v>120</v>
+      </c>
+      <c r="B66" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="14.25" customHeight="1">
       <c r="A67" t="s">
-        <v>123</v>
-      </c>
-      <c r="B67" t="s">
-        <v>124</v>
+        <v>122</v>
+      </c>
+      <c r="B67">
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="14.25" customHeight="1">
       <c r="A68" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B68" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="14.25" customHeight="1">
       <c r="A69" t="s">
+        <v>125</v>
+      </c>
+      <c r="B69" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A70" t="s">
         <v>127</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B70" t="s">
         <v>128</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C70" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="71" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A71" t="s">
+    <row r="71" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="72" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A72" t="s">
         <v>130</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B72" t="s">
         <v>131</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C72" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="73" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A73" t="s">
-        <v>133</v>
-      </c>
-      <c r="B73" t="s">
-        <v>134</v>
-      </c>
-    </row>
+    <row r="73" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="74" spans="1:3" ht="14.25" customHeight="1">
       <c r="A74" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B74" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="14.25" customHeight="1">
       <c r="A75" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B75" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="14.25" customHeight="1">
       <c r="A76" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B76" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="14.25" customHeight="1">
       <c r="A77" t="s">
-        <v>141</v>
-      </c>
-      <c r="B77">
-        <v>1</v>
+        <v>139</v>
+      </c>
+      <c r="B77" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="14.25" customHeight="1">
       <c r="A78" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B78">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="14.25" customHeight="1">
       <c r="A79" t="s">
+        <v>142</v>
+      </c>
+      <c r="B79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A80" t="s">
         <v>143</v>
       </c>
-      <c r="B79">
+      <c r="B80">
         <v>2</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="81" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A81" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="B81" t="s">
-        <v>134</v>
-      </c>
-    </row>
+    <row r="81" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="82" spans="1:2" ht="14.25" customHeight="1">
       <c r="A82" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>203</v>
+        <v>144</v>
+      </c>
+      <c r="B82" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="14.25" customHeight="1">
       <c r="A83" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="B83" t="s">
-        <v>146</v>
+        <v>145</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="14.25" customHeight="1">
       <c r="A84" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>189</v>
+        <v>147</v>
+      </c>
+      <c r="B84" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="14.25" customHeight="1">
       <c r="A85" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>258</v>
+        <v>189</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="14.25" customHeight="1">
       <c r="A86" s="2" t="s">
-        <v>148</v>
+        <v>190</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>149</v>
+        <v>257</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="14.25" customHeight="1">
       <c r="A87" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="B87" t="s">
-        <v>151</v>
+        <v>148</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="14.25" customHeight="1">
       <c r="A88" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B88" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="14.25" customHeight="1">
       <c r="A89" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B89" t="s">
-        <v>140</v>
+        <v>152</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="14.25" customHeight="1">
       <c r="A90" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="B90">
-        <v>1</v>
+        <v>154</v>
+      </c>
+      <c r="B90" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="14.25" customHeight="1">
       <c r="A91" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B91">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="14.25" customHeight="1">
       <c r="A92" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A93" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="B92">
+      <c r="B93">
         <v>1</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A93" t="s">
-        <v>158</v>
-      </c>
-      <c r="B93">
-        <v>35</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="14.25" customHeight="1">
       <c r="A94" t="s">
-        <v>160</v>
-      </c>
-      <c r="B94" t="s">
-        <v>159</v>
+        <v>158</v>
+      </c>
+      <c r="B94">
+        <v>35</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="14.25" customHeight="1">
       <c r="A95" t="s">
+        <v>160</v>
+      </c>
+      <c r="B95" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A96" t="s">
         <v>162</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B96" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A96" s="2" t="s">
+    <row r="97" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A97" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B97" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="97" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A97" s="2" t="s">
+    <row r="98" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A98" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="B97" s="2" t="s">
+      <c r="B98" s="2" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="98" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A98" s="2" t="s">
+    <row r="99" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A99" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="B98" s="2" t="s">
+      <c r="B99" s="2" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="99" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A99" s="2" t="s">
+    <row r="100" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A100" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="B99" s="2" t="s">
+      <c r="B100" s="2" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="100" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A100" s="2" t="s">
+    <row r="101" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A101" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="B100" s="2" t="s">
+      <c r="B101" s="2" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="101" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A101" s="2" t="s">
+    <row r="102" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A102" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="B101" s="2" t="s">
+      <c r="B102" s="2" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="102" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="103" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A103" t="s">
+    <row r="103" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="104" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A104" t="s">
         <v>163</v>
       </c>
-      <c r="B103" t="s">
+      <c r="B104" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A104" t="s">
+    <row r="105" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A105" t="s">
         <v>164</v>
       </c>
-      <c r="B104" t="s">
+      <c r="B105" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A105" t="s">
+    <row r="106" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A106" t="s">
         <v>165</v>
       </c>
-      <c r="B105" t="s">
+      <c r="B106" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="106" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A106" t="s">
+    <row r="107" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A107" t="s">
         <v>182</v>
       </c>
-      <c r="B106">
+      <c r="B107">
         <v>6</v>
       </c>
     </row>
-    <row r="107" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A107" t="s">
+    <row r="108" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A108" t="s">
         <v>221</v>
-      </c>
-      <c r="B107" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A108" t="s">
-        <v>166</v>
       </c>
       <c r="B108" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="109" spans="1:3" ht="14.25" customHeight="1">
+    <row r="109" spans="1:2" ht="14.25" customHeight="1">
       <c r="A109" t="s">
+        <v>166</v>
+      </c>
+      <c r="B109" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A110" t="s">
         <v>167</v>
       </c>
-      <c r="B109">
+      <c r="B110">
         <v>2</v>
       </c>
     </row>
-    <row r="110" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A110" t="s">
+    <row r="111" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A111" t="s">
         <v>168</v>
       </c>
-      <c r="B110" t="s">
+      <c r="B111" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="111" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A111" t="s">
+    <row r="112" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A112" t="s">
         <v>170</v>
       </c>
-      <c r="B111" t="s">
+      <c r="B112" t="s">
         <v>171</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A112" t="s">
-        <v>172</v>
-      </c>
-      <c r="B112" t="s">
-        <v>173</v>
-      </c>
-      <c r="C112" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="14.25" customHeight="1">
       <c r="A113" t="s">
+        <v>172</v>
+      </c>
+      <c r="B113" t="s">
+        <v>173</v>
+      </c>
+      <c r="C113" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A114" t="s">
         <v>175</v>
       </c>
-      <c r="B113" t="s">
+      <c r="B114" t="s">
         <v>176</v>
       </c>
-      <c r="C113" t="s">
+      <c r="C114" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="114" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="115" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A115" t="s">
-        <v>205</v>
-      </c>
-      <c r="B115" t="s">
-        <v>104</v>
-      </c>
-    </row>
+    <row r="115" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="116" spans="1:3" ht="14.25" customHeight="1">
       <c r="A116" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B116" t="s">
-        <v>207</v>
+        <v>104</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="14.25" customHeight="1">
       <c r="A117" t="s">
-        <v>208</v>
-      </c>
-      <c r="B117">
-        <v>1</v>
+        <v>206</v>
+      </c>
+      <c r="B117" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="14.25" customHeight="1">
       <c r="A118" t="s">
-        <v>209</v>
-      </c>
-      <c r="B118" t="s">
-        <v>210</v>
+        <v>208</v>
+      </c>
+      <c r="B118">
+        <v>1</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="14.25" customHeight="1">
       <c r="A119" t="s">
-        <v>211</v>
-      </c>
-      <c r="B119">
-        <v>1</v>
+        <v>209</v>
+      </c>
+      <c r="B119" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="14.25" customHeight="1">
       <c r="A120" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B120">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="14.25" customHeight="1">
       <c r="A121" t="s">
-        <v>254</v>
-      </c>
-      <c r="B121" t="s">
-        <v>104</v>
+        <v>212</v>
+      </c>
+      <c r="B121">
+        <v>0</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="14.25" customHeight="1">
       <c r="A122" t="s">
-        <v>242</v>
+        <v>254</v>
       </c>
       <c r="B122" t="s">
-        <v>264</v>
-      </c>
-      <c r="C122" t="s">
-        <v>253</v>
+        <v>104</v>
       </c>
     </row>
     <row r="123" spans="1:3" ht="14.25" customHeight="1">
       <c r="A123" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B123" t="s">
-        <v>244</v>
+        <v>263</v>
+      </c>
+      <c r="C123" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="124" spans="1:3" ht="14.25" customHeight="1">
       <c r="A124" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B124" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="14.25" customHeight="1">
       <c r="A125" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B125" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="14.25" customHeight="1">
       <c r="A126" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B126" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="14.25" customHeight="1">
       <c r="A127" t="s">
+        <v>247</v>
+      </c>
+      <c r="B127" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A128" t="s">
         <v>250</v>
       </c>
-      <c r="B127" t="s">
+      <c r="B128" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="128" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="129" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A129" t="s">
-        <v>222</v>
-      </c>
-      <c r="B129" s="2" t="s">
-        <v>223</v>
-      </c>
-    </row>
+    <row r="129" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="130" spans="1:3" ht="14.25" customHeight="1">
       <c r="A130" t="s">
-        <v>231</v>
-      </c>
-      <c r="B130" t="s">
-        <v>134</v>
+        <v>222</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="131" spans="1:3" ht="14.25" customHeight="1">
       <c r="A131" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B131" t="s">
-        <v>233</v>
+        <v>134</v>
       </c>
     </row>
     <row r="132" spans="1:3" ht="14.25" customHeight="1">
       <c r="A132" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="B132" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
     </row>
     <row r="133" spans="1:3" ht="14.25" customHeight="1">
       <c r="A133" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B133" t="s">
-        <v>259</v>
+        <v>229</v>
       </c>
     </row>
     <row r="134" spans="1:3" ht="14.25" customHeight="1">
       <c r="A134" t="s">
-        <v>260</v>
+        <v>225</v>
       </c>
       <c r="B134" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="135" spans="1:3" ht="14.25" customHeight="1">
       <c r="A135" t="s">
-        <v>226</v>
+        <v>259</v>
       </c>
       <c r="B135" t="s">
-        <v>227</v>
+        <v>260</v>
       </c>
     </row>
     <row r="136" spans="1:3" ht="14.25" customHeight="1">
       <c r="A136" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B136" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="137" spans="1:3" ht="14.25" customHeight="1">
       <c r="A137" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="B137" t="s">
-        <v>241</v>
-      </c>
-      <c r="C137" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
     </row>
     <row r="138" spans="1:3" ht="14.25" customHeight="1">
       <c r="A138" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B138" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C138" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="139" spans="1:3" ht="14.25" customHeight="1">
       <c r="A139" t="s">
+        <v>236</v>
+      </c>
+      <c r="B139" t="s">
+        <v>240</v>
+      </c>
+      <c r="C139" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A140" t="s">
         <v>238</v>
       </c>
-      <c r="B139" t="s">
+      <c r="B140" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="140" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="141" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="142" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="143" spans="1:3" ht="14.25" customHeight="1"/>
@@ -4084,6 +4098,7 @@
     <row r="777" ht="14.25" customHeight="1"/>
     <row r="778" ht="14.25" customHeight="1"/>
     <row r="779" ht="14.25" customHeight="1"/>
+    <row r="780" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
comit all fix of the last bugs
</commit_message>
<xml_diff>
--- a/STS IR Bot Performer/Data/Config.xlsx
+++ b/STS IR Bot Performer/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\martin.martinez\Documents\github-IRBot\STS_InternalReviewBot\STS IR Bot Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F7BB3FE-B7DB-47D2-A129-C4F6066C5031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{440E0095-123A-4C6B-89E8-67E6CE104548}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24855" yWindow="2070" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="675" yWindow="2070" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="269">
   <si>
     <t>Name</t>
   </si>
@@ -837,6 +837,12 @@
   </si>
   <si>
     <t>\\somproddfs1.prod.sovos.org\depts\TaxReturnOutSourcing\Preparer\UIPathPublish\IR Bot Temp Files\pdfTemp &lt;USERNAME&gt; &lt;CUSTOMER&gt;.pdf</t>
+  </si>
+  <si>
+    <t>ALExceptionalCase</t>
+  </si>
+  <si>
+    <t>PUF</t>
   </si>
 </sst>
 </file>
@@ -901,7 +907,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -913,7 +919,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2349,10 +2354,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z780"/>
+  <dimension ref="A1:Z781"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2602,7 +2607,7 @@
       <c r="A25" t="s">
         <v>98</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B25" t="s">
         <v>264</v>
       </c>
       <c r="C25" t="s">
@@ -2613,7 +2618,7 @@
       <c r="A26" t="s">
         <v>265</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B26" t="s">
         <v>266</v>
       </c>
     </row>
@@ -2660,551 +2665,554 @@
         <v>71</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="34" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A34" t="s">
-        <v>72</v>
-      </c>
-      <c r="B34" t="s">
-        <v>73</v>
-      </c>
-    </row>
+    <row r="33" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A33" t="s">
+        <v>267</v>
+      </c>
+      <c r="B33" t="s">
+        <v>268</v>
+      </c>
+      <c r="C33" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="35" spans="1:3" ht="14.25" customHeight="1">
       <c r="A35" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B35" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="14.25" customHeight="1">
       <c r="A36" t="s">
+        <v>74</v>
+      </c>
+      <c r="B36" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A37" t="s">
         <v>75</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="38" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A38" t="s">
-        <v>54</v>
-      </c>
-      <c r="B38" t="s">
-        <v>55</v>
-      </c>
-    </row>
+    <row r="38" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="39" spans="1:3" ht="14.25" customHeight="1">
       <c r="A39" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B39" t="s">
-        <v>57</v>
-      </c>
-      <c r="C39" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="14.25" customHeight="1">
       <c r="A40" t="s">
+        <v>56</v>
+      </c>
+      <c r="B40" t="s">
+        <v>57</v>
+      </c>
+      <c r="C40" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A41" t="s">
         <v>59</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B41" t="s">
         <v>60</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C41" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="42" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A42" t="s">
-        <v>178</v>
-      </c>
-      <c r="B42" t="s">
-        <v>184</v>
-      </c>
-    </row>
+    <row r="42" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="43" spans="1:3" ht="14.25" customHeight="1">
       <c r="A43" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="B43" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="14.25" customHeight="1">
       <c r="A44" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="B44" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="14.25" customHeight="1">
       <c r="A45" t="s">
+        <v>179</v>
+      </c>
+      <c r="B45" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A46" t="s">
         <v>255</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B46" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="47" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A47" t="s">
-        <v>63</v>
-      </c>
-      <c r="B47" t="s">
-        <v>64</v>
-      </c>
-    </row>
+    <row r="47" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="48" spans="1:3" ht="14.25" customHeight="1">
       <c r="A48" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B48" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="14.25" customHeight="1">
       <c r="A49" t="s">
-        <v>88</v>
+        <v>65</v>
       </c>
       <c r="B49" t="s">
-        <v>89</v>
+        <v>66</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="14.25" customHeight="1">
       <c r="A50" t="s">
-        <v>114</v>
+        <v>88</v>
       </c>
       <c r="B50" t="s">
-        <v>115</v>
+        <v>89</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="14.25" customHeight="1">
       <c r="A51" t="s">
-        <v>96</v>
+        <v>114</v>
       </c>
       <c r="B51" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="14.25" customHeight="1">
       <c r="A52" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B52" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="14.25" customHeight="1">
       <c r="A53" t="s">
+        <v>100</v>
+      </c>
+      <c r="B53" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A54" t="s">
         <v>185</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B54" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="55" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A55" t="s">
+    <row r="55" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="56" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A56" t="s">
         <v>102</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B56" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="57" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A57" t="s">
-        <v>103</v>
-      </c>
-      <c r="B57" t="s">
-        <v>104</v>
-      </c>
-    </row>
+    <row r="57" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="58" spans="1:3" ht="14.25" customHeight="1">
       <c r="A58" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B58" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="14.25" customHeight="1">
       <c r="A59" t="s">
+        <v>105</v>
+      </c>
+      <c r="B59" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A60" t="s">
         <v>107</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B60" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="61" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A61" t="s">
+    <row r="61" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="62" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A62" t="s">
         <v>109</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B62" t="s">
         <v>110</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C62" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="63" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A63" t="s">
-        <v>112</v>
-      </c>
-      <c r="B63" t="s">
-        <v>113</v>
-      </c>
-      <c r="C63" t="s">
-        <v>116</v>
-      </c>
-    </row>
+    <row r="63" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="64" spans="1:3" ht="14.25" customHeight="1">
       <c r="A64" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B64" t="s">
-        <v>118</v>
+        <v>113</v>
+      </c>
+      <c r="C64" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="14.25" customHeight="1">
       <c r="A65" t="s">
-        <v>119</v>
-      </c>
-      <c r="B65">
-        <v>1</v>
+        <v>117</v>
+      </c>
+      <c r="B65" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="14.25" customHeight="1">
       <c r="A66" t="s">
-        <v>120</v>
-      </c>
-      <c r="B66" t="s">
-        <v>121</v>
+        <v>119</v>
+      </c>
+      <c r="B66">
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="14.25" customHeight="1">
       <c r="A67" t="s">
-        <v>122</v>
-      </c>
-      <c r="B67">
-        <v>1</v>
+        <v>120</v>
+      </c>
+      <c r="B67" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="14.25" customHeight="1">
       <c r="A68" t="s">
-        <v>123</v>
-      </c>
-      <c r="B68" t="s">
-        <v>124</v>
+        <v>122</v>
+      </c>
+      <c r="B68">
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="14.25" customHeight="1">
       <c r="A69" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B69" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="14.25" customHeight="1">
       <c r="A70" t="s">
+        <v>125</v>
+      </c>
+      <c r="B70" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A71" t="s">
         <v>127</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B71" t="s">
         <v>128</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C71" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="72" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A72" t="s">
+    <row r="72" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="73" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A73" t="s">
         <v>130</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B73" t="s">
         <v>131</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C73" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="74" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A74" t="s">
-        <v>133</v>
-      </c>
-      <c r="B74" t="s">
-        <v>134</v>
-      </c>
-    </row>
+    <row r="74" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="75" spans="1:3" ht="14.25" customHeight="1">
       <c r="A75" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B75" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="14.25" customHeight="1">
       <c r="A76" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B76" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="14.25" customHeight="1">
       <c r="A77" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B77" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="14.25" customHeight="1">
       <c r="A78" t="s">
-        <v>141</v>
-      </c>
-      <c r="B78">
-        <v>1</v>
+        <v>139</v>
+      </c>
+      <c r="B78" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="14.25" customHeight="1">
       <c r="A79" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B79">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="14.25" customHeight="1">
       <c r="A80" t="s">
+        <v>142</v>
+      </c>
+      <c r="B80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A81" t="s">
         <v>143</v>
       </c>
-      <c r="B80">
+      <c r="B81">
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="82" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A82" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="B82" t="s">
-        <v>134</v>
-      </c>
-    </row>
+    <row r="82" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="83" spans="1:2" ht="14.25" customHeight="1">
       <c r="A83" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>203</v>
+        <v>144</v>
+      </c>
+      <c r="B83" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="14.25" customHeight="1">
       <c r="A84" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="B84" t="s">
-        <v>146</v>
+        <v>145</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="14.25" customHeight="1">
       <c r="A85" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>189</v>
+        <v>147</v>
+      </c>
+      <c r="B85" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="14.25" customHeight="1">
       <c r="A86" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>257</v>
+        <v>189</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="14.25" customHeight="1">
       <c r="A87" s="2" t="s">
-        <v>148</v>
+        <v>190</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>149</v>
+        <v>257</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="14.25" customHeight="1">
       <c r="A88" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="B88" t="s">
-        <v>151</v>
+        <v>148</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="14.25" customHeight="1">
       <c r="A89" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B89" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="14.25" customHeight="1">
       <c r="A90" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B90" t="s">
-        <v>140</v>
+        <v>152</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="14.25" customHeight="1">
       <c r="A91" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="B91">
-        <v>1</v>
+        <v>154</v>
+      </c>
+      <c r="B91" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="14.25" customHeight="1">
       <c r="A92" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B92">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="14.25" customHeight="1">
       <c r="A93" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A94" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="B93">
+      <c r="B94">
         <v>1</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A94" t="s">
-        <v>158</v>
-      </c>
-      <c r="B94">
-        <v>35</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="14.25" customHeight="1">
       <c r="A95" t="s">
-        <v>160</v>
-      </c>
-      <c r="B95" t="s">
-        <v>159</v>
+        <v>158</v>
+      </c>
+      <c r="B95">
+        <v>35</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="14.25" customHeight="1">
       <c r="A96" t="s">
+        <v>160</v>
+      </c>
+      <c r="B96" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A97" t="s">
         <v>162</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B97" t="s">
         <v>161</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A97" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="B97" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="14.25" customHeight="1">
       <c r="A98" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="B98" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
+      </c>
+      <c r="B98" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="14.25" customHeight="1">
       <c r="A99" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="14.25" customHeight="1">
       <c r="A100" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="14.25" customHeight="1">
       <c r="A101" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="14.25" customHeight="1">
       <c r="A102" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A103" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="B102" s="2" t="s">
+      <c r="B103" s="2" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="103" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="104" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A104" t="s">
-        <v>163</v>
-      </c>
-      <c r="B104" t="s">
-        <v>220</v>
-      </c>
-    </row>
+    <row r="104" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="105" spans="1:2" ht="14.25" customHeight="1">
       <c r="A105" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B105" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="14.25" customHeight="1">
       <c r="A106" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B106" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="14.25" customHeight="1">
       <c r="A107" t="s">
-        <v>182</v>
-      </c>
-      <c r="B107">
-        <v>6</v>
+        <v>165</v>
+      </c>
+      <c r="B107" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="14.25" customHeight="1">
       <c r="A108" t="s">
-        <v>221</v>
-      </c>
-      <c r="B108" t="s">
-        <v>128</v>
+        <v>182</v>
+      </c>
+      <c r="B108">
+        <v>6</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="14.25" customHeight="1">
       <c r="A109" t="s">
-        <v>166</v>
+        <v>221</v>
       </c>
       <c r="B109" t="s">
         <v>128</v>
@@ -3212,254 +3220,261 @@
     </row>
     <row r="110" spans="1:2" ht="14.25" customHeight="1">
       <c r="A110" t="s">
-        <v>167</v>
-      </c>
-      <c r="B110">
-        <v>2</v>
+        <v>166</v>
+      </c>
+      <c r="B110" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="14.25" customHeight="1">
       <c r="A111" t="s">
-        <v>168</v>
-      </c>
-      <c r="B111" t="s">
-        <v>169</v>
+        <v>167</v>
+      </c>
+      <c r="B111">
+        <v>2</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="14.25" customHeight="1">
       <c r="A112" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B112" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="14.25" customHeight="1">
       <c r="A113" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B113" t="s">
-        <v>173</v>
-      </c>
-      <c r="C113" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="14.25" customHeight="1">
       <c r="A114" t="s">
+        <v>172</v>
+      </c>
+      <c r="B114" t="s">
+        <v>173</v>
+      </c>
+      <c r="C114" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A115" t="s">
         <v>175</v>
       </c>
-      <c r="B114" t="s">
+      <c r="B115" t="s">
         <v>176</v>
       </c>
-      <c r="C114" t="s">
+      <c r="C115" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="115" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="116" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A116" t="s">
-        <v>205</v>
-      </c>
-      <c r="B116" t="s">
-        <v>104</v>
-      </c>
-    </row>
+    <row r="116" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="117" spans="1:3" ht="14.25" customHeight="1">
       <c r="A117" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B117" t="s">
-        <v>207</v>
+        <v>104</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="14.25" customHeight="1">
       <c r="A118" t="s">
-        <v>208</v>
-      </c>
-      <c r="B118">
-        <v>1</v>
+        <v>206</v>
+      </c>
+      <c r="B118" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="14.25" customHeight="1">
       <c r="A119" t="s">
-        <v>209</v>
-      </c>
-      <c r="B119" t="s">
-        <v>210</v>
+        <v>208</v>
+      </c>
+      <c r="B119">
+        <v>1</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="14.25" customHeight="1">
       <c r="A120" t="s">
-        <v>211</v>
-      </c>
-      <c r="B120">
-        <v>1</v>
+        <v>209</v>
+      </c>
+      <c r="B120" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="14.25" customHeight="1">
       <c r="A121" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B121">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="14.25" customHeight="1">
       <c r="A122" t="s">
-        <v>254</v>
-      </c>
-      <c r="B122" t="s">
-        <v>104</v>
+        <v>212</v>
+      </c>
+      <c r="B122">
+        <v>0</v>
       </c>
     </row>
     <row r="123" spans="1:3" ht="14.25" customHeight="1">
       <c r="A123" t="s">
-        <v>242</v>
+        <v>254</v>
       </c>
       <c r="B123" t="s">
-        <v>263</v>
-      </c>
-      <c r="C123" t="s">
-        <v>253</v>
+        <v>104</v>
       </c>
     </row>
     <row r="124" spans="1:3" ht="14.25" customHeight="1">
       <c r="A124" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B124" t="s">
-        <v>244</v>
+        <v>263</v>
+      </c>
+      <c r="C124" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="14.25" customHeight="1">
       <c r="A125" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B125" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="14.25" customHeight="1">
       <c r="A126" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B126" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="14.25" customHeight="1">
       <c r="A127" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B127" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="14.25" customHeight="1">
       <c r="A128" t="s">
+        <v>247</v>
+      </c>
+      <c r="B128" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A129" t="s">
         <v>250</v>
       </c>
-      <c r="B128" t="s">
+      <c r="B129" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="129" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="130" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A130" t="s">
-        <v>222</v>
-      </c>
-      <c r="B130" s="2" t="s">
-        <v>223</v>
-      </c>
-    </row>
+    <row r="130" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="131" spans="1:3" ht="14.25" customHeight="1">
       <c r="A131" t="s">
-        <v>231</v>
-      </c>
-      <c r="B131" t="s">
-        <v>134</v>
+        <v>222</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="132" spans="1:3" ht="14.25" customHeight="1">
       <c r="A132" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B132" t="s">
-        <v>233</v>
+        <v>134</v>
       </c>
     </row>
     <row r="133" spans="1:3" ht="14.25" customHeight="1">
       <c r="A133" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="B133" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
     </row>
     <row r="134" spans="1:3" ht="14.25" customHeight="1">
       <c r="A134" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B134" t="s">
-        <v>258</v>
+        <v>229</v>
       </c>
     </row>
     <row r="135" spans="1:3" ht="14.25" customHeight="1">
       <c r="A135" t="s">
-        <v>259</v>
+        <v>225</v>
       </c>
       <c r="B135" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="136" spans="1:3" ht="14.25" customHeight="1">
       <c r="A136" t="s">
-        <v>226</v>
+        <v>259</v>
       </c>
       <c r="B136" t="s">
-        <v>227</v>
+        <v>260</v>
       </c>
     </row>
     <row r="137" spans="1:3" ht="14.25" customHeight="1">
       <c r="A137" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B137" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="138" spans="1:3" ht="14.25" customHeight="1">
       <c r="A138" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="B138" t="s">
-        <v>241</v>
-      </c>
-      <c r="C138" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
     </row>
     <row r="139" spans="1:3" ht="14.25" customHeight="1">
       <c r="A139" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B139" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C139" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="140" spans="1:3" ht="14.25" customHeight="1">
       <c r="A140" t="s">
+        <v>236</v>
+      </c>
+      <c r="B140" t="s">
+        <v>240</v>
+      </c>
+      <c r="C140" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A141" t="s">
         <v>238</v>
       </c>
-      <c r="B140" t="s">
+      <c r="B141" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="141" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="142" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="143" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="144" spans="1:3" ht="14.25" customHeight="1"/>
@@ -4099,6 +4114,7 @@
     <row r="778" ht="14.25" customHeight="1"/>
     <row r="779" ht="14.25" customHeight="1"/>
     <row r="780" ht="14.25" customHeight="1"/>
+    <row r="781" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
new validation for LA R-1029 for get gross sales
</commit_message>
<xml_diff>
--- a/STS IR Bot Performer/Data/Config.xlsx
+++ b/STS IR Bot Performer/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\martin.martinez\Documents\github-IRBot\STS_InternalReviewBot\STS IR Bot Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{440E0095-123A-4C6B-89E8-67E6CE104548}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E4A205C-998D-4B66-B3B3-AD1D528F6DDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="675" yWindow="2070" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="273">
   <si>
     <t>Name</t>
   </si>
@@ -843,6 +843,18 @@
   </si>
   <si>
     <t>PUF</t>
+  </si>
+  <si>
+    <t>StateBalancing_LA_GrossSalesTabR1029</t>
+  </si>
+  <si>
+    <t>StateBalancing_LA_GrossSalesClickOnTextR1029</t>
+  </si>
+  <si>
+    <t>Only for LA R-1029 and LA R-1029E</t>
+  </si>
+  <si>
+    <t>Gross sales of tangible###Gross Sales of Tangible###Gross Sales of tangible###Gross sales of Tangible###GROSS SALES OF THE TANGIBLEGROSS SALES###Gross Sales###Gross sales###SERVICES AS REPORTED TO THE STATE###services as reported###RENTALS AND SERVICES AS REPORTED TO THE STATE OF LOUISIANA###and services as reported to the State of LA###SERVICES AS REPORTED TO THE STATE OF LOUISIANA###GROSS SALES OF TANGIBLE</t>
   </si>
 </sst>
 </file>
@@ -2354,10 +2366,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z781"/>
+  <dimension ref="A1:Z783"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="0">
+      <selection activeCell="B124" sqref="B124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3323,160 +3335,180 @@
     </row>
     <row r="123" spans="1:3" ht="14.25" customHeight="1">
       <c r="A123" t="s">
-        <v>254</v>
-      </c>
-      <c r="B123" t="s">
-        <v>104</v>
+        <v>269</v>
+      </c>
+      <c r="B123">
+        <v>1</v>
+      </c>
+      <c r="C123" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="124" spans="1:3" ht="14.25" customHeight="1">
       <c r="A124" t="s">
-        <v>242</v>
+        <v>270</v>
       </c>
       <c r="B124" t="s">
-        <v>263</v>
+        <v>272</v>
       </c>
       <c r="C124" t="s">
-        <v>253</v>
+        <v>271</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="14.25" customHeight="1">
       <c r="A125" t="s">
-        <v>243</v>
+        <v>254</v>
       </c>
       <c r="B125" t="s">
-        <v>244</v>
+        <v>104</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="14.25" customHeight="1">
       <c r="A126" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B126" t="s">
-        <v>246</v>
+        <v>263</v>
+      </c>
+      <c r="C126" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="14.25" customHeight="1">
       <c r="A127" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="B127" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="14.25" customHeight="1">
       <c r="A128" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B128" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
     </row>
     <row r="129" spans="1:3" ht="14.25" customHeight="1">
       <c r="A129" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B129" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" ht="14.25" customHeight="1"/>
+        <v>249</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A130" t="s">
+        <v>247</v>
+      </c>
+      <c r="B130" t="s">
+        <v>252</v>
+      </c>
+    </row>
     <row r="131" spans="1:3" ht="14.25" customHeight="1">
       <c r="A131" t="s">
-        <v>222</v>
-      </c>
-      <c r="B131" s="2" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A132" t="s">
-        <v>231</v>
-      </c>
-      <c r="B132" t="s">
-        <v>134</v>
-      </c>
-    </row>
+        <v>250</v>
+      </c>
+      <c r="B131" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="133" spans="1:3" ht="14.25" customHeight="1">
       <c r="A133" t="s">
-        <v>232</v>
-      </c>
-      <c r="B133" t="s">
-        <v>233</v>
+        <v>222</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="134" spans="1:3" ht="14.25" customHeight="1">
       <c r="A134" t="s">
-        <v>224</v>
+        <v>231</v>
       </c>
       <c r="B134" t="s">
-        <v>229</v>
+        <v>134</v>
       </c>
     </row>
     <row r="135" spans="1:3" ht="14.25" customHeight="1">
       <c r="A135" t="s">
-        <v>225</v>
+        <v>232</v>
       </c>
       <c r="B135" t="s">
-        <v>258</v>
+        <v>233</v>
       </c>
     </row>
     <row r="136" spans="1:3" ht="14.25" customHeight="1">
       <c r="A136" t="s">
-        <v>259</v>
+        <v>224</v>
       </c>
       <c r="B136" t="s">
-        <v>260</v>
+        <v>229</v>
       </c>
     </row>
     <row r="137" spans="1:3" ht="14.25" customHeight="1">
       <c r="A137" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B137" t="s">
-        <v>227</v>
+        <v>258</v>
       </c>
     </row>
     <row r="138" spans="1:3" ht="14.25" customHeight="1">
       <c r="A138" t="s">
-        <v>228</v>
+        <v>259</v>
       </c>
       <c r="B138" t="s">
-        <v>230</v>
+        <v>260</v>
       </c>
     </row>
     <row r="139" spans="1:3" ht="14.25" customHeight="1">
       <c r="A139" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="B139" t="s">
-        <v>241</v>
-      </c>
-      <c r="C139" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
     </row>
     <row r="140" spans="1:3" ht="14.25" customHeight="1">
       <c r="A140" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="B140" t="s">
-        <v>240</v>
-      </c>
-      <c r="C140" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
     </row>
     <row r="141" spans="1:3" ht="14.25" customHeight="1">
       <c r="A141" t="s">
+        <v>234</v>
+      </c>
+      <c r="B141" t="s">
+        <v>241</v>
+      </c>
+      <c r="C141" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A142" t="s">
+        <v>236</v>
+      </c>
+      <c r="B142" t="s">
+        <v>240</v>
+      </c>
+      <c r="C142" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A143" t="s">
         <v>238</v>
       </c>
-      <c r="B141" t="s">
+      <c r="B143" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="142" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="143" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="144" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="145" ht="14.25" customHeight="1"/>
     <row r="146" ht="14.25" customHeight="1"/>
@@ -4115,6 +4147,8 @@
     <row r="779" ht="14.25" customHeight="1"/>
     <row r="780" ht="14.25" customHeight="1"/>
     <row r="781" ht="14.25" customHeight="1"/>
+    <row r="782" ht="14.25" customHeight="1"/>
+    <row r="783" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add new send mail workflow
</commit_message>
<xml_diff>
--- a/STS IR Bot Performer/Data/Config.xlsx
+++ b/STS IR Bot Performer/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\martin.martinez\Documents\github-IRBot\STS_InternalReviewBot\STS IR Bot Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E4A205C-998D-4B66-B3B3-AD1D528F6DDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF645B70-DE9E-414A-BFA6-A8F1DE5ED94F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="280">
   <si>
     <t>Name</t>
   </si>
@@ -855,6 +855,27 @@
   </si>
   <si>
     <t>Gross sales of tangible###Gross Sales of Tangible###Gross Sales of tangible###Gross sales of Tangible###GROSS SALES OF THE TANGIBLEGROSS SALES###Gross Sales###Gross sales###SERVICES AS REPORTED TO THE STATE###services as reported###RENTALS AND SERVICES AS REPORTED TO THE STATE OF LOUISIANA###and services as reported to the State of LA###SERVICES AS REPORTED TO THE STATE OF LOUISIANA###GROSS SALES OF TANGIBLE</t>
+  </si>
+  <si>
+    <t>ServerMail</t>
+  </si>
+  <si>
+    <t>chkmailrelay.corp.sovos.local</t>
+  </si>
+  <si>
+    <t>PortMail</t>
+  </si>
+  <si>
+    <t>DefaultMailAdress</t>
+  </si>
+  <si>
+    <t>uipathdevelopment@sovos.com</t>
+  </si>
+  <si>
+    <t>DefaultMailName</t>
+  </si>
+  <si>
+    <t>UiPath Development</t>
   </si>
 </sst>
 </file>
@@ -2366,10 +2387,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z783"/>
+  <dimension ref="A1:Z788"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="0">
-      <selection activeCell="B124" sqref="B124"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2539,993 +2560,1021 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" s="5" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A17" s="5" t="s">
+    <row r="17" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A17" t="s">
+        <v>273</v>
+      </c>
+      <c r="B17" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A18" t="s">
+        <v>276</v>
+      </c>
+      <c r="B18" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A19" t="s">
+        <v>275</v>
+      </c>
+      <c r="B19">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A20" t="s">
+        <v>278</v>
+      </c>
+      <c r="B20" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="22" spans="1:3" s="5" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A22" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B22" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C22" s="5" t="s">
         <v>215</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" s="6" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A18" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" s="6" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A19" s="5" t="s">
-        <v>262</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>261</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" s="5" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A20" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A21" t="s">
-        <v>85</v>
-      </c>
-      <c r="B21" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" s="6" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A22" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="23" spans="1:3" s="6" customFormat="1" ht="14.25" customHeight="1">
       <c r="A23" s="6" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A24" t="s">
-        <v>91</v>
-      </c>
-      <c r="B24" t="s">
-        <v>181</v>
-      </c>
-      <c r="C24" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A25" t="s">
-        <v>98</v>
-      </c>
-      <c r="B25" t="s">
-        <v>264</v>
-      </c>
-      <c r="C25" t="s">
-        <v>99</v>
+        <v>216</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" s="6" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A24" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" s="5" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A25" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
       <c r="A26" t="s">
-        <v>265</v>
+        <v>85</v>
       </c>
       <c r="B26" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="28" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A28" t="s">
-        <v>82</v>
-      </c>
-      <c r="B28" t="s">
-        <v>83</v>
-      </c>
-      <c r="C28" t="s">
-        <v>84</v>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" s="6" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A27" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" s="6" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A28" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1">
       <c r="A29" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B29" t="s">
-        <v>87</v>
+        <v>181</v>
+      </c>
+      <c r="C29" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1">
       <c r="A30" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="B30" t="s">
-        <v>94</v>
+        <v>264</v>
       </c>
       <c r="C30" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="32" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A32" t="s">
-        <v>69</v>
-      </c>
-      <c r="B32" t="s">
-        <v>70</v>
-      </c>
-      <c r="C32" t="s">
-        <v>71</v>
-      </c>
-    </row>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A31" t="s">
+        <v>265</v>
+      </c>
+      <c r="B31" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="33" spans="1:3" ht="14.25" customHeight="1">
       <c r="A33" t="s">
-        <v>267</v>
+        <v>82</v>
       </c>
       <c r="B33" t="s">
-        <v>268</v>
+        <v>83</v>
       </c>
       <c r="C33" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="14.25" customHeight="1"/>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A34" t="s">
+        <v>86</v>
+      </c>
+      <c r="B34" t="s">
+        <v>87</v>
+      </c>
+    </row>
     <row r="35" spans="1:3" ht="14.25" customHeight="1">
       <c r="A35" t="s">
-        <v>72</v>
+        <v>93</v>
       </c>
       <c r="B35" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A36" t="s">
-        <v>74</v>
-      </c>
-      <c r="B36" t="s">
-        <v>77</v>
-      </c>
-    </row>
+        <v>94</v>
+      </c>
+      <c r="C35" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="37" spans="1:3" ht="14.25" customHeight="1">
       <c r="A37" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B37" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="39" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A39" t="s">
-        <v>54</v>
-      </c>
-      <c r="B39" t="s">
-        <v>55</v>
-      </c>
-    </row>
+        <v>70</v>
+      </c>
+      <c r="C37" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A38" t="s">
+        <v>267</v>
+      </c>
+      <c r="B38" t="s">
+        <v>268</v>
+      </c>
+      <c r="C38" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="40" spans="1:3" ht="14.25" customHeight="1">
       <c r="A40" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="B40" t="s">
-        <v>57</v>
-      </c>
-      <c r="C40" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="14.25" customHeight="1">
       <c r="A41" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="B41" t="s">
-        <v>60</v>
-      </c>
-      <c r="C41" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="43" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A43" t="s">
-        <v>178</v>
-      </c>
-      <c r="B43" t="s">
-        <v>184</v>
-      </c>
-    </row>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A42" t="s">
+        <v>75</v>
+      </c>
+      <c r="B42" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="44" spans="1:3" ht="14.25" customHeight="1">
       <c r="A44" t="s">
-        <v>187</v>
+        <v>54</v>
       </c>
       <c r="B44" t="s">
-        <v>183</v>
+        <v>55</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="14.25" customHeight="1">
       <c r="A45" t="s">
-        <v>179</v>
+        <v>56</v>
       </c>
       <c r="B45" t="s">
-        <v>180</v>
+        <v>57</v>
+      </c>
+      <c r="C45" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="14.25" customHeight="1">
       <c r="A46" t="s">
-        <v>255</v>
+        <v>59</v>
       </c>
       <c r="B46" t="s">
-        <v>256</v>
+        <v>60</v>
+      </c>
+      <c r="C46" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="48" spans="1:3" ht="14.25" customHeight="1">
       <c r="A48" t="s">
+        <v>178</v>
+      </c>
+      <c r="B48" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A49" t="s">
+        <v>187</v>
+      </c>
+      <c r="B49" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A50" t="s">
+        <v>179</v>
+      </c>
+      <c r="B50" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A51" t="s">
+        <v>255</v>
+      </c>
+      <c r="B51" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="53" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A53" t="s">
         <v>63</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B53" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A49" t="s">
+    <row r="54" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A54" t="s">
         <v>65</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B54" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A50" t="s">
+    <row r="55" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A55" t="s">
         <v>88</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B55" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A51" t="s">
+    <row r="56" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A56" t="s">
         <v>114</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B56" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A52" t="s">
+    <row r="57" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A57" t="s">
         <v>96</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B57" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A53" t="s">
+    <row r="58" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A58" t="s">
         <v>100</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B58" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A54" t="s">
+    <row r="59" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A59" t="s">
         <v>185</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B59" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="56" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A56" t="s">
+    <row r="60" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="61" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A61" t="s">
         <v>102</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B61" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="58" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A58" t="s">
+    <row r="62" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="63" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A63" t="s">
         <v>103</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B63" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A59" t="s">
+    <row r="64" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A64" t="s">
         <v>105</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B64" t="s">
         <v>106</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A60" t="s">
-        <v>107</v>
-      </c>
-      <c r="B60" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="62" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A62" t="s">
-        <v>109</v>
-      </c>
-      <c r="B62" t="s">
-        <v>110</v>
-      </c>
-      <c r="C62" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="64" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A64" t="s">
-        <v>112</v>
-      </c>
-      <c r="B64" t="s">
-        <v>113</v>
-      </c>
-      <c r="C64" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="14.25" customHeight="1">
       <c r="A65" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="B65" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A66" t="s">
-        <v>119</v>
-      </c>
-      <c r="B66">
-        <v>1</v>
-      </c>
-    </row>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="67" spans="1:3" ht="14.25" customHeight="1">
       <c r="A67" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="B67" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A68" t="s">
-        <v>122</v>
-      </c>
-      <c r="B68">
-        <v>1</v>
-      </c>
-    </row>
+        <v>110</v>
+      </c>
+      <c r="C67" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="69" spans="1:3" ht="14.25" customHeight="1">
       <c r="A69" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="B69" t="s">
-        <v>124</v>
+        <v>113</v>
+      </c>
+      <c r="C69" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="14.25" customHeight="1">
       <c r="A70" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="B70" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="14.25" customHeight="1">
       <c r="A71" t="s">
-        <v>127</v>
-      </c>
-      <c r="B71" t="s">
-        <v>128</v>
-      </c>
-      <c r="C71" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" ht="14.25" customHeight="1"/>
+        <v>119</v>
+      </c>
+      <c r="B71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A72" t="s">
+        <v>120</v>
+      </c>
+      <c r="B72" t="s">
+        <v>121</v>
+      </c>
+    </row>
     <row r="73" spans="1:3" ht="14.25" customHeight="1">
       <c r="A73" t="s">
-        <v>130</v>
-      </c>
-      <c r="B73" t="s">
-        <v>131</v>
-      </c>
-      <c r="C73" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" ht="14.25" customHeight="1"/>
+        <v>122</v>
+      </c>
+      <c r="B73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A74" t="s">
+        <v>123</v>
+      </c>
+      <c r="B74" t="s">
+        <v>124</v>
+      </c>
+    </row>
     <row r="75" spans="1:3" ht="14.25" customHeight="1">
       <c r="A75" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="B75" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="14.25" customHeight="1">
       <c r="A76" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="B76" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A77" t="s">
-        <v>136</v>
-      </c>
-      <c r="B77" t="s">
-        <v>137</v>
-      </c>
-    </row>
+        <v>128</v>
+      </c>
+      <c r="C76" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="78" spans="1:3" ht="14.25" customHeight="1">
       <c r="A78" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="B78" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A79" t="s">
-        <v>141</v>
-      </c>
-      <c r="B79">
-        <v>1</v>
-      </c>
-    </row>
+        <v>131</v>
+      </c>
+      <c r="C78" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="80" spans="1:3" ht="14.25" customHeight="1">
       <c r="A80" t="s">
-        <v>142</v>
-      </c>
-      <c r="B80">
-        <v>0</v>
+        <v>133</v>
+      </c>
+      <c r="B80" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="14.25" customHeight="1">
       <c r="A81" t="s">
+        <v>135</v>
+      </c>
+      <c r="B81" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A82" t="s">
+        <v>136</v>
+      </c>
+      <c r="B82" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A83" t="s">
+        <v>139</v>
+      </c>
+      <c r="B83" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A84" t="s">
+        <v>141</v>
+      </c>
+      <c r="B84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A85" t="s">
+        <v>142</v>
+      </c>
+      <c r="B85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A86" t="s">
         <v>143</v>
       </c>
-      <c r="B81">
+      <c r="B86">
         <v>2</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="83" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A83" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="B83" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A84" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A85" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="B85" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A86" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A87" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
+    <row r="87" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="88" spans="1:2" ht="14.25" customHeight="1">
       <c r="A88" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>149</v>
+        <v>144</v>
+      </c>
+      <c r="B88" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="14.25" customHeight="1">
       <c r="A89" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="B89" t="s">
-        <v>151</v>
+        <v>145</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="14.25" customHeight="1">
       <c r="A90" s="2" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B90" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="14.25" customHeight="1">
       <c r="A91" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="B91" t="s">
-        <v>140</v>
+        <v>188</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="14.25" customHeight="1">
       <c r="A92" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="B92">
-        <v>1</v>
+        <v>190</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="14.25" customHeight="1">
       <c r="A93" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="B93">
-        <v>0</v>
+        <v>148</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="14.25" customHeight="1">
       <c r="A94" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="B94">
+        <v>150</v>
+      </c>
+      <c r="B94" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A95" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B95" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A96" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B96" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A97" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B97">
         <v>1</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A95" t="s">
-        <v>158</v>
-      </c>
-      <c r="B95">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A96" t="s">
-        <v>160</v>
-      </c>
-      <c r="B96" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A97" t="s">
-        <v>162</v>
-      </c>
-      <c r="B97" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="14.25" customHeight="1">
       <c r="A98" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="B98" t="s">
-        <v>192</v>
+        <v>156</v>
+      </c>
+      <c r="B98">
+        <v>0</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="14.25" customHeight="1">
       <c r="A99" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="B99" s="2" t="s">
-        <v>194</v>
+        <v>157</v>
+      </c>
+      <c r="B99">
+        <v>1</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A100" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="B100" s="2" t="s">
-        <v>196</v>
+      <c r="A100" t="s">
+        <v>158</v>
+      </c>
+      <c r="B100">
+        <v>35</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A101" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="B101" s="2" t="s">
-        <v>198</v>
+      <c r="A101" t="s">
+        <v>160</v>
+      </c>
+      <c r="B101" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A102" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="B102" s="2" t="s">
-        <v>200</v>
+      <c r="A102" t="s">
+        <v>162</v>
+      </c>
+      <c r="B102" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="14.25" customHeight="1">
       <c r="A103" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B103" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A104" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A105" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A106" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A107" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A108" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="B103" s="2" t="s">
+      <c r="B108" s="2" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="104" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="105" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A105" t="s">
-        <v>163</v>
-      </c>
-      <c r="B105" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A106" t="s">
-        <v>164</v>
-      </c>
-      <c r="B106" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A107" t="s">
-        <v>165</v>
-      </c>
-      <c r="B107" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A108" t="s">
-        <v>182</v>
-      </c>
-      <c r="B108">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A109" t="s">
-        <v>221</v>
-      </c>
-      <c r="B109" t="s">
-        <v>128</v>
-      </c>
-    </row>
+    <row r="109" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="110" spans="1:2" ht="14.25" customHeight="1">
       <c r="A110" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B110" t="s">
-        <v>128</v>
+        <v>220</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="14.25" customHeight="1">
       <c r="A111" t="s">
-        <v>167</v>
-      </c>
-      <c r="B111">
-        <v>2</v>
+        <v>164</v>
+      </c>
+      <c r="B111" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="14.25" customHeight="1">
       <c r="A112" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B112" t="s">
-        <v>169</v>
+        <v>218</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="14.25" customHeight="1">
       <c r="A113" t="s">
-        <v>170</v>
-      </c>
-      <c r="B113" t="s">
-        <v>171</v>
+        <v>182</v>
+      </c>
+      <c r="B113">
+        <v>6</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="14.25" customHeight="1">
       <c r="A114" t="s">
-        <v>172</v>
+        <v>221</v>
       </c>
       <c r="B114" t="s">
-        <v>173</v>
-      </c>
-      <c r="C114" t="s">
-        <v>174</v>
+        <v>128</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="14.25" customHeight="1">
       <c r="A115" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="B115" t="s">
-        <v>176</v>
-      </c>
-      <c r="C115" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" ht="14.25" customHeight="1"/>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A116" t="s">
+        <v>167</v>
+      </c>
+      <c r="B116">
+        <v>2</v>
+      </c>
+    </row>
     <row r="117" spans="1:3" ht="14.25" customHeight="1">
       <c r="A117" t="s">
-        <v>205</v>
+        <v>168</v>
       </c>
       <c r="B117" t="s">
-        <v>104</v>
+        <v>169</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="14.25" customHeight="1">
       <c r="A118" t="s">
-        <v>206</v>
+        <v>170</v>
       </c>
       <c r="B118" t="s">
-        <v>207</v>
+        <v>171</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="14.25" customHeight="1">
       <c r="A119" t="s">
-        <v>208</v>
-      </c>
-      <c r="B119">
-        <v>1</v>
+        <v>172</v>
+      </c>
+      <c r="B119" t="s">
+        <v>173</v>
+      </c>
+      <c r="C119" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="14.25" customHeight="1">
       <c r="A120" t="s">
-        <v>209</v>
+        <v>175</v>
       </c>
       <c r="B120" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A121" t="s">
-        <v>211</v>
-      </c>
-      <c r="B121">
-        <v>1</v>
-      </c>
-    </row>
+        <v>176</v>
+      </c>
+      <c r="C120" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="122" spans="1:3" ht="14.25" customHeight="1">
       <c r="A122" t="s">
-        <v>212</v>
-      </c>
-      <c r="B122">
-        <v>0</v>
+        <v>205</v>
+      </c>
+      <c r="B122" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="123" spans="1:3" ht="14.25" customHeight="1">
       <c r="A123" t="s">
-        <v>269</v>
-      </c>
-      <c r="B123">
-        <v>1</v>
-      </c>
-      <c r="C123" t="s">
-        <v>271</v>
+        <v>206</v>
+      </c>
+      <c r="B123" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="124" spans="1:3" ht="14.25" customHeight="1">
       <c r="A124" t="s">
-        <v>270</v>
-      </c>
-      <c r="B124" t="s">
-        <v>272</v>
-      </c>
-      <c r="C124" t="s">
-        <v>271</v>
+        <v>208</v>
+      </c>
+      <c r="B124">
+        <v>1</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="14.25" customHeight="1">
       <c r="A125" t="s">
-        <v>254</v>
+        <v>209</v>
       </c>
       <c r="B125" t="s">
-        <v>104</v>
+        <v>210</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="14.25" customHeight="1">
       <c r="A126" t="s">
-        <v>242</v>
-      </c>
-      <c r="B126" t="s">
-        <v>263</v>
-      </c>
-      <c r="C126" t="s">
-        <v>253</v>
+        <v>211</v>
+      </c>
+      <c r="B126">
+        <v>1</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="14.25" customHeight="1">
       <c r="A127" t="s">
-        <v>243</v>
-      </c>
-      <c r="B127" t="s">
-        <v>244</v>
+        <v>212</v>
+      </c>
+      <c r="B127">
+        <v>0</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="14.25" customHeight="1">
       <c r="A128" t="s">
-        <v>245</v>
-      </c>
-      <c r="B128" t="s">
-        <v>246</v>
+        <v>269</v>
+      </c>
+      <c r="B128">
+        <v>1</v>
+      </c>
+      <c r="C128" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="129" spans="1:3" ht="14.25" customHeight="1">
       <c r="A129" t="s">
-        <v>248</v>
+        <v>270</v>
       </c>
       <c r="B129" t="s">
-        <v>249</v>
+        <v>272</v>
+      </c>
+      <c r="C129" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="130" spans="1:3" ht="14.25" customHeight="1">
       <c r="A130" t="s">
-        <v>247</v>
+        <v>254</v>
       </c>
       <c r="B130" t="s">
-        <v>252</v>
+        <v>104</v>
       </c>
     </row>
     <row r="131" spans="1:3" ht="14.25" customHeight="1">
       <c r="A131" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="B131" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" ht="14.25" customHeight="1"/>
+        <v>263</v>
+      </c>
+      <c r="C131" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A132" t="s">
+        <v>243</v>
+      </c>
+      <c r="B132" t="s">
+        <v>244</v>
+      </c>
+    </row>
     <row r="133" spans="1:3" ht="14.25" customHeight="1">
       <c r="A133" t="s">
-        <v>222</v>
-      </c>
-      <c r="B133" s="2" t="s">
-        <v>223</v>
+        <v>245</v>
+      </c>
+      <c r="B133" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="134" spans="1:3" ht="14.25" customHeight="1">
       <c r="A134" t="s">
-        <v>231</v>
+        <v>248</v>
       </c>
       <c r="B134" t="s">
-        <v>134</v>
+        <v>249</v>
       </c>
     </row>
     <row r="135" spans="1:3" ht="14.25" customHeight="1">
       <c r="A135" t="s">
-        <v>232</v>
+        <v>247</v>
       </c>
       <c r="B135" t="s">
-        <v>233</v>
+        <v>252</v>
       </c>
     </row>
     <row r="136" spans="1:3" ht="14.25" customHeight="1">
       <c r="A136" t="s">
-        <v>224</v>
+        <v>250</v>
       </c>
       <c r="B136" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A137" t="s">
-        <v>225</v>
-      </c>
-      <c r="B137" t="s">
-        <v>258</v>
-      </c>
-    </row>
+        <v>251</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="138" spans="1:3" ht="14.25" customHeight="1">
       <c r="A138" t="s">
-        <v>259</v>
-      </c>
-      <c r="B138" t="s">
-        <v>260</v>
+        <v>222</v>
+      </c>
+      <c r="B138" s="2" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="139" spans="1:3" ht="14.25" customHeight="1">
       <c r="A139" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="B139" t="s">
-        <v>227</v>
+        <v>134</v>
       </c>
     </row>
     <row r="140" spans="1:3" ht="14.25" customHeight="1">
       <c r="A140" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="B140" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
     </row>
     <row r="141" spans="1:3" ht="14.25" customHeight="1">
       <c r="A141" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="B141" t="s">
-        <v>241</v>
-      </c>
-      <c r="C141" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
     </row>
     <row r="142" spans="1:3" ht="14.25" customHeight="1">
       <c r="A142" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
       <c r="B142" t="s">
-        <v>240</v>
-      </c>
-      <c r="C142" t="s">
-        <v>237</v>
+        <v>258</v>
       </c>
     </row>
     <row r="143" spans="1:3" ht="14.25" customHeight="1">
       <c r="A143" t="s">
+        <v>259</v>
+      </c>
+      <c r="B143" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A144" t="s">
+        <v>226</v>
+      </c>
+      <c r="B144" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A145" t="s">
+        <v>228</v>
+      </c>
+      <c r="B145" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A146" t="s">
+        <v>234</v>
+      </c>
+      <c r="B146" t="s">
+        <v>241</v>
+      </c>
+      <c r="C146" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A147" t="s">
+        <v>236</v>
+      </c>
+      <c r="B147" t="s">
+        <v>240</v>
+      </c>
+      <c r="C147" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A148" t="s">
         <v>238</v>
       </c>
-      <c r="B143" t="s">
+      <c r="B148" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="144" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="145" ht="14.25" customHeight="1"/>
-    <row r="146" ht="14.25" customHeight="1"/>
-    <row r="147" ht="14.25" customHeight="1"/>
-    <row r="148" ht="14.25" customHeight="1"/>
-    <row r="149" ht="14.25" customHeight="1"/>
-    <row r="150" ht="14.25" customHeight="1"/>
-    <row r="151" ht="14.25" customHeight="1"/>
-    <row r="152" ht="14.25" customHeight="1"/>
-    <row r="153" ht="14.25" customHeight="1"/>
-    <row r="154" ht="14.25" customHeight="1"/>
-    <row r="155" ht="14.25" customHeight="1"/>
-    <row r="156" ht="14.25" customHeight="1"/>
-    <row r="157" ht="14.25" customHeight="1"/>
-    <row r="158" ht="14.25" customHeight="1"/>
-    <row r="159" ht="14.25" customHeight="1"/>
-    <row r="160" ht="14.25" customHeight="1"/>
+    <row r="149" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="150" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="151" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="152" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="153" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="154" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="155" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="156" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="157" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="158" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="159" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="160" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="161" ht="14.25" customHeight="1"/>
     <row r="162" ht="14.25" customHeight="1"/>
     <row r="163" ht="14.25" customHeight="1"/>
@@ -4149,6 +4198,11 @@
     <row r="781" ht="14.25" customHeight="1"/>
     <row r="782" ht="14.25" customHeight="1"/>
     <row r="783" ht="14.25" customHeight="1"/>
+    <row r="784" ht="14.25" customHeight="1"/>
+    <row r="785" ht="14.25" customHeight="1"/>
+    <row r="786" ht="14.25" customHeight="1"/>
+    <row r="787" ht="14.25" customHeight="1"/>
+    <row r="788" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
quit simulate click in save for Colorado website and change name of parameter in send mail workflow
</commit_message>
<xml_diff>
--- a/STS IR Bot Performer/Data/Config.xlsx
+++ b/STS IR Bot Performer/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\martin.martinez\Documents\github-IRBot\STS_InternalReviewBot\STS IR Bot Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF645B70-DE9E-414A-BFA6-A8F1DE5ED94F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14BA7B89-5F4E-4CFD-BF9C-1D7BCBF3A6CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-30" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -2390,7 +2390,7 @@
   <dimension ref="A1:Z788"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
SUMTER is not take into account for SC State Balancing
</commit_message>
<xml_diff>
--- a/STS IR Bot Performer/Data/Config.xlsx
+++ b/STS IR Bot Performer/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\martin.martinez\Documents\github-IRBot\STS_InternalReviewBot\STS IR Bot Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14BA7B89-5F4E-4CFD-BF9C-1D7BCBF3A6CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E782B2E9-2571-4837-98EA-53292BBFBEEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-30" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -761,9 +761,6 @@
     <t>(&lt;COUNTY_LIST&gt;)\s+[\d\.\,]+\s+[\d\.\,]+</t>
   </si>
   <si>
-    <t>AIKEN|ALLENDALE|ANDERSON|BAMBERG|BARNWELL|BERKELEY|CALHOUN|CHARLESTON|CHEROKEE|CHESTER|CHESTERFIELD|CLARENDON|COLLETON|DARLINGTON|DILLON|EDGEFIELD|FLORENCE|GREENWOOD|HORRY|JASPER|KERSHAW|LANCASTER|LAURENS|LEE|LEXINGTON|MARION|MARLBORO|MCCORMICK|NEWBERRY|ORANGEBURG|RICHLAND|SALUDA|SPARTANBURG|SUMTER|WILLIAMSBURG|YORK</t>
-  </si>
-  <si>
     <t>StateBalancing_LA_GrossSalesClickOnText</t>
   </si>
   <si>
@@ -876,6 +873,9 @@
   </si>
   <si>
     <t>UiPath Development</t>
+  </si>
+  <si>
+    <t>AIKEN|ALLENDALE|ANDERSON|BAMBERG|BARNWELL|BERKELEY|CALHOUN|CHARLESTON|CHEROKEE|CHESTER|CHESTERFIELD|CLARENDON|COLLETON|DARLINGTON|DILLON|EDGEFIELD|FLORENCE|GREENWOOD|HORRY|JASPER|KERSHAW|LANCASTER|LAURENS|LEE|LEXINGTON|MARION|MARLBORO|MCCORMICK|NEWBERRY|ORANGEBURG|RICHLAND|SALUDA|SPARTANBURG|WILLIAMSBURG|YORK</t>
   </si>
 </sst>
 </file>
@@ -2389,8 +2389,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z788"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="B146" sqref="B146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2562,23 +2562,23 @@
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
       <c r="A17" t="s">
+        <v>272</v>
+      </c>
+      <c r="B17" t="s">
         <v>273</v>
-      </c>
-      <c r="B17" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" t="s">
+        <v>275</v>
+      </c>
+      <c r="B18" t="s">
         <v>276</v>
-      </c>
-      <c r="B18" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B19">
         <v>25</v>
@@ -2586,10 +2586,10 @@
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" t="s">
+        <v>277</v>
+      </c>
+      <c r="B20" t="s">
         <v>278</v>
-      </c>
-      <c r="B20" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2614,10 +2614,10 @@
     </row>
     <row r="24" spans="1:3" s="6" customFormat="1" ht="14.25" customHeight="1">
       <c r="A24" s="5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>68</v>
@@ -2674,7 +2674,7 @@
         <v>98</v>
       </c>
       <c r="B30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C30" t="s">
         <v>99</v>
@@ -2682,10 +2682,10 @@
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1">
       <c r="A31" t="s">
+        <v>264</v>
+      </c>
+      <c r="B31" t="s">
         <v>265</v>
-      </c>
-      <c r="B31" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2733,10 +2733,10 @@
     </row>
     <row r="38" spans="1:3" ht="14.25" customHeight="1">
       <c r="A38" t="s">
+        <v>266</v>
+      </c>
+      <c r="B38" t="s">
         <v>267</v>
-      </c>
-      <c r="B38" t="s">
-        <v>268</v>
       </c>
       <c r="C38" t="s">
         <v>71</v>
@@ -2825,10 +2825,10 @@
     </row>
     <row r="51" spans="1:2" ht="14.25" customHeight="1">
       <c r="A51" t="s">
+        <v>254</v>
+      </c>
+      <c r="B51" t="s">
         <v>255</v>
-      </c>
-      <c r="B51" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="14.25" customHeight="1"/>
@@ -3112,7 +3112,7 @@
         <v>190</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="14.25" customHeight="1">
@@ -3389,29 +3389,29 @@
     </row>
     <row r="128" spans="1:3" ht="14.25" customHeight="1">
       <c r="A128" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B128">
         <v>1</v>
       </c>
       <c r="C128" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="129" spans="1:3" ht="14.25" customHeight="1">
       <c r="A129" t="s">
+        <v>269</v>
+      </c>
+      <c r="B129" t="s">
+        <v>271</v>
+      </c>
+      <c r="C129" t="s">
         <v>270</v>
-      </c>
-      <c r="B129" t="s">
-        <v>272</v>
-      </c>
-      <c r="C129" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="130" spans="1:3" ht="14.25" customHeight="1">
       <c r="A130" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B130" t="s">
         <v>104</v>
@@ -3419,53 +3419,53 @@
     </row>
     <row r="131" spans="1:3" ht="14.25" customHeight="1">
       <c r="A131" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B131" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C131" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="132" spans="1:3" ht="14.25" customHeight="1">
       <c r="A132" t="s">
+        <v>242</v>
+      </c>
+      <c r="B132" t="s">
         <v>243</v>
-      </c>
-      <c r="B132" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="133" spans="1:3" ht="14.25" customHeight="1">
       <c r="A133" t="s">
+        <v>244</v>
+      </c>
+      <c r="B133" t="s">
         <v>245</v>
-      </c>
-      <c r="B133" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="134" spans="1:3" ht="14.25" customHeight="1">
       <c r="A134" t="s">
+        <v>247</v>
+      </c>
+      <c r="B134" t="s">
         <v>248</v>
-      </c>
-      <c r="B134" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="135" spans="1:3" ht="14.25" customHeight="1">
       <c r="A135" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B135" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="136" spans="1:3" ht="14.25" customHeight="1">
       <c r="A136" t="s">
+        <v>249</v>
+      </c>
+      <c r="B136" t="s">
         <v>250</v>
-      </c>
-      <c r="B136" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="137" spans="1:3" ht="14.25" customHeight="1"/>
@@ -3506,15 +3506,15 @@
         <v>225</v>
       </c>
       <c r="B142" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="143" spans="1:3" ht="14.25" customHeight="1">
       <c r="A143" t="s">
+        <v>258</v>
+      </c>
+      <c r="B143" t="s">
         <v>259</v>
-      </c>
-      <c r="B143" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="144" spans="1:3" ht="14.25" customHeight="1">
@@ -3538,7 +3538,7 @@
         <v>234</v>
       </c>
       <c r="B146" t="s">
-        <v>241</v>
+        <v>279</v>
       </c>
       <c r="C146" t="s">
         <v>235</v>

</xml_diff>

<commit_message>
LA state balancing - Get gross sales by Screen scraping. New regex added in Config file. Old LA state balancing version was deleted.
</commit_message>
<xml_diff>
--- a/STS IR Bot Performer/Data/Config.xlsx
+++ b/STS IR Bot Performer/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\martin.martinez\Documents\github-IRBot\STS_InternalReviewBot\STS IR Bot Performer\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nahuel.delacruz\OneDrive - Sovos Compliance\Desktop\Nahuel\Projects\STS Internal Review bot\STS IR Bot Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E782B2E9-2571-4837-98EA-53292BBFBEEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF3BC42E-D678-4757-9DD2-0B293E3DDF9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-30" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="282">
   <si>
     <t>Name</t>
   </si>
@@ -876,6 +876,12 @@
   </si>
   <si>
     <t>AIKEN|ALLENDALE|ANDERSON|BAMBERG|BARNWELL|BERKELEY|CALHOUN|CHARLESTON|CHEROKEE|CHESTER|CHESTERFIELD|CLARENDON|COLLETON|DARLINGTON|DILLON|EDGEFIELD|FLORENCE|GREENWOOD|HORRY|JASPER|KERSHAW|LANCASTER|LAURENS|LEE|LEXINGTON|MARION|MARLBORO|MCCORMICK|NEWBERRY|ORANGEBURG|RICHLAND|SALUDA|SPARTANBURG|WILLIAMSBURG|YORK</t>
+  </si>
+  <si>
+    <t>StateBalancing_LA_RegexGetGrossSalesInFilingOptions</t>
+  </si>
+  <si>
+    <t>[\d\.\,]+(?=.*Enter your State of Louisiana)</t>
   </si>
 </sst>
 </file>
@@ -2387,10 +2393,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z788"/>
+  <dimension ref="A1:Z789"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="B146" sqref="B146"/>
+    <sheetView tabSelected="1" topLeftCell="A114" workbookViewId="0">
+      <selection activeCell="A133" sqref="A133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3438,132 +3444,139 @@
     </row>
     <row r="133" spans="1:3" ht="14.25" customHeight="1">
       <c r="A133" t="s">
-        <v>244</v>
+        <v>280</v>
       </c>
       <c r="B133" t="s">
-        <v>245</v>
+        <v>281</v>
       </c>
     </row>
     <row r="134" spans="1:3" ht="14.25" customHeight="1">
       <c r="A134" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B134" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="135" spans="1:3" ht="14.25" customHeight="1">
       <c r="A135" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B135" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="136" spans="1:3" ht="14.25" customHeight="1">
       <c r="A136" t="s">
+        <v>246</v>
+      </c>
+      <c r="B136" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A137" t="s">
         <v>249</v>
       </c>
-      <c r="B136" t="s">
+      <c r="B137" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="137" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="138" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A138" t="s">
-        <v>222</v>
-      </c>
-      <c r="B138" s="2" t="s">
-        <v>223</v>
-      </c>
-    </row>
+    <row r="138" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="139" spans="1:3" ht="14.25" customHeight="1">
       <c r="A139" t="s">
-        <v>231</v>
-      </c>
-      <c r="B139" t="s">
-        <v>134</v>
+        <v>222</v>
+      </c>
+      <c r="B139" s="2" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="140" spans="1:3" ht="14.25" customHeight="1">
       <c r="A140" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B140" t="s">
-        <v>233</v>
+        <v>134</v>
       </c>
     </row>
     <row r="141" spans="1:3" ht="14.25" customHeight="1">
       <c r="A141" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="B141" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
     </row>
     <row r="142" spans="1:3" ht="14.25" customHeight="1">
       <c r="A142" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B142" t="s">
-        <v>257</v>
+        <v>229</v>
       </c>
     </row>
     <row r="143" spans="1:3" ht="14.25" customHeight="1">
       <c r="A143" t="s">
-        <v>258</v>
+        <v>225</v>
       </c>
       <c r="B143" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="144" spans="1:3" ht="14.25" customHeight="1">
       <c r="A144" t="s">
-        <v>226</v>
+        <v>258</v>
       </c>
       <c r="B144" t="s">
-        <v>227</v>
+        <v>259</v>
       </c>
     </row>
     <row r="145" spans="1:3" ht="14.25" customHeight="1">
       <c r="A145" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B145" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="146" spans="1:3" ht="14.25" customHeight="1">
       <c r="A146" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="B146" t="s">
-        <v>279</v>
-      </c>
-      <c r="C146" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
     </row>
     <row r="147" spans="1:3" ht="14.25" customHeight="1">
       <c r="A147" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B147" t="s">
-        <v>240</v>
+        <v>279</v>
       </c>
       <c r="C147" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="148" spans="1:3" ht="14.25" customHeight="1">
       <c r="A148" t="s">
+        <v>236</v>
+      </c>
+      <c r="B148" t="s">
+        <v>240</v>
+      </c>
+      <c r="C148" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A149" t="s">
         <v>238</v>
       </c>
-      <c r="B148" t="s">
+      <c r="B149" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="149" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="150" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="151" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="152" spans="1:3" ht="14.25" customHeight="1"/>
@@ -4203,6 +4216,7 @@
     <row r="786" ht="14.25" customHeight="1"/>
     <row r="787" ht="14.25" customHeight="1"/>
     <row r="788" ht="14.25" customHeight="1"/>
+    <row r="789" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>